<commit_message>
Finish stratified sampling with 80 10 10 split and started the monologue dataset
</commit_message>
<xml_diff>
--- a/testing_excel.xlsx
+++ b/testing_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gartopou\PycharmProjects\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC88EF78-5C5E-4705-9A75-E7DBFCFFFCE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF8865D-519D-46D5-96C5-34CE19E2B1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="769" firstSheet="15" activeTab="23" xr2:uid="{3104A2F9-7A17-4E5B-B5FF-CB166158170B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="769" firstSheet="16" activeTab="25" xr2:uid="{3104A2F9-7A17-4E5B-B5FF-CB166158170B}"/>
   </bookViews>
   <sheets>
     <sheet name="Greeting_Goodbyes" sheetId="2" r:id="rId1"/>
@@ -38,6 +38,7 @@
     <sheet name="Guard_skill" sheetId="31" r:id="rId23"/>
     <sheet name="Stromcloak-imperial" sheetId="32" r:id="rId24"/>
     <sheet name="Guard_interactions" sheetId="33" r:id="rId25"/>
+    <sheet name="Introduction" sheetId="39" r:id="rId26"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5728" uniqueCount="1661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5751" uniqueCount="1684">
   <si>
     <t>Greetings</t>
   </si>
@@ -5043,13 +5044,85 @@
   </si>
   <si>
     <t>the wedding arrangements between an NPC and the Player</t>
+  </si>
+  <si>
+    <t>The Last of Us</t>
+  </si>
+  <si>
+    <t>Game Title</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>The Witcher 3: Wild Hunt</t>
+  </si>
+  <si>
+    <t>I see you gather before me, hungry, terrified, clutching your babes to your breasts. Emperor Emhyr has marched his legions into our lands, laid siege to every fortress from here to the Blue Mountains. Rabid and ravenous, he bites and bites away. Men of the North, you stand at the precipice; your kings have failed you. So now you turn to the gods. And yet you do not plead, you do not kneel to dust your heads with ash. Instead, you wail, "Why have the gods forsaken us?" We must look into the trials we failed long ago. In a time past, our world intertwined with another through an upheaval scholars call the Conjunction of the Spheres. The gods allowed unholy forces to slip into our domain. The offspring of that cataclysm was the nefarious force called magic. Yet we did not banish it. Instead, we studied the arcane for our own power and wealth. And the monsters at our door—the unholy relics of this conjunction, the trolls, the corpse eaters. Did we raise our swords against them? Or have we laid this burden on others, on so-called witches? Stray children taught the ways of foul sorcery, their bodies mutated through blasphemous ritual, sent to fight monsters, though they could not distinguish good from evil. The flicker of humanity long extinguished within them. Yes, their numbers have dwindled through the years, but a few still roam our lands, offering their bloody work for coin. To this day, they shame us with their very existence. The North bleeds, flogged by war. The battles are the gods' whip, chastisement for our sins. Let us not forget the terrors; the scourge is from beyond our world. The Wild Hunt rides the sky with every full moon. The dark raiders abduct our children into lands unknown. Some say they herald a second conjunction. Can we chart a course back into the light? Will we find the strength to banish the mages from our kingdoms, unite around the warmth of the eternal fire? Nigh is the time of the sword and axe. Nigh is the time of madness and disdain.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of confirmed deaths has passed 200. The governor has called a state of emergency. Hundreds of bodies line the streets. Panic spread worldwide after a leaked report from the World Health Organization showed that the latest vaccination tests have failed. Bureaucrats have power, and we can finally take necessary actions. Los Angeles is now under martial law. All residents must report to designated quarantines. This has continued for a third consecutive day, and winter rations are at an all-time low. A group called the Fireflies claimed responsibility for both attacks. Their public charter calls for the return of all branches of government. Demonstrations broke out following the execution of six more alleged Fireflies. "Still rise with us. Remember, when you are lost in the darkness, look for the light. Believe in the Fireflies."
+</t>
+  </si>
+  <si>
+    <t>Elden Ring</t>
+  </si>
+  <si>
+    <t>Fallout 3</t>
+  </si>
+  <si>
+    <t>The fallen leaves tell a story: the great Elden Ring was shattered. In our home, across the fog, the Lands Between, Queen Marika the Eternal is nowhere to be found. On the Night of the Black Knives, Godwin the Golden was the first to perish. Soon, Marika's offspring, demigods all, claimed the shards of the Elden Ring. The mad taint of their newfound strength triggered the Shattering—a war from which no lord arose, leading to abandonment by the Greater Will. Rise now, ye Tarnished, the dead who yet live. The call of long-lost grace speaks to us all—chieftain of the badlands, the ever-brilliant Goldmask, Fia the deathbed companion, the loathsome Dung Eater, and one other whom grace would again bless. A Tarnished of no renown, cross the fog to the Lands Between to stand before the Elden Ring and become the Elden Lord.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">War. War never changes. Since the dawn of humankind, when our ancestors first discovered the killing power of rock and bone, blood has been spilled in the name of everything from God to justice to simple psychotic rage. In the year 2077, after millennia of armed conflict, the destructive nature of man could sustain itself no longer. The world was plunged into an abyss of nuclear fire and radiation. But it was not the end of the world. Instead, the apocalypse was simply the prologue to another bloody chapter of human history. For man had succeeded in destroying the world, but war never changes.
+In the early days, thousands were spared the horrors of the Holocaust by taking refuge in enormous underground shelters known as vaults. But when they emerged, they had only the hell of the wastes to greet them, except those in Vault 101. For on that fateful day, when fire rained from the sky, the giant steel door of Vault 101 slid closed and never reopened. It was here you were born; it is here you will die. Because in Vault 101, no one ever enters, and no one ever leaves.
+</t>
+  </si>
+  <si>
+    <t>Fallout 4</t>
+  </si>
+  <si>
+    <t>War. War never changes. In 1945, my great-great-grandfather, serving in the army, wondered when he'd get to go home to his wife and the son he'd never seen. He got his wish when the U.S. ended World War II by dropping atomic bombs on Hiroshima and Nagasaki. The world awaited Armageddon. Instead, something miraculous happened. We began to use atomic energy not as a weapon but as a nearly limitless source of power. People enjoyed luxuries once thought the realm of science fiction: domestic robots, fusion-powered cars, portable computers. But then, in the 21st century, people awoke from the American dream. Years of consumption led to shortages of every major resource. The entire world unraveled; peace became a distant memory. It is now the year 2077. We stand on the brink of total war, and I am afraid—for myself, for my wife, for my infant son. Because if my time in the army taught me one thing, it’s that war, war never changes.</t>
+  </si>
+  <si>
+    <t>Fallout: New Vegas</t>
+  </si>
+  <si>
+    <t>War. War never changes. When atomic fire consumed the earth, those who survived did so in great underground vaults. When they opened, their inhabitants set out across the ruins to build new societies. As decades passed, the American Southwest united under the New California Republic, dedicated to democracy and the rule of law. As the Republic grew, it sent scouts east into the Mojave Desert. They found a city untouched by warheads and a great wall spanning the Colorado River. The NCR sent its army to occupy Hoover Dam. Meanwhile, Caesar's Legion, a vast army of slaves, rose across the Colorado. Four years ago, the NCR barely held the dam against the Legion's onslaught. The Legion now gathers strength. The New Vegas Strip remains open under Mr. House and his robots. You are a courier, hired to deliver a package to New Vegas, but your job has taken a turn for the worse. "Sorry you got twisted up in this. From where you're kneeling, it must seem like an 18-carat run of bad luck. The truth is, the game was rigged from the start."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Borderlands </t>
+  </si>
+  <si>
+    <t>Borderlands 2</t>
+  </si>
+  <si>
+    <t>Borderlands 3</t>
+  </si>
+  <si>
+    <t>So you want to hear a story, huh? What about treasure hunters? Have I got a story for you. Pandora, this is our home, but make no mistake, this is not a planet of peace and love. They say it's a wasteland, that it's dangerous, that only a fool would search for something of value here. Then perhaps I am a fool. But do not be fooled by what Pandora appears to be. There was a legend, many people tell it: the legend of the Vault. My father would always go on about the Vault, even with his dying breath. Advanced alien technology, infinite wealth, fame, power, women. So you can understand why some little kiddos grow up to become Vault Hunters. Well, I have a story you may not believe, but I tell you it is true. The legend of the Vault is real and it is here on Pandora, and a Guardian Angel appeared to guide the Vault Hunters to their prize. The tale begins right here on Pandora with brave Vault Hunters, the Guardian Angel, and most importantly, me.</t>
+  </si>
+  <si>
+    <t>So you want to hear another story, one where the very fate of Pandora hangs in the balance? If not, too bad, I'm telling you anyway. First, there was the Vault, an alien prison opened with a mystical key. To the warriors opening the Vault, it was just a container of tentacles and disappointment. They vanished into the wastelands, certain that the Vault held no treasure at all. They were wrong. The Vault's opening triggered the growth of Eridium, a priceless alien element. Soon, the rare and valuable mineral emerged all across Pandora. Its appearance attracted many, including the Hyperion Corporation. They came to Pandora to mine Eridium and bring order to the savage planet. Through their excavations, Hyperion uncovered evidence of an even greater Vault. Their leader vowed to find it, to use its power to civilize the Borderlands once and for all. But Hyperion weren't the only ones searching for the next Vault. The call of danger and loot is not easily resisted. Certain warriors came to Pandora in droves to uncover its hidden secrets. Some would call them adventurers, others call them fools, but I call them Vault Hunters. Our story begins with them and with a man named Handsome Jack.</t>
+  </si>
+  <si>
+    <t>So you want to hear a story, a tale of adventure across two stars? Come, listen to old Marcus. Have I got a story for you. My tale begins here, on this backwater planet called Pandora. Some say it is a wasteland of greed and violence, and it is, but if you've got the skills to pay the bills, Pandora is full of opportunity. Vault Hunters braved the merciless Borderlands in search of secret alien treasure. My father told me tales of Vault Hunting when I was but a little Marcus boy, and now I tell you. You ask, what treasures do the Vaults hide? Wealth, or maybe nonsense like charity or family? I don't know. Use your imagination. Whatever the prize, a Vault Hunter must have the determination to seize victory from the jealous hands of fate. Now, my story is about a very special band of adventurers who have only just started their journey. They are bold and hungry. Maybe old Marcus tells you this story because they remind me of myself. Don't let it go to your head. These new Vault Hunters are answering a Siren's call. Her name is Lilith, and she is a hero who saved Pandora a dozen times over. Lilith is recruiting a team to hunt for a man who leads to Vaults all over the galaxy. But she is not the only one. Dark forces have overrun the Borderlands, unlike anything the galaxy has seen before. My story begins right here on Pandora with our new Vault Hunters and most importanly, me.</t>
+  </si>
+  <si>
+    <t>Helldiver 2</t>
+  </si>
+  <si>
+    <t>Super Earth, our home. Prosperity, liberty, and democracy are our way of life. Freedom doesn't come free, and familiar scenes like these are happening all over the galaxy right now. You could be next, unless you make the most important decision of your life. Prove to yourself that you have the strength and the courage to be free. Join the Helldivers. Become part of an elite peacekeeping force, see exotic new life forms, and spread managed democracy.</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5078,6 +5151,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -5099,7 +5178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -5115,6 +5194,8 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5133,9 +5214,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5173,7 +5254,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5279,7 +5360,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5421,7 +5502,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -19030,7 +19111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9FCF089-81A6-4F6F-BFF5-089ECF9774AA}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13:D22"/>
     </sheetView>
   </sheetViews>
@@ -20851,6 +20932,120 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48AA9C6D-EFEE-4389-B779-BD4A88AD0E00}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.33203125" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1662</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1661</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1664</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1667</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1668</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1673</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>1674</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1676</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1677</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1683</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F8191EA-EF3D-4D61-BB9C-839E6E5AEF96}">
   <dimension ref="A1:B28"/>

</xml_diff>

<commit_message>
Update the dataset and write the LLM training query for the introductory monologues
</commit_message>
<xml_diff>
--- a/testing_excel.xlsx
+++ b/testing_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gartopou\PycharmProjects\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91EDAF7-FC19-4118-B73A-067AD5FC6020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09BADB9-36F9-4C50-BA71-835AC58DC81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="769" firstSheet="16" activeTab="25" xr2:uid="{3104A2F9-7A17-4E5B-B5FF-CB166158170B}"/>
   </bookViews>
@@ -5055,13 +5055,6 @@
     <t>The Witcher 3: Wild Hunt</t>
   </si>
   <si>
-    <t>I see you gather before me, hungry, terrified, clutching your babes to your breasts. Emperor Emhyr has marched his legions into our lands, laid siege to every fortress from here to the Blue Mountains. Rabid and ravenous, he bites and bites away. Men of the North, you stand at the precipice; your kings have failed you. So now you turn to the gods. And yet you do not plead, you do not kneel to dust your heads with ash. Instead, you wail, "Why have the gods forsaken us?" We must look into the trials we failed long ago. In a time past, our world intertwined with another through an upheaval scholars call the Conjunction of the Spheres. The gods allowed unholy forces to slip into our domain. The offspring of that cataclysm was the nefarious force called magic. Yet we did not banish it. Instead, we studied the arcane for our own power and wealth. And the monsters at our door—the unholy relics of this conjunction, the trolls, the corpse eaters. Did we raise our swords against them? Or have we laid this burden on others, on so-called witches? Stray children taught the ways of foul sorcery, their bodies mutated through blasphemous ritual, sent to fight monsters, though they could not distinguish good from evil. The flicker of humanity long extinguished within them. Yes, their numbers have dwindled through the years, but a few still roam our lands, offering their bloody work for coin. To this day, they shame us with their very existence. The North bleeds, flogged by war. The battles are the gods' whip, chastisement for our sins. Let us not forget the terrors; the scourge is from beyond our world. The Wild Hunt rides the sky with every full moon. The dark raiders abduct our children into lands unknown. Some say they herald a second conjunction. Can we chart a course back into the light? Will we find the strength to banish the mages from our kingdoms, unite around the warmth of the eternal fire? Nigh is the time of the sword and axe. Nigh is the time of madness and disdain.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of confirmed deaths has passed 200. The governor has called a state of emergency. Hundreds of bodies line the streets. Panic spread worldwide after a leaked report from the World Health Organization showed that the latest vaccination tests have failed. Bureaucrats have power, and we can finally take necessary actions. Los Angeles is now under martial law. All residents must report to designated quarantines. This has continued for a third consecutive day, and winter rations are at an all-time low. A group called the Fireflies claimed responsibility for both attacks. Their public charter calls for the return of all branches of government. Demonstrations broke out following the execution of six more alleged Fireflies. "Still rise with us. Remember, when you are lost in the darkness, look for the light. Believe in the Fireflies."
-</t>
-  </si>
-  <si>
     <t>Elden Ring</t>
   </si>
   <si>
@@ -5082,9 +5075,6 @@
     <t>Fallout: New Vegas</t>
   </si>
   <si>
-    <t>War. War never changes. When atomic fire consumed the earth, those who survived did so in great underground vaults. When they opened, their inhabitants set out across the ruins to build new societies. As decades passed, the American Southwest united under the New California Republic, dedicated to democracy and the rule of law. As the Republic grew, it sent scouts east into the Mojave Desert. They found a city untouched by warheads and a great wall spanning the Colorado River. The NCR sent its army to occupy Hoover Dam. Meanwhile, Caesar's Legion, a vast army of slaves, rose across the Colorado. Four years ago, the NCR barely held the dam against the Legion's onslaught. The Legion now gathers strength. The New Vegas Strip remains open under Mr. House and his robots. You are a courier, hired to deliver a package to New Vegas, but your job has taken a turn for the worse. "Sorry you got twisted up in this. From where you're kneeling, it must seem like an 18-carat run of bad luck. The truth is, the game was rigged from the start."</t>
-  </si>
-  <si>
     <t>Borderlands 2</t>
   </si>
   <si>
@@ -5139,9 +5129,6 @@
     <t>Used to be, when people talked about the end of the world, we locked them up or laughed them off, sometimes both, but we never took them seriously. Maybe we should have. But I'm getting ahead of myself. Better to start at the beginning, with the abduction of Desmond Miles, my son. This boy had no ambition, no direction, no plans for the future. What he did have was a heritage, one he chose to deny. It nearly cost him his life. He was captured and imprisoned. Those who took him believed he could help them find something—the Apple, one of several artifacts we call Pieces of Eden, bits of ancient technology scattered across the globe. Some hidden, some found, all of them dangerous. Most are held by a single group, the same group that now had Desmond. You know them as Abstergo Industries. We know them as the Templars, as the enemy. We've been fighting them for thousands of years, even longer if you believe the stories of their origins. I do, after all I've seen.
 The truth, that's the beauty and the horror of the Animus, a device that allows us to enter and experience the lives of our ancestors. It holds the power to change everything, to show us history the way it really happened. Up until its creation, to the victor went the spoils, went the truth. We're trying to fix that, to free minds and bodies both, but there's only so much that we can do, and the Templars have the upper hand these days. But something larger than the Assassins and Templars is approaching, bigger than all of us, and if we can't find a way to stop it, these next few weeks will probably be our last, everyone's last. In the end, it all comes down to him, to Desmond. Through the Animus, he discovered his heritage, explored the lives of his ancestors, and uncovered their secrets. When that was done, he trained; he used another ancestor to provide decades of experience in the span of a few days. It worked, we think, we hope. Soon, though, soon we'll know.
 That ominous date fast approaches—December 21st, 2012. None of us knows what it'll bring, only that this is where they want us to be when it does. They've been guiding us in their own fractured, frustrating way. These voices from the first civilization, the ones who came before, a precursor race of immense power and uncertain motives. They're the ones who made the Pieces of Eden. This is where they've led him, and through him, us. He stands at the entrance to this long-lost place, armed with the knowledge of Altair and the abilities of Ezio. He holds in his hands the Apple of Eden, and we stand at his side, ready to support him however we can. His name is Desmond Miles, and he has brought us to the end.</t>
-  </si>
-  <si>
-    <t>Yes, indeed. It is called Lothric, where the transitory lands of the Lords of Cinder converge. In venturing north, the pilgrims discover the truth of the old words: "The fire fades and the lords go without thrones." When the link of fire is threatened, the bell tolls, unearthing the old Lords of Cinder from their graves...Aldrich, Saint of the Deep... Farron's Undead Legion, the Abyss Watchers... And the reclusive lord of the Profaned Capital, Yhorm the Giant... Only, in truth... the Lords will abandon their thrones... And the Unkindled will rise. Nameless, accursed Undead, unfit even to be cinder. And so it is, that ash seeketh embers.</t>
   </si>
   <si>
     <t>Perhaps you've seen it, maybe in a dream. A murky, forgotten land. A place where souls may mend your ailing mind. You will lose everything... once Branded. The symbol of the curse. An augur of darkness. Your past. Your future. Your very light. None will have meaning, and you won't even care. By then, you'll be something other than human. A thing that feeds on souls. A Hollow. Long ago, in a walled off land, far to the north, a great king built a great kingdom. I believe they called it Drangleic. Perhaps you're familiar. No, how could you be. But one day, you will stand before its decrepit gate. Without really knowing why... Like a moth drawn to a flame. Your wings will burn in anguish. Time after time. For that is your fate. The fate of the cursed.</t>
@@ -5234,12 +5221,6 @@
   </si>
   <si>
     <t>Pillars of Eternity II: Deadfire</t>
-  </si>
-  <si>
-    <t>Eora: a world where mortals live, die, and are reborn through the turning of the Wheel, the cycle of reincarnation is watched over by the gods and made possible through pillars of a mystical substance known as adra. Five years ago, you traveled from your home to the Deerwood, a nation that had waged war against the incarnated God of Light, Eothas, resulting in his destruction. The country suffered from a plague of Hollowborn infants, born without souls, a tragedy many believed was punishment for killing a god.
-In an ancient, secluded ruin, you witnessed a secret ritual that inadvertently transformed you into a Watcher, one who can see and speak with souls. This ritual also gave you horrible visions—waking nightmares of a past life that threatened your sanity. To put them to rest, you pursued the man who had led the ritual, a seemingly immortal agent of the gods known as Thaos Ix Arkannon. With divine assistance, you confronted and defeated Thaos, ending your visions and resolving the Hollowborn crisis. In so doing, you also learned the great secret that Thaos had protected: that the ancient empire of Engwith had transformed themselves into gods.
-Your visions finally put to rest, you retired to the castle of Caed Nua, built atop a massive statue of pure adra, where you ruled in relative peace and prosperity. 
-"Made a nice story. You fixing up that old keep, lifting the curse. Must ‘ve told it a hundred times. But … something got to gnawin’ at me… Thinkin’ the spirits there were not really at rest. Maybe the gods weren't finished with us yet. I used to dream that when my god came back, he would forgive us. That's the trouble with dreams… sooner or later, we all have to wake up.”</t>
   </si>
   <si>
     <t>This is the story of a man named Stanley. Stanley worked for a company in a big building where he was employee number 427. Employee Number 427's job was simple: he sat at his desk in room 427, and he pushed buttons on a keyboard. Orders came to him through a monitor on his desk, telling him what buttons to push, how long to push them, and in what order. This is what Employee 427 did every day of every month and every year, and although others might have considered it soul-rending, Stanley relished every moment that the orders came in, as though he had been made exactly for this job. And Stanley was happy.
@@ -5398,177 +5379,196 @@
     <t>Context</t>
   </si>
   <si>
-    <t>In "The Last of Us," the introductory monologue is delivered by a news reporter who grimly details the escalating crisis. This sets the stage for the game's post-apocalyptic narrative, where society collapses due to a devastating fungal outbreak. Players follow Joel, a hardened survivor, and Ellie, a young girl who might hold the key to humanity's survival, as they navigate a world filled with infected mutants and hostile human factions. The Fireflies, a revolutionary militia group, seek to restore government control, adding to the chaos and conflict that define the game's intense and emotional journey.</t>
-  </si>
-  <si>
-    <t>In "The Witcher 3: Wild Hunt," the introductory monologue is delivered by a foreboding narrator who addresses the chaos and despair gripping the land. This sets the stage for the game's dark fantasy narrative, where players follow Geralt of Rivia, a monster hunter known as a Witcher, on a quest to find his adopted daughter Ciri, who is being pursued by the otherworldly Wild Hunt. The game is set in a war-torn world filled with political intrigue, dangerous creatures, and morally complex choices. As Geralt, players must navigate through the turmoil, battling both human and monstrous foes, while making decisions that shape the fate of the world and its inhabitants.</t>
-  </si>
-  <si>
-    <t>In "Fallout 3," the introductory monologue is delivered by the narrator, setting a grim tone for the game. This monologue introduces players to a post-apocalyptic world devastated by nuclear war in 2077. Players assume the role of a character born and raised in Vault 101, one of the many underground shelters designed to protect humanity from the horrors of nuclear fallout. The vault's motto, "no one ever enters, and no one ever leaves," shapes the protagonist's early life until circumstances force them to venture into the harsh and desolate wasteland of the Capital Wasteland. As they search for their missing father, players must navigate through a world filled with radiation, mutated creatures, and hostile factions, all while uncovering the secrets of their family's past and the broader mysteries of the post-apocalyptic society.</t>
-  </si>
-  <si>
-    <t>In "Fallout 4," the introductory monologue is delivered by the protagonist, setting the stage for the game's post-apocalyptic narrative. The game begins in 2077, just before a nuclear war devastates the world. Players take on the role of a character who survives the apocalypse by taking refuge in Vault 111. Emerging 200 years later, the protagonist finds a drastically changed world and embarks on a quest to find their kidnapped son. The journey takes them through the Commonwealth, a region filled with mutated creatures, hostile factions, and the remnants of pre-war society, as they uncover the truth about their past and influence the future of the wasteland.</t>
-  </si>
-  <si>
     <t>Borderlands</t>
   </si>
   <si>
-    <t>In "Fallout: New Vegas," the introductory monologue is delivered by the narrator and sets the stage for the game's post-apocalyptic narrative. Players assume the role of a courier in the Mojave Desert, an area where the New California Republic and Caesar's Legion vie for control of the Hoover Dam. The city of New Vegas remains untouched by nuclear war, under the control of Mr. House and his robotic army. As the courier, players begin their journey after surviving an ambush intended to prevent the delivery of a mysterious package. The protagonist's quest for revenge and discovery leads them through a world filled with factions, conflicts, and the remnants of pre-war society, ultimately influencing the fate of New Vegas and its inhabitants.</t>
-  </si>
-  <si>
-    <t>In "Borderlands," the introductory monologue, delivered by the character Marcus Kincaid, sets the stage for the game's adventure-filled narrative. Players take on the role of Vault Hunters on the planet Pandora, a lawless and dangerous world rumored to hold the legendary Vault, filled with advanced alien technology and unimaginable riches. Guided by a mysterious Guardian Angel, the Vault Hunters embark on a quest to find this mythical treasure. The journey is filled with peril, bizarre creatures, and treacherous bandits, as they uncover the secrets of Pandora and strive to claim the legendary Vault's bounty.</t>
-  </si>
-  <si>
-    <t>In "Borderlands 2," the introductory monologue is delivered by the charismatic and humorous narrator, Marcus Kincaid. This monologue sets the stage for the game's high-stakes narrative. Players assume the role of new Vault Hunters on Pandora, a planet now infused with the rare and valuable mineral Eridium, which emerged after the first Vault's opening. The Hyperion Corporation, led by the ruthless Handsome Jack, seeks to exploit this resource and bring order to Pandora by uncovering an even greater Vault. Drawn by the promise of danger and loot, the Vault Hunters embark on a quest to stop Handsome Jack, uncover Pandora's hidden secrets, and ultimately save the planet from his tyrannical grip. The journey is filled with intense battles, quirky characters, and a struggle against the corporate oppression of Hyperion.</t>
-  </si>
-  <si>
-    <t>In "Borderlands 3," the introductory monologue is delivered by Marcus Kincaid, setting the stage for the game's thrilling adventure. Players take on the role of new Vault Hunters on the planet Pandora, a land known for its greed and violence but also its opportunities. Guided by tales of hidden alien treasures, these Vault Hunters embark on a journey answering the call of Lilith, a legendary Siren and hero of Pandora. She is assembling a team to hunt for a man leading to Vaults across the galaxy. However, dark forces have emerged, posing unprecedented threats to the Borderlands. The adventure begins with these bold and hungry Vault Hunters, embarking on a quest filled with danger, treasure, and the enduring charm of Marcus's storytelling.</t>
-  </si>
-  <si>
-    <t>In "God of War III," the introductory monologue is delivered by Gaia, the Titaness of Earth, setting the stage for the epic conclusion of Kratos's journey. The narrator recounts the rise of Kratos, who, despite becoming the new God of War, remains haunted by the tragic memories of murdering his own family. Neither death nor the Sisters of Fate could contain him. As the game begins, Kratos, driven by an unyielding desire for vengeance, embarks on a relentless quest to bring down the gods of Olympus who have wronged him. This climactic chapter sees Kratos confronting powerful deities and mythical creatures, fueled by his rage and determination to seek justice for the torment he has endured.</t>
-  </si>
-  <si>
-    <t>In "Assassin's Creed: Revelations," the introductory monologue is delivered by Ezio Auditore in a letter to his sister, Claudia, setting the stage for his journey. Ezio has arrived in Masyaf, seeking a hidden library mentioned by their father. This library, located beneath Masyaf Castle, is believed to contain invaluable wisdom and secrets left by the legendary Assassin, Altair. Players take on the role of Ezio, now a seasoned Master Assassin, as he navigates the perilous journey to uncover the hidden knowledge. The road to Masyaf is fraught with mercenaries and bandits, making the mission dangerous and uncertain. As Ezio, players must use their skills and cunning to overcome these threats, unravel the mysteries of the past, and gain insight into the true purpose of the Assassin Brotherhood. The game delves into Ezio's introspective quest for clarity and understanding, while also connecting his fate with that of Altair and Desmond Miles, bridging the gaps between different eras of the Assassin's Creed saga.</t>
-  </si>
-  <si>
-    <t>In "Assassin's Creed: Mirage," the introductory monologue is delivered by a narrator reflecting on the memory of a pivotal figure. This sets the stage for the game's narrative, focusing on a man who rose from being a common thief on the streets of Baghdad to a significant member of the Hidden Ones, the predecessors of the Assassin Brotherhood. Players take on the role of this man, navigating the bustling and dangerous streets of Baghdad during the height of the Abbasid Caliphate. Despite the city's golden age, a sinister rot lies beneath, with the Order of the Ancients spreading their influence and cruelty. As a member of the Hidden Ones, the protagonist engages in a shadowy struggle against these oppressive forces. The journey is not just one of external conflict but also of personal growth and understanding. The protagonist's story is a testament to honoring the Creed, challenging it, and recognizing the thin line between the shadows they walk and the light they serve. Players must navigate this complex world, making choices that reflect the eternal struggle between freedom and oppression, light and darkness.</t>
-  </si>
-  <si>
-    <t>In "Assassin's Creed III," the introductory monologue is delivered by William Miles, setting the stage for the game's narrative. He reflects on the end of the world, a concept once dismissed but now frighteningly real. The story begins with the abduction of Desmond Miles, his son, who possesses a denied heritage. Desmond was captured by Abstergo Industries, known to the Assassins as the Templars, who sought his help to find the Apple of Eden, a powerful artifact. Players take on the role of Desmond Miles, using the Animus to explore the lives of his ancestors and uncover hidden truths about the Assassins and Templars. As Desmond, players must gain the knowledge and skills of his ancestors, Altair and Ezio, to prevent an impending apocalypse foretold to occur on December 21, 2012. The journey involves mastering combat and stealth, solving complex puzzles, and making strategic decisions that impact the course of history. Armed with the Apple of Eden and supported by his fellow Assassins, Desmond stands at the brink of the final confrontation, ready to use his newfound abilities to save humanity from disaster.</t>
-  </si>
-  <si>
-    <t>In "Dark Souls III," the introductory monologue is delivered by an unseen narrator, setting the stage for the game's dark and foreboding narrative. It begins with a description of Lothric, a land where the transitory realms of the Lords of Cinder converge. As the fire fades and the lords forsake their thrones, a bell tolls, awakening the old Lords of Cinder from their graves: Aldrich, Saint of the Deep; Farron's Undead Legion, the Abyss Watchers; and Yhorm the Giant, the reclusive lord of the Profaned Capital. However, the Lords abandon their thrones, leaving the Unkindled to rise. Players assume the role of an Unkindled, a nameless and accursed undead, unfit even to be cinder. Their journey involves seeking embers, confronting the revived Lords of Cinder, and ultimately rekindling the First Flame to prevent the world from falling into darkness. The player's role is to navigate this treacherous world, mastering its challenging combat, uncovering its hidden lore, and making decisions that shape the fate of Lothric and its inhabitants.</t>
-  </si>
-  <si>
-    <t>In "Dark Souls II," the introductory monologue is delivered by an unseen narrator, setting the stage for the game's dark and mysterious narrative. The story begins by introducing a murky, forgotten land where souls can mend an ailing mind. Players are warned that they will lose everything once branded with the symbol of the curse, becoming something other than human—a Hollow. The narrative speaks of a walled-off land far to the north where a great king built the kingdom of Drangleic. As players, you assume the role of a cursed individual drawn to Drangleic without fully understanding why, like a moth to a flame. Your journey will be one of relentless anguish, facing challenges and uncovering the deep lore of this decrepit kingdom. The player's role involves navigating the perilous world of Drangleic, mastering its brutal combat, and seeking to lift the curse that plagues them, all while unraveling the secrets of this enigmatic land.</t>
-  </si>
-  <si>
-    <t>In "The Elder Scrolls IV: Oblivion," the introductory monologue is delivered by Emperor Uriel Septim VII, who reflects on his long reign and impending doom. This sets the stage for the game's epic fantasy narrative, where players take on the role of an anonymous prisoner destined to thwart a dire prophecy. As gates to the demonic realm of Oblivion open and dark forces threaten to engulf the land of Tamriel, players must navigate a richly detailed world, undertake quests, and battle fearsome enemies. The story unfolds with the player seeking to find and protect the lost heir to the throne, ultimately striving to seal the gates of Oblivion and save the Empire from destruction.</t>
-  </si>
-  <si>
-    <t>In "The Elder Scrolls Online," the introductory monologue is delivered by a narrator who sets the ominous tone of impending conflict and ancient evil. This sets the stage for the game's expansive MMORPG narrative, where players enter the world of Tamriel during a time of great turmoil and war. The year is 582 of the Second Era, and various factions vie for control of the Imperial City and the Ruby Throne. Players can choose from a variety of races and classes, embarking on epic quests, exploring vast regions, and battling both monsters and rival factions. As they uncover hidden dangers and dark schemes, players must navigate alliances and conflicts, shaping the fate of Tamriel in an ever-evolving world filled with adventure and danger.</t>
-  </si>
-  <si>
-    <t>In "Fallout 2," the introductory monologue is delivered by a narrator who reflects on the unchanging nature of war and the catastrophic events that led to the world's near-destruction. This sets the stage for the game's post-apocalyptic narrative, where players take on the role of the Chosen One, a descendant of the legendary Vault Dweller. Emerging from the tribal village of Arroyo, the player embarks on a perilous journey to save their home from ecological disaster. The story unfolds in a vast, irradiated wasteland filled with mutated creatures, ruthless factions, and remnants of pre-war technology. As the Chosen One, players must navigate this dangerous world, making crucial decisions that will determine the fate of their tribe and the future of humanity.</t>
-  </si>
-  <si>
-    <t>In "Metal Gear Solid V: The Phantom Pain," the introductory monologue is delivered by a narrator who describes the evolution of modern warfare into an automated and controlled system. This sets the stage for the game's complex narrative, where players follow the story of Big Boss, also known as Venom Snake, as he builds a new private army to take revenge on the shadowy organization Cipher. The game is set in an open world, where players undertake missions across various global conflict zones, employing stealth, strategy, and combat skills. The narrative delves into themes of revenge, loyalty, and the impact of war, all while exploring the technological advancements that have transformed the battlefield into a highly regulated and monitored environment. As Venom Snake, players must navigate this dangerous world, building and managing their own mercenary army, the Diamond Dogs. They engage in tactical espionage operations, gather resources, recruit soldiers, and develop new weapons and technology.</t>
-  </si>
-  <si>
-    <t>In "Alan Wake II," the introductory monologue is delivered by a narrator who sets a haunting and mysterious tone. This sets the stage for the game's psychological horror narrative, where players follow Alan Wake, a troubled writer, as he navigates a surreal and nightmarish world. Alan Wake's journey is deeply entwined with the dark lore of Cauldron Lake, a mysterious body of water with the power to blur the lines between fiction and reality. The lake's supernatural influence has a history of ensnaring creative minds, warping their creations into terrifying manifestations. As Alan delves deeper into this twisted reality, he encounters shadowy figures and malevolent forces drawn from his own writings, all while trying to reclaim his lost memories and escape the encroaching darkness. The lore-rich environment is filled with references to ancient myths, eerie folklore, and the psychological horror elements that define Alan's struggle. Throughout the game, players must uncover the truth behind the dark presence that haunts Cauldron Lake, confront their deepest fears, and piece together the fragmented narrative to ultimately survive the harrowing ordeal.</t>
-  </si>
-  <si>
-    <t>In "Darkest Dungeon," the introductory monologue is delivered by the Ancestor, who sets a grim and foreboding tone. This sets the stage for the game's gothic horror narrative, where players inherit a decayed estate plagued by eldritch horrors and madness. The Ancestor recounts how his insatiable curiosity and pursuit of forbidden knowledge led him to unearth a portal to an ancient, malevolent force beneath the manor. This act unleashed unspeakable evils that now corrupt the land and its inhabitants. Players take on the role of the heir, tasked with reclaiming the family estate and confronting the horrors that lurk within the Darkest Dungeon. The journey is fraught with peril, as players must assemble and lead a band of flawed heroes through nightmarish dungeons, battling terrifying creatures and coping with the ever-present threat of insanity. The game's rich lore is steeped in themes of decay, corruption, and the psychological toll of facing one's deepest fears. To restore the family’s honor, players must delve into the depths of the manor, uncover its dark secrets, and ultimately confront the ancient evil that has taken root in their ancestral home.</t>
-  </si>
-  <si>
-    <t>In "Rise of the Ronin," the introductory monologue is delivered by a narrator who sets the historical and tumultuous tone of the game. This sets the stage for the game's narrative, set during the closing days of Japan's Edo period under the Tokugawa Shogunate. For three centuries, Japan remained isolated from the rest of the world, experiencing an era of apparent peace and prosperity. However, beneath this facade, tensions simmered as the feudal lords, or Daimyo, were held under strict control, fostering seeds of rebellion. In the remote mountains of Kurosu, a secret rebellion began to take shape with the clandestine forging of weapons. The Shogunate's forces discovered the plot and responded with brutal reprisals. Yet, another formidable force was being forged: the Veiled Edge. These elite warriors, masters of stealth and swordsmanship, trained in pairs known as blade twins, were unparalleled in their abilities. Players take on the role of a member of the Veiled Edge, navigating a world filled with political intrigue, ancient traditions, and the upheaval of a nation on the brink of revolution. The game's rich lore delves into the complexities of loyalty, honor, and the struggle for freedom, set against the backdrop of a changing Japan.</t>
-  </si>
-  <si>
-    <t>In "Sekiro: Shadows Die Twice," the introductory monologue sets the stage for the game's intense and immersive narrative. Taking place in the closing years of the Sengoku era, Japan is engulfed in relentless conflict. Amidst the chaos, Master swordsman Isshin Ashina seizes control of the land through a violent coup. A young orphan from the battlefield is taken under his wing, training to become a formidable shinobi. Twenty years later, the Ashina clan faces imminent collapse, and the shinobi, known as Wolf, finds himself bereft of both his mentor and the young lord he was duty-bound to protect. Players guide Wolf through a perilous journey of vengeance and redemption, navigating a beautifully crafted world filled with deadly foes and intricate challenges, as he seeks to restore his honor and rescue his lord.</t>
-  </si>
-  <si>
-    <t>In "Pillars of Eternity II: Deadfire," the introductory monologue sets the stage for the game's rich narrative. In the world of Eora, mortals live, die, and are reborn through the Wheel, overseen by the gods and facilitated by adra pillars. Five years ago, the protagonist, whom the player controls, was transformed into a Watcher with the ability to see and speak with souls. The player ended a crisis of soulless infants and defeated the immortal agent Thaos Ix Arkannon. After uncovering that the ancient Engwithans had turned themselves into gods, the protagonist retired to rule the castle of Caed Nua. However, unresolved tensions hint at further divine machinations, propelling the player into new adventures.</t>
-  </si>
-  <si>
     <t>The Stanley Parable</t>
   </si>
   <si>
-    <t>In "The Stanley Parable," the introductory monologue sets the stage for the game's narrative. The player takes on the role of Stanley, an office worker who discovers that his colleagues have mysteriously vanished. As Stanley, the player navigates the deserted office, making choices that impact the story's direction. The game explores themes of free will, control, and the nature of decision-making, with the player's actions leading to various endings, all while a narrator comments on and sometimes reacts to Stanley's choices.</t>
-  </si>
-  <si>
-    <t>In "Killzone," the introductory monologue is delivered by Scolar Visari, the  ruthless leader of the Helghast and sets sets the stage for the game's intense and dramatic narrative. The player takes on the role of a soldier in the Interplanetary Strategic Alliance (ISA) fighting against Visari's forces. The Helghast, once oppressed and exiled to the harsh planet of Helghan, have grown stronger under Visari's leadership and now seek vengeance against those who wronged them. The player must navigate through war-torn environments, battling the formidable Helghast forces to protect their own people and prevent the Helghast from achieving their goal of conquest and retribution. The game explores themes of revenge, survival, and the brutal reality of war.</t>
-  </si>
-  <si>
-    <t>In "Call of Duty: Modern Warfare III," the introductory monologue sets the stage for the game's high-stakes narrative and is delivered by Vladimir Makarov, the primary antagonist. Makarov's actions have turned the world into a battlefield, exploiting deceit and the desire for vengeance to incite widespread conflict. The player takes on the roles of multiple soldiers across various international task forces as they combat Makarov's global threat. As the story unfolds, the player navigates through intense combat scenarios and covert operations to thwart Makarov's plans and restore peace. The game delves into themes of deception, the cost of war, and the impact of individual actions on global events.</t>
-  </si>
-  <si>
-    <t>In "BioShock," the introductory monologue is delivered by Andrew Ryan, the visionary founder of the underwater city of Rapture. This sets the stage for the game's thought-provoking narrative. The player takes on the role of Jack, a man who finds himself in the mysterious and decaying utopia of Rapture after a plane crash. As Jack explores the city, he uncovers the dark secrets behind its creation and the societal collapse that ensued. The game delves into themes of objectivism, free will, and the consequences of unbridled ambition, as the player navigates through the dystopian landscape, facing mutated inhabitants and unraveling the truth about Rapture's downfall.</t>
-  </si>
-  <si>
-    <t>In "Dragon Age: Origins," the introductory monologue is delivered by Duncan, a senior member of the Grey Wardens. This sets the stage for the game's epic fantasy narrative. The player takes on the role of a new recruit to the Grey Wardens, an ancient order dedicated to combating the darkspawn—a monstrous race that threatens to bring about another Blight. As the darkspawn menace resurfaces, the player must unite the fractured kingdoms of Thedas, form alliances, and build an army to face the looming threat. The game explores themes of sacrifice, unity, and heroism, as the player navigates a richly detailed world filled with complex characters and moral choices, ultimately striving to save the world from annihilation.</t>
-  </si>
-  <si>
-    <t>In "Child of Light," the introductory monologue is delivered by a narrator, setting the stage for the game's enchanting narrative. The player takes on the role of Aurora, a young girl who mysteriously falls into a deep sleep and awakens in the magical land of Lemuria. As Aurora, the player embarks on a quest to return home by battling dark creatures and restoring the stolen light to Lemuria. Along the way, she gathers companions and uncovers the secrets of her destiny. The game explores themes of bravery, love, and self-discovery, all wrapped in a beautifully illustrated, fairy-tale world filled with poetry and wonder.</t>
-  </si>
-  <si>
-    <t>In "Metroid Prime," the introductory monologue is delivered by the main Character, setting the stage for the game's thrilling sci-fi narrative. The player takes on the role of Samus Aran, an interstellar bounty hunter who previously defeated the Space Pirates and their leader, Mother Brain, on Planet Zebes. Despite this victory, remnants of the Space Pirate forces survived and fled to regroup. Now, Samus has discovered a potential pirate colony on Planet Tallon IV. The player must explore this alien world, uncover its secrets, and thwart the Space Pirates' plans for resurgence. The game delves into themes of exploration, survival, and the relentless pursuit of justice as Samus battles to eliminate the pirate threat once and for all.</t>
-  </si>
-  <si>
-    <t>In "Mass Effect," the introductory monologue is delivered by a narrator, setting the stage for the game's expansive sci-fi narrative. The player takes on the role of Commander Shepard, a skilled soldier in the Systems Alliance. In 2148, humanity discovered advanced technology on Mars left behind by an ancient spacefaring civilization, which enabled faster-than-light travel and ushered in a new era of space exploration. This technology, known as Mass Effect, allowed humanity to join a galactic community of diverse alien species. As Commander Shepard, the player must navigate political intrigue, form alliances, and combat a looming threat that endangers the entire galaxy. The game explores themes of unity, destiny, and the struggle to protect all life from annihilation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In "Metro 2033," the introductory monologue delivered by Artyom sets the stage for the game's intense narrative. The player assumes the role of Artyom, a young man born just before a nuclear war forced humanity to seek refuge in the underground Metro stations of Moscow. Twenty years later, the Metro has become a bastion of human survival amidst a frozen, irradiated wasteland. As Artyom, the player must navigate the dangers of both the tunnels and the surface, contending with mutants, hostile factions, and a new, mysterious threat. The game explores themes of survival, hope, and the enduring human spirit as Artyom embarks on a perilous journey to save his home and uncover the secrets of the post-apocalyptic world.
+    <t>an</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>In "The Last of Us", the introductory monologue is delivered by a news reporter who grimly details the escalating crisis. This sets the stage for the game's post-apocalyptic narrative, where society collapses due to a devastating fungal outbreak. Players follow Joel, a hardened survivor, and Ellie, a young girl who might hold the key to humanity's survival, as they navigate a world filled with infected mutants and hostile human factions. The Fireflies, a revolutionary militia group, seek to restore government control, adding to the chaos and conflict that define the game's intense and emotional journey.</t>
+  </si>
+  <si>
+    <t>In "The Witcher 3: Wild Hunt", the introductory monologue is delivered by a foreboding narrator who addresses the chaos and despair gripping the land. This sets the stage for the game's dark fantasy narrative, where players follow Geralt of Rivia, a monster hunter known as a Witcher, on a quest to find his adopted daughter Ciri, who is being pursued by the otherworldly Wild Hunt. The game is set in a war-torn world filled with political intrigue, dangerous creatures, and morally complex choices. As Geralt, players must navigate through the turmoil, battling both human and monstrous foes, while making decisions that shape the fate of the world and its inhabitants.</t>
+  </si>
+  <si>
+    <t>In "Elden Ring", the introductory monologue delivered by a narrator sets the stage for the game's epic dark fantasy narrative. The player takes on the role of a Tarnished, one of the dead who yet live, called back to the Lands Between to restore the fractured world. The once-great Elden Ring has been shattered, and Queen Marika the Eternal has disappeared. On the Night of the Black Knives, the demigod Godwin the Golden was the first to fall, leading Marika's demigod offspring to seize the shards of the Elden Ring. Their newfound power triggered the Shattering, a catastrophic war that left the Lands Between in chaos and abandoned by the Greater Will. The Tarnished, including chieftains, sorcerers, and other notable figures, are beckoned by the call of long-lost grace to reclaim their destiny. As a Tarnished of no renown, the player must cross the fog to the Lands Between, face formidable foes, and seek to reunite the Elden Ring, ultimately striving to become the Elden Lord. The game explores themes of power, legacy, and redemption in a richly detailed and mysterious world.</t>
+  </si>
+  <si>
+    <t>In "Fallout 3", the introductory monologue is delivered by the narrator, setting a grim tone for the game. This monologue introduces players to a post-apocalyptic world devastated by nuclear war in 2077. Players assume the role of a character born and raised in Vault 101, one of the many underground shelters designed to protect humanity from the horrors of nuclear fallout. The vault's motto, "no one ever enters, and no one ever leaves", shapes the protagonist's early life until circumstances force them to venture into the harsh and desolate wasteland of the Capital Wasteland. As they search for their missing father, players must navigate through a world filled with radiation, mutated creatures, and hostile factions, all while uncovering the secrets of their family's past and the broader mysteries of the post-apocalyptic society.</t>
+  </si>
+  <si>
+    <t>In "Fallout 4", the introductory monologue is delivered by the protagonist, setting the stage for the game's post-apocalyptic narrative. The game begins in 2077, just before a nuclear war devastates the world. Players take on the role of a character who survives the apocalypse by taking refuge in Vault 111. Emerging 200 years later, the protagonist finds a drastically changed world and embarks on a quest to find their kidnapped son. The journey takes them through the Commonwealth, a region filled with mutated creatures, hostile factions, and the remnants of pre-war society, as they uncover the truth about their past and influence the future of the wasteland.</t>
+  </si>
+  <si>
+    <t>In "Fallout: New Vegas", the introductory monologue is delivered by the narrator and sets the stage for the game's post-apocalyptic narrative. Players assume the role of a courier in the Mojave Desert, an area where the New California Republic and Caesar's Legion vie for control of the Hoover Dam. The city of New Vegas remains untouched by nuclear war, under the control of Mr. House and his robotic army. As the courier, players begin their journey after surviving an ambush intended to prevent the delivery of a mysterious package. The protagonist's quest for revenge and discovery leads them through a world filled with factions, conflicts, and the remnants of pre-war society, ultimately influencing the fate of New Vegas and its inhabitants.</t>
+  </si>
+  <si>
+    <t>In "Borderlands", the introductory monologue, delivered by the character Marcus Kincaid, sets the stage for the game's adventure-filled narrative. Players take on the role of Vault Hunters on the planet Pandora, a lawless and dangerous world rumored to hold the legendary Vault, filled with advanced alien technology and unimaginable riches. Guided by a mysterious Guardian Angel, the Vault Hunters embark on a quest to find this mythical treasure. The journey is filled with peril, bizarre creatures, and treacherous bandits, as they uncover the secrets of Pandora and strive to claim the legendary Vault's bounty.</t>
+  </si>
+  <si>
+    <t>In "Borderlands 2", the introductory monologue is delivered by the charismatic and humorous narrator, Marcus Kincaid. This monologue sets the stage for the game's high-stakes narrative. Players assume the role of new Vault Hunters on Pandora, a planet now infused with the rare and valuable mineral Eridium, which emerged after the first Vault's opening. The Hyperion Corporation, led by the ruthless Handsome Jack, seeks to exploit this resource and bring order to Pandora by uncovering an even greater Vault. Drawn by the promise of danger and loot, the Vault Hunters embark on a quest to stop Handsome Jack, uncover Pandora's hidden secrets, and ultimately save the planet from his tyrannical grip. The journey is filled with intense battles, quirky characters, and a struggle against the corporate oppression of Hyperion.</t>
+  </si>
+  <si>
+    <t>In "Borderlands 3", the introductory monologue is delivered by Marcus Kincaid, setting the stage for the game's thrilling adventure. Players take on the role of new Vault Hunters on the planet Pandora, a land known for its greed and violence but also its opportunities. Guided by tales of hidden alien treasures, these Vault Hunters embark on a journey answering the call of Lilith, a legendary Siren and hero of Pandora. She is assembling a team to hunt for a man leading to Vaults across the galaxy. However, dark forces have emerged, posing unprecedented threats to the Borderlands. The adventure begins with these bold and hungry Vault Hunters, embarking on a quest filled with danger, treasure, and the enduring charm of Marcus's storytelling.</t>
+  </si>
+  <si>
+    <t>In "Helldivers 2", the introductory monologue delivered by a recruitment officer sets the stage for the game's action-packed narrative. The player takes on the role of a new recruit in the Helldivers, an elite peacekeeping force dedicated to protecting Super Earth and spreading its values of democracy and freedom across the galaxy. Facing constant threats from hostile alien species such as the Bugs, Cyborgs, and Illuminates, the Helldivers engage in cooperative missions on various planets, battling to defend strategic locations and uphold their way of life. The game focuses on themes of duty, sacrifice, and the relentless fight for freedom, as players work together to complete challenging missions, combat diverse and dangerous enemies, and ensure the survival and expansion of Super Earth's ideals in an ever-dangerous universe.</t>
+  </si>
+  <si>
+    <t>In "God of War III", the introductory monologue is delivered by Gaia, the Titaness of Earth, setting the stage for the epic conclusion of Kratos's journey. The narrator recounts the rise of Kratos, who, despite becoming the new God of War, remains haunted by the tragic memories of murdering his own family. Neither death nor the Sisters of Fate could contain him. As the game begins, Kratos, driven by an unyielding desire for vengeance, embarks on a relentless quest to bring down the gods of Olympus who have wronged him. This climactic chapter sees Kratos confronting powerful deities and mythical creatures, fueled by his rage and determination to seek justice for the torment he has endured.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+In "Dying Light 2", the introductory monologue delivered by a narrator sets the stage for the game's post-apocalyptic narrative. The player takes on the role of Aiden Caldwell, a pilgrim who traverses dangerous wastelands to connect isolated human settlements. Civilization has collapsed due to a new variant of the Hurran virus, which spread rapidly after escaping from secret military research labs. Now, the remnants of humanity live in small enclaves, with one last city standing as a bastion of hope. This city is isolated, governed by unique rules, and represents humanity's final chance to learn from past mistakes. The game explores themes of survival, choice, and consequence, as every decision Aiden makes shapes the future of this fragile society. The player must navigate the city, forge alliances, and face threats both human and infected to determine the fate of humanity.</t>
+  </si>
+  <si>
+    <t>In "Assassin's Creed: Revelations", the introductory monologue is delivered by Ezio Auditore in a letter to his sister, Claudia, setting the stage for his journey. Ezio has arrived in Masyaf, seeking a hidden library mentioned by their father. This library, located beneath Masyaf Castle, is believed to contain invaluable wisdom and secrets left by the legendary Assassin, Altair. Players take on the role of Ezio, now a seasoned Master Assassin, as he navigates the perilous journey to uncover the hidden knowledge. The road to Masyaf is fraught with mercenaries and bandits, making the mission dangerous and uncertain. As Ezio, players must use their skills and cunning to overcome these threats, unravel the mysteries of the past, and gain insight into the true purpose of the Assassin Brotherhood. The game delves into Ezio's introspective quest for clarity and understanding, while also connecting his fate with that of Altair and Desmond Miles, bridging the gaps between different eras of the Assassin's Creed saga.</t>
+  </si>
+  <si>
+    <t>In "Assassin's Creed: Mirage", the introductory monologue is delivered by a narrator reflecting on the memory of a pivotal figure. This sets the stage for the game's narrative, focusing on a man who rose from being a common thief on the streets of Baghdad to a significant member of the Hidden Ones, the predecessors of the Assassin Brotherhood. Players take on the role of this man, navigating the bustling and dangerous streets of Baghdad during the height of the Abbasid Caliphate. Despite the city's golden age, a sinister rot lies beneath, with the Order of the Ancients spreading their influence and cruelty. As a member of the Hidden Ones, the protagonist engages in a shadowy struggle against these oppressive forces. The journey is not just one of external conflict but also of personal growth and understanding. The protagonist's story is a testament to honoring the Creed, challenging it, and recognizing the thin line between the shadows they walk and the light they serve. Players must navigate this complex world, making choices that reflect the eternal struggle between freedom and oppression, light and darkness.</t>
+  </si>
+  <si>
+    <t>In "Assassin's Creed III", the introductory monologue is delivered by William Miles, setting the stage for the game's narrative. He reflects on the end of the world, a concept once dismissed but now frighteningly real. The story begins with the abduction of Desmond Miles, his son, who possesses a denied heritage. Desmond was captured by Abstergo Industries, known to the Assassins as the Templars, who sought his help to find the Apple of Eden, a powerful artifact. Players take on the role of Desmond Miles, using the Animus to explore the lives of his ancestors and uncover hidden truths about the Assassins and Templars. As Desmond, players must gain the knowledge and skills of his ancestors, Altair and Ezio, to prevent an impending apocalypse foretold to occur on December 21, 2012. The journey involves mastering combat and stealth, solving complex puzzles, and making strategic decisions that impact the course of history. Armed with the Apple of Eden and supported by his fellow Assassins, Desmond stands at the brink of the final confrontation, ready to use his newfound abilities to save humanity from disaster.</t>
+  </si>
+  <si>
+    <t>In "Dark Souls III", the introductory monologue is delivered by an unseen narrator, setting the stage for the game's dark and foreboding narrative. It begins with a description of Lothric, a land where the transitory realms of the Lords of Cinder converge. As the fire fades and the lords forsake their thrones, a bell tolls, awakening the old Lords of Cinder from their graves: Aldrich, Saint of the Deep; Farron's Undead Legion, the Abyss Watchers; and Yhorm the Giant, the reclusive lord of the Profaned Capital. However, the Lords abandon their thrones, leaving the Unkindled to rise. Players assume the role of an Unkindled, a nameless and accursed undead, unfit even to be cinder. Their journey involves seeking embers, confronting the revived Lords of Cinder, and ultimately rekindling the First Flame to prevent the world from falling into darkness. The player's role is to navigate this treacherous world, mastering its challenging combat, uncovering its hidden lore, and making decisions that shape the fate of Lothric and its inhabitants.</t>
+  </si>
+  <si>
+    <t>In "Dark Souls II", the introductory monologue is delivered by an unseen narrator, setting the stage for the game's dark and mysterious narrative. The story begins by introducing a murky, forgotten land where souls can mend an ailing mind. Players are warned that they will lose everything once branded with the symbol of the curse, becoming something other than human—a Hollow. The narrative speaks of a walled-off land far to the north where a great king built the kingdom of Drangleic. As players, you assume the role of a cursed individual drawn to Drangleic without fully understanding why, like a moth to a flame. Your journey will be one of relentless anguish, facing challenges and uncovering the deep lore of this decrepit kingdom. The player's role involves navigating the perilous world of Drangleic, mastering its brutal combat, and seeking to lift the curse that plagues them, all while unraveling the secrets of this enigmatic land.</t>
+  </si>
+  <si>
+    <t>In "Dark Souls", the introductory monologue is delivered by an unseen narrator, setting the stage for the game's dark and mythic narrative. The story begins in the Age of Ancients, a time when the world was unformed and shrouded by fog, populated by gray crags, Archtrees, and Everlasting Dragons. Then, Fire emerged, bringing disparity—heat and cold, life and death, light and dark. From the dark, powerful beings found the Souls of Lords within the flame. With their newfound strength, they challenged the Dragons, leading to the Age of Fire. However, the flames are fading, and darkness threatens to take over. Now, only embers remain, and humanity is left in endless night. Among the living are those branded with the accursed Darksign. Players assume the role of an Undead, branded by the Darksign and corralled to the north, where they are locked away to await the end of the world. This is your fate. As the Undead, you must navigate a perilous world, uncover its deep lore, and seek to rekindle the fading flames, battling formidable foes and overcoming tremendous challenges along the way.</t>
+  </si>
+  <si>
+    <t>In "The Elder Scrolls IV: Oblivion", the introductory monologue is delivered by Emperor Uriel Septim VII, who reflects on his long reign and impending doom. This sets the stage for the game's epic fantasy narrative, where players take on the role of an anonymous prisoner destined to thwart a dire prophecy. As gates to the demonic realm of Oblivion open and dark forces threaten to engulf the land of Tamriel, players must navigate a richly detailed world, undertake quests, and battle fearsome enemies. The story unfolds with the player seeking to find and protect the lost heir to the throne, ultimately striving to seal the gates of Oblivion and save the Empire from destruction.</t>
+  </si>
+  <si>
+    <t>In "The Elder Scrolls Online", the introductory monologue is delivered by a narrator who sets the ominous tone of impending conflict and ancient evil. This sets the stage for the game's expansive MMORPG narrative, where players enter the world of Tamriel during a time of great turmoil and war. The year is 582 of the Second Era, and various factions vie for control of the Imperial City and the Ruby Throne. Players can choose from a variety of races and classes, embarking on epic quests, exploring vast regions, and battling both monsters and rival factions. As they uncover hidden dangers and dark schemes, players must navigate alliances and conflicts, shaping the fate of Tamriel in an ever-evolving world filled with adventure and danger.</t>
+  </si>
+  <si>
+    <t>In "Fallout 2", the introductory monologue is delivered by a narrator who reflects on the unchanging nature of war and the catastrophic events that led to the world's near-destruction. This sets the stage for the game's post-apocalyptic narrative, where players take on the role of the Chosen One, a descendant of the legendary Vault Dweller. Emerging from the tribal village of Arroyo, the player embarks on a perilous journey to save their home from ecological disaster. The story unfolds in a vast, irradiated wasteland filled with mutated creatures, ruthless factions, and remnants of pre-war technology. As the Chosen One, players must navigate this dangerous world, making crucial decisions that will determine the fate of their tribe and the future of humanity.</t>
+  </si>
+  <si>
+    <t>In "Metal Gear Solid V: The Phantom Pain", the introductory monologue is delivered by a narrator who describes the evolution of modern warfare into an automated and controlled system. This sets the stage for the game's complex narrative, where players follow the story of Big Boss, also known as Venom Snake, as he builds a new private army to take revenge on the shadowy organization Cipher. The game is set in an open world, where players undertake missions across various global conflict zones, employing stealth, strategy, and combat skills. The narrative delves into themes of revenge, loyalty, and the impact of war, all while exploring the technological advancements that have transformed the battlefield into a highly regulated and monitored environment. As Venom Snake, players must navigate this dangerous world, building and managing their own mercenary army, the Diamond Dogs. They engage in tactical espionage operations, gather resources, recruit soldiers, and develop new weapons and technology.</t>
+  </si>
+  <si>
+    <t>In "Alan Wake", the introductory monologue is delivered by the titular character, Alan Wake, a writer grappling with unsettling nightmares and a vivid imagination. This sets the stage for the game's psychological thriller narrative, where players follow Alan Wake as he embarks on a quest to find his missing wife, Alice, in the mysterious town of Bright Falls. The story begins with a haunting dream sequence that sets the tone for the surreal and dark events that follow. As Alan Wake, players explore a world where the lines between reality and fiction blur, with nightmarish occurrences manifesting from Wake's own writing. The game combines elements of action and horror, as players use light to combat the shadowy entities that emerge from the darkness. Throughout the game, players uncover manuscript pages that foreshadow events, adding to the suspense and intrigue. The narrative delves into themes of fear, the power of storytelling, and the struggle between light and darkness. Players must navigate the eerie environment, solve puzzles, and confront their deepest fears to uncover the truth behind Alice's disappearance and Alan's own psychological torment. The unanswered mysteries and unsettling atmosphere make "Alan Wake" a memorable and gripping experience.</t>
+  </si>
+  <si>
+    <t>In "Alan Wake II", the introductory monologue is delivered by a narrator who sets a haunting and mysterious tone. This sets the stage for the game's psychological horror narrative, where players follow Alan Wake, a troubled writer, as he navigates a surreal and nightmarish world. Alan Wake's journey is deeply entwined with the dark lore of Cauldron Lake, a mysterious body of water with the power to blur the lines between fiction and reality. The lake's supernatural influence has a history of ensnaring creative minds, warping their creations into terrifying manifestations. As Alan delves deeper into this twisted reality, he encounters shadowy figures and malevolent forces drawn from his own writings, all while trying to reclaim his lost memories and escape the encroaching darkness. The lore-rich environment is filled with references to ancient myths, eerie folklore, and the psychological horror elements that define Alan's struggle. Throughout the game, players must uncover the truth behind the dark presence that haunts Cauldron Lake, confront their deepest fears, and piece together the fragmented narrative to ultimately survive the harrowing ordeal.</t>
+  </si>
+  <si>
+    <t>In "Darkest Dungeon", the introductory monologue is delivered by the Ancestor, who sets a grim and foreboding tone. This sets the stage for the game's gothic horror narrative, where players inherit a decayed estate plagued by eldritch horrors and madness. The Ancestor recounts how his insatiable curiosity and pursuit of forbidden knowledge led him to unearth a portal to an ancient, malevolent force beneath the manor. This act unleashed unspeakable evils that now corrupt the land and its inhabitants. Players take on the role of the heir, tasked with reclaiming the family estate and confronting the horrors that lurk within the Darkest Dungeon. The journey is fraught with peril, as players must assemble and lead a band of flawed heroes through nightmarish dungeons, battling terrifying creatures and coping with the ever-present threat of insanity. The game's rich lore is steeped in themes of decay, corruption, and the psychological toll of facing one's deepest fears. To restore the family’s honor, players must delve into the depths of the manor, uncover its dark secrets, and ultimately confront the ancient evil that has taken root in their ancestral home.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In "NieR: Automata", the introductory monologue delivered by the protagonist, 2B, sets the stage for the game's profound and philosophical narrative. The player takes on the role of 2B, an android soldier in the YoRHa unit, tasked with fighting a proxy war on Earth between human-made androids and alien-created machines. The remnants of humanity have fled to the Moon, leaving Earth as a battleground. As 2B, alongside her companion 9S, the player uncovers hidden truths about the war, their enemies, and themselves. The game explores themes of existentialism, the nature of life and death, and the search for meaning in a seemingly endless cycle of conflict. Through intense combat and emotional storytelling, the player's choices and actions reveal the complex layers of this post-apocalyptic world, challenging their perceptions of purpose and identity.
 </t>
   </si>
   <si>
-    <t>In "Metro: Exodus," the introductory monologue delivered by Artyom sets the stage for the game's post-apocalyptic journey. The player takes on the role of Artyom, a survivor living in the Metro tunnels beneath Moscow after a devastating nuclear war. Driven by a belief that life still exists beyond the irradiated ruins, Artyom embarks on a perilous quest to find a new home on the surface. Alongside a group of fellow survivors, he travels across the vast, dangerous landscapes of Russia aboard the Aurora, a heavily modified steam locomotive. The game explores themes of survival, hope, and the search for a better future, as Artyom and his companions face hostile environments, mutated creatures, and human adversaries in their quest to rebuild their lives.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In "Vampyr," the introductory monologue sets the tone for the game's dark and atmospheric narrative. The player takes on the role of Dr. Jonathan Reid, a renowned surgeon in early 20th-century London who is transformed into a vampire amidst a deadly flu epidemic. Struggling with his new supernatural condition, Jonathan must find a balance between his duty to save the citizens as a doctor and his uncontrollable thirst for blood. As he navigates the eerie, plague-ridden streets of London, Jonathan uncovers dark secrets and faces moral dilemmas that challenge his humanity. The game explores themes of life, death, and redemption, with the player's choices deeply influencing the fate of the city's inhabitants and Jonathan's own destiny.
+    <t>In "Rise of the Ronin", the introductory monologue is delivered by a narrator who sets the historical and tumultuous tone of the game. This sets the stage for the game's narrative, set during the closing days of Japan's Edo period under the Tokugawa Shogunate. For three centuries, Japan remained isolated from the rest of the world, experiencing an era of apparent peace and prosperity. However, beneath this facade, tensions simmered as the feudal lords, or Daimyo, were held under strict control, fostering seeds of rebellion. In the remote mountains of Kurosu, a secret rebellion began to take shape with the clandestine forging of weapons. The Shogunate's forces discovered the plot and responded with brutal reprisals. Yet, another formidable force was being forged: the Veiled Edge. These elite warriors, masters of stealth and swordsmanship, trained in pairs known as blade twins, were unparalleled in their abilities. Players take on the role of a member of the Veiled Edge, navigating a world filled with political intrigue, ancient traditions, and the upheaval of a nation on the brink of revolution. The game's rich lore delves into the complexities of loyalty, honor, and the struggle for freedom, set against the backdrop of a changing Japan.</t>
+  </si>
+  <si>
+    <t>In "Sekiro: Shadows Die Twice", the introductory monologue sets the stage for the game's intense and immersive narrative. Taking place in the closing years of the Sengoku era, Japan is engulfed in relentless conflict. Amidst the chaos, Master swordsman Isshin Ashina seizes control of the land through a violent coup. A young orphan from the battlefield is taken under his wing, training to become a formidable shinobi. Twenty years later, the Ashina clan faces imminent collapse, and the shinobi, known as Wolf, finds himself bereft of both his mentor and the young lord he was duty-bound to protect. Players guide Wolf through a perilous journey of vengeance and redemption, navigating a beautifully crafted world filled with deadly foes and intricate challenges, as he seeks to restore his honor and rescue his lord.</t>
+  </si>
+  <si>
+    <t>In "Pillars of Eternity II: Deadfire", the introductory monologue sets the stage for the game's rich narrative. In the world of Eora, mortals live, die, and are reborn through the Wheel, overseen by the gods and facilitated by adra pillars. Five years ago, the protagonist, whom the player controls, was transformed into a Watcher with the ability to see and speak with souls. The player ended a crisis of soulless infants and defeated the immortal agent Thaos Ix Arkannon. After uncovering that the ancient Engwithans had turned themselves into gods, the protagonist retired to rule the castle of Caed Nua. However, unresolved tensions hint at further divine machinations, propelling the player into new adventures.</t>
+  </si>
+  <si>
+    <t>In "The Stanley Parable", the introductory monologue sets the stage for the game's narrative. The player takes on the role of Stanley, an office worker who discovers that his colleagues have mysteriously vanished. As Stanley, the player navigates the deserted office, making choices that impact the story's direction. The game explores themes of free will, control, and the nature of decision-making, with the player's actions leading to various endings, all while a narrator comments on and sometimes reacts to Stanley's choices.</t>
+  </si>
+  <si>
+    <t>In "Killzone", the introductory monologue is delivered by Scolar Visari, the  ruthless leader of the Helghast and sets sets the stage for the game's intense and dramatic narrative. The player takes on the role of a soldier in the Interplanetary Strategic Alliance (ISA) fighting against Visari's forces. The Helghast, once oppressed and exiled to the harsh planet of Helghan, have grown stronger under Visari's leadership and now seek vengeance against those who wronged them. The player must navigate through war-torn environments, battling the formidable Helghast forces to protect their own people and prevent the Helghast from achieving their goal of conquest and retribution. The game explores themes of revenge, survival, and the brutal reality of war.</t>
+  </si>
+  <si>
+    <t>In "Call of Duty: Modern Warfare III", the introductory monologue sets the stage for the game's high-stakes narrative and is delivered by Vladimir Makarov, the primary antagonist. Makarov's actions have turned the world into a battlefield, exploiting deceit and the desire for vengeance to incite widespread conflict. The player takes on the roles of multiple soldiers across various international task forces as they combat Makarov's global threat. As the story unfolds, the player navigates through intense combat scenarios and covert operations to thwart Makarov's plans and restore peace. The game delves into themes of deception, the cost of war, and the impact of individual actions on global events.</t>
+  </si>
+  <si>
+    <t>In "Batman: Arkham Knight", the introductory monologue is delivered by Commissioner Gordon, setting the stage for the game's dark and intense narrative. Gotham City has descended into chaos following the death of the Joker, with criminal elements seizing control. The player takes on the role of Batman, Gotham’s last hope, as he faces a new threat led by the mysterious Arkham Knight and the returning Scarecrow. The game follows Batman as he battles to restore order, confronting his greatest foes and grappling with his own demons. Themes of fear, redemption, and the hero’s journey are central to this final chapter in the Arkham series.</t>
+  </si>
+  <si>
+    <t>In "Half-Life 2", the introductory monologue delivered by the enigmatic G-Man sets the stage for the game's gripping and dystopian narrative. The player takes on the role of Gordon Freeman, a theoretical physicist who is awakened by the G-Man to find Earth under the oppressive rule of the alien Combine. Humanity is on the brink of extinction, and the world is heavily controlled, with citizens living in fear. As Gordon, the player must navigate through this bleak environment, joining forces with the resistance to fight against the Combine's tyranny. The game explores themes of freedom, resistance, and the impact of one individual's actions in the face of overwhelming odds. Through innovative gameplay and immersive storytelling, players experience the struggle to reclaim Earth and uncover the deeper mysteries surrounding the G-Man's intentions and the true nature of the Combine's control.</t>
+  </si>
+  <si>
+    <t>In "BioShock", the introductory monologue is delivered by Andrew Ryan, the visionary founder of the underwater city of Rapture. This sets the stage for the game's thought-provoking narrative. The player takes on the role of Jack, a man who finds himself in the mysterious and decaying utopia of Rapture after a plane crash. As Jack explores the city, he uncovers the dark secrets behind its creation and the societal collapse that ensued. The game delves into themes of objectivism, free will, and the consequences of unbridled ambition, as the player navigates through the dystopian landscape, facing mutated inhabitants and unraveling the truth about Rapture's downfall.</t>
+  </si>
+  <si>
+    <t>In "Dragon Age: Origins", the introductory monologue is delivered by Duncan, a senior member of the Grey Wardens. This sets the stage for the game's epic fantasy narrative. The player takes on the role of a new recruit to the Grey Wardens, an ancient order dedicated to combating the darkspawn—a monstrous race that threatens to bring about another Blight. As the darkspawn menace resurfaces, the player must unite the fractured kingdoms of Thedas, form alliances, and build an army to face the looming threat. The game explores themes of sacrifice, unity, and heroism, as the player navigates a richly detailed world filled with complex characters and moral choices, ultimately striving to save the world from annihilation.</t>
+  </si>
+  <si>
+    <t>In "Child of Light", the introductory monologue is delivered by a narrator, setting the stage for the game's enchanting narrative. The player takes on the role of Aurora, a young girl who mysteriously falls into a deep sleep and awakens in the magical land of Lemuria. As Aurora, the player embarks on a quest to return home by battling dark creatures and restoring the stolen light to Lemuria. Along the way, she gathers companions and uncovers the secrets of her destiny. The game explores themes of bravery, love, and self-discovery, all wrapped in a beautifully illustrated, fairy-tale world filled with poetry and wonder.</t>
+  </si>
+  <si>
+    <t>In "Metroid Prime", the introductory monologue is delivered by the main Character, setting the stage for the game's thrilling sci-fi narrative. The player takes on the role of Samus Aran, an interstellar bounty hunter who previously defeated the Space Pirates and their leader, Mother Brain, on Planet Zebes. Despite this victory, remnants of the Space Pirate forces survived and fled to regroup. Now, Samus has discovered a potential pirate colony on Planet Tallon IV. The player must explore this alien world, uncover its secrets, and thwart the Space Pirates' plans for resurgence. The game delves into themes of exploration, survival, and the relentless pursuit of justice as Samus battles to eliminate the pirate threat once and for all.</t>
+  </si>
+  <si>
+    <t>In "Mass Effect", the introductory monologue is delivered by a narrator, setting the stage for the game's expansive sci-fi narrative. The player takes on the role of Commander Shepard, a skilled soldier in the Systems Alliance. In 2148, humanity discovered advanced technology on Mars left behind by an ancient spacefaring civilization, which enabled faster-than-light travel and ushered in a new era of space exploration. This technology, known as Mass Effect, allowed humanity to join a galactic community of diverse alien species. As Commander Shepard, the player must navigate political intrigue, form alliances, and combat a looming threat that endangers the entire galaxy. The game explores themes of unity, destiny, and the struggle to protect all life from annihilation.</t>
+  </si>
+  <si>
+    <t>In "Fallout 76", the introductory monologue is delivered by the Overseer of Vault 76, setting the stage for the game's post-apocalyptic narrative. The player emerges as one of the first survivors to leave Vault 76, a secure underground shelter built to preserve America's best and brightest. The game begins on July 4th, 2076, marking 300 years since the founding of the United States. After a nuclear war devastates the world, the player must venture into the wasteland of West Virginia to rebuild society. The game explores themes of survival, community, and the enduring spirit of humanity as players work together to restore civilization in the face of a harsh and dangerous new world.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In "Metro 2033", the introductory monologue delivered by Artyom sets the stage for the game's intense narrative. The player assumes the role of Artyom, a young man born just before a nuclear war forced humanity to seek refuge in the underground Metro stations of Moscow. Twenty years later, the Metro has become a bastion of human survival amidst a frozen, irradiated wasteland. As Artyom, the player must navigate the dangers of both the tunnels and the surface, contending with mutants, hostile factions, and a new, mysterious threat. The game explores themes of survival, hope, and the enduring human spirit as Artyom embarks on a perilous journey to save his home and uncover the secrets of the post-apocalyptic world.
 </t>
   </si>
   <si>
-    <t>In "Fallout," the introductory monologue delivered by the narrator, sets the stage for the game's post-apocalyptic narrative. The player takes on the role of a Vault Dweller, a descendant of those who survived the nuclear war of 2077 by seeking refuge in Vault 13. For generations, the inhabitants have lived in the safety of the underground Vault, isolated from the devastated world above. However, the Vault's water purification chip fails, and the player is tasked with venturing into the dangerous, irradiated wasteland to find a replacement. The game explores themes of survival, the consequences of war, and the rebuilding of civilization, as the player navigates through a world filled with mutated creatures, hostile factions, and remnants of pre-war society. The player's actions and decisions will shape the future of the wasteland and determine the fate of humanity's remnants.</t>
-  </si>
-  <si>
-    <t>In "DOOM: Eternal," the introductory monologue delivered by the ARC (Armored Response Coalition) sets the stage for the game's intense and brutal narrative. The player takes on the role of the Doom Slayer, humanity's last hope against the demonic forces of Hell that have overrun Earth. Tasked with stopping the apocalypse, the Doom Slayer must battle through hordes of demons using a vast arsenal of weapons and brutal combat skills. The game explores themes of unrelenting determination, the fight against overwhelming odds, and the quest to save humanity from annihilation. As the Doom Slayer, the player navigates through various hellish landscapes, ripping and tearing through enemies to fulfill the mission: to end the demonic invasion and restore order to the universe.</t>
-  </si>
-  <si>
-    <t>In "Titanfall 2," the introductory monologue delivered by Jack Cooper sets the stage for the game's high-octane narrative. The player takes on the role of Jack Cooper, a rifleman in the Frontier Militia, who dreams of becoming a pilot—elite warriors capable of controlling powerful Titans. Pilots are fast, agile, and formidable, with a unique bond to their Titans that makes them nearly unstoppable. The Frontier, Cooper's home, has been ravaged by the oppressive IMC, which exploits the region's resources and brutalizes its inhabitants. Despite recent victories, the fight against the IMC is far from over. Cooper's journey begins with a mission that quickly spirals into chaos, leading him to inherit a Titan named BT-7274 after its pilot is killed. As Cooper and BT form a bond, the player navigates through intense combat scenarios, utilizing both Pilot agility and Titan firepower. The game explores themes of camaraderie, resilience, and the struggle for freedom, as Cooper strives to honor his fallen mentor and help liberate the Frontier from IMC control.</t>
-  </si>
-  <si>
-    <t>In "Mad Max: Fury Road," the introductory monologue delivered by Max Rockatansky sets the stage for the game's post-apocalyptic narrative. The player takes on the role of Max, a lone survivor in a desolate world where civilization has collapsed and most of humanity has perished. Those who were born into this harsh new reality know no other life, while the survivors from the old world are haunted by memories of what once was. Max, a broken man driven by his past, navigates through the wasteland, battling vicious warlords and scavenging for resources. The game explores themes of survival, loss, and the relentless fight to find hope and redemption in a brutal, unforgiving environment. As Max, the player must overcome overwhelming odds and forge alliances to endure in this desolate landscape.</t>
-  </si>
-  <si>
-    <t>In "Middle-earth: Shadow of Mordor," the introductory monologue delivered by a narrator sets the stage for the game's dark and epic narrative. The player takes on the role of Talion, a Ranger of Gondor, who is stationed at the Black Gate of Mordor. This once mighty fortress is now a desolate outpost where the Rangers have guarded against the resurgence of the Dark Lord Sauron for two and a half thousand years. As the power and malice of Sauron grow, he returns to Mordor, bringing shadow and flame that devastate the land. Talion, along with his family, falls victim to Sauron's forces, but he is resurrected and bound to a mysterious Wraith, Celebrimbor. Together, they embark on a quest for vengeance against Sauron and his minions. The game explores themes of revenge, redemption, and the blurred lines between good and evil. As Talion, the player must navigate the treacherous land of Mordor, build an army, and dismantle Sauron's forces from within using a unique nemesis system that personalizes enemy interactions and rivalries.</t>
-  </si>
-  <si>
-    <t>In "Kingdom Come: Deliverance," the introductory monologue delivered by Henry, the protagonist, sets the stage for the game's historical narrative. The game is set in the Kingdom of Bohemia during a time of great turmoil following the death of Emperor Charles IV. His son, Wenceslas IV, ascends to the throne but proves to be an ineffective ruler, neglecting his duties in favor of personal indulgences. This leads to political instability, prompting Wenceslas's half-brother, King Sigismund of Hungary, to seize the opportunity to take control. Sigismund kidnaps Wenceslas and invades Bohemia with a mercenary army, causing widespread chaos and destruction. The player takes on the role of Henry, a blacksmith's son whose peaceful life is shattered when his village is attacked by Sigismund's forces. Driven by a desire for revenge and justice, Henry becomes embroiled in the conflict, seeking to restore order to his homeland. The game explores themes of loyalty, vengeance, and the struggle for power in a meticulously recreated medieval world, where the player's choices and actions shape Henry's journey and the fate of Bohemia.</t>
-  </si>
-  <si>
-    <t>In "Batman: Arkham Knight," the introductory monologue is delivered by Commissioner Gordon, setting the stage for the game's dark and intense narrative. Gotham City has descended into chaos following the death of the Joker, with criminal elements seizing control. The player takes on the role of Batman, Gotham’s last hope, as he faces a new threat led by the mysterious Arkham Knight and the returning Scarecrow. The game follows Batman as he battles to restore order, confronting his greatest foes and grappling with his own demons. Themes of fear, redemption, and the hero’s journey are central to this final chapter in the Arkham series.</t>
-  </si>
-  <si>
-    <t>In "Elden Ring," the introductory monologue delivered by a narrator sets the stage for the game's epic dark fantasy narrative. The player takes on the role of a Tarnished, one of the dead who yet live, called back to the Lands Between to restore the fractured world. The once-great Elden Ring has been shattered, and Queen Marika the Eternal has disappeared. On the Night of the Black Knives, the demigod Godwin the Golden was the first to fall, leading Marika's demigod offspring to seize the shards of the Elden Ring. Their newfound power triggered the Shattering, a catastrophic war that left the Lands Between in chaos and abandoned by the Greater Will. The Tarnished, including chieftains, sorcerers, and other notable figures, are beckoned by the call of long-lost grace to reclaim their destiny. As a Tarnished of no renown, the player must cross the fog to the Lands Between, face formidable foes, and seek to reunite the Elden Ring, ultimately striving to become the Elden Lord. The game explores themes of power, legacy, and redemption in a richly detailed and mysterious world.</t>
-  </si>
-  <si>
-    <t>In "Helldivers 2," the introductory monologue delivered by a recruitment officer sets the stage for the game's action-packed narrative. The player takes on the role of a new recruit in the Helldivers, an elite peacekeeping force dedicated to protecting Super Earth and spreading its values of democracy and freedom across the galaxy. Facing constant threats from hostile alien species such as the Bugs, Cyborgs, and Illuminates, the Helldivers engage in cooperative missions on various planets, battling to defend strategic locations and uphold their way of life. The game focuses on themes of duty, sacrifice, and the relentless fight for freedom, as players work together to complete challenging missions, combat diverse and dangerous enemies, and ensure the survival and expansion of Super Earth's ideals in an ever-dangerous universe.</t>
-  </si>
-  <si>
-    <t>an</t>
-  </si>
-  <si>
-    <t>In "Alan Wake," the introductory monologue is delivered by the titular character, Alan Wake, a writer grappling with unsettling nightmares and a vivid imagination. This sets the stage for the game's psychological thriller narrative, where players follow Alan Wake as he embarks on a quest to find his missing wife, Alice, in the mysterious town of Bright Falls. The story begins with a haunting dream sequence that sets the tone for the surreal and dark events that follow. As Alan Wake, players explore a world where the lines between reality and fiction blur, with nightmarish occurrences manifesting from Wake's own writing. The game combines elements of action and horror, as players use light to combat the shadowy entities that emerge from the darkness. Throughout the game, players uncover manuscript pages that foreshadow events, adding to the suspense and intrigue. The narrative delves into themes of fear, the power of storytelling, and the struggle between light and darkness. Players must navigate the eerie environment, solve puzzles, and confront their deepest fears to uncover the truth behind Alice's disappearance and Alan's own psychological torment. The unanswered mysteries and unsettling atmosphere make "Alan Wake" a memorable and gripping experience.</t>
-  </si>
-  <si>
-    <t>In "Dark Souls," the introductory monologue is delivered by an unseen narrator, setting the stage for the game's dark and mythic narrative. The story begins in the Age of Ancients, a time when the world was unformed and shrouded by fog, populated by gray crags, Archtrees, and Everlasting Dragons. Then, Fire emerged, bringing disparity—heat and cold, life and death, light and dark. From the dark, powerful beings found the Souls of Lords within the flame. With their newfound strength, they challenged the Dragons, leading to the Age of Fire. However, the flames are fading, and darkness threatens to take over. Now, only embers remain, and humanity is left in endless night. Among the living are those branded with the accursed Darksign. Players assume the role of an Undead, branded by the Darksign and corralled to the north, where they are locked away to await the end of the world. This is your fate. As the Undead, you must navigate a perilous world, uncover its deep lore, and seek to rekindle the fading flames, battling formidable foes and overcoming tremendous challenges along the way.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-In "Dying Light 2," the introductory monologue delivered by a narrator sets the stage for the game's post-apocalyptic narrative. The player takes on the role of Aiden Caldwell, a pilgrim who traverses dangerous wastelands to connect isolated human settlements. Civilization has collapsed due to a new variant of the Hurran virus, which spread rapidly after escaping from secret military research labs. Now, the remnants of humanity live in small enclaves, with one last city standing as a bastion of hope. This city is isolated, governed by unique rules, and represents humanity's final chance to learn from past mistakes. The game explores themes of survival, choice, and consequence, as every decision Aiden makes shapes the future of this fragile society. The player must navigate the city, forge alliances, and face threats both human and infected to determine the fate of humanity.</t>
-  </si>
-  <si>
-    <t>In "Fallout 76," the introductory monologue is delivered by the Overseer of Vault 76, setting the stage for the game's post-apocalyptic narrative. The player emerges as one of the first survivors to leave Vault 76, a secure underground shelter built to preserve America's best and brightest. The game begins on July 4th, 2076, marking 300 years since the founding of the United States. After a nuclear war devastates the world, the player must venture into the wasteland of West Virginia to rebuild society. The game explores themes of survival, community, and the enduring spirit of humanity as players work together to restore civilization in the face of a harsh and dangerous new world.</t>
-  </si>
-  <si>
-    <t>In "Godfall," the introductory monologue delivered by the main protagonist, Orin, sets the stage for the game's epic fantasy narrative. The player takes on the role of Orin, a powerful warrior from the Knight's Order, who was betrayed by his own brother, Macros. Macros sought to achieve godhood, manipulating his fellow warriors and turning them against each other. Left for dead by Macros, Orin survives and begins a quest for vengeance. The player must gather powerful weapons and armor, known as Valorplates, to combat Macros and his army. As Orin, the player navigates through various realms, battling formidable enemies and uncovering the truth behind Macros's treachery. The game explores themes of betrayal, redemption, and the relentless pursuit of justice in a world filled with mythic heroes and divine powers.</t>
-  </si>
-  <si>
-    <t>Game</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In "NieR: Automata," the introductory monologue delivered by the protagonist, 2B, sets the stage for the game's profound and philosophical narrative. The player takes on the role of 2B, an android soldier in the YoRHa unit, tasked with fighting a proxy war on Earth between human-made androids and alien-created machines. The remnants of humanity have fled to the Moon, leaving Earth as a battleground. As 2B, alongside her companion 9S, the player uncovers hidden truths about the war, their enemies, and themselves. The game explores themes of existentialism, the nature of life and death, and the search for meaning in a seemingly endless cycle of conflict. Through intense combat and emotional storytelling, the player's choices and actions reveal the complex layers of this post-apocalyptic world, challenging their perceptions of purpose and identity.
+    <t>In "Metro: Exodus", the introductory monologue delivered by Artyom sets the stage for the game's post-apocalyptic journey. The player takes on the role of Artyom, a survivor living in the Metro tunnels beneath Moscow after a devastating nuclear war. Driven by a belief that life still exists beyond the irradiated ruins, Artyom embarks on a perilous quest to find a new home on the surface. Alongside a group of fellow survivors, he travels across the vast, dangerous landscapes of Russia aboard the Aurora, a heavily modified steam locomotive. The game explores themes of survival, hope, and the search for a better future, as Artyom and his companions face hostile environments, mutated creatures, and human adversaries in their quest to rebuild their lives.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In "Vampyr", the introductory monologue sets the tone for the game's dark and atmospheric narrative. The player takes on the role of Dr. Jonathan Reid, a renowned surgeon in early 20th-century London who is transformed into a vampire amidst a deadly flu epidemic. Struggling with his new supernatural condition, Jonathan must find a balance between his duty to save the citizens as a doctor and his uncontrollable thirst for blood. As he navigates the eerie, plague-ridden streets of London, Jonathan uncovers dark secrets and faces moral dilemmas that challenge his humanity. The game explores themes of life, death, and redemption, with the player's choices deeply influencing the fate of the city's inhabitants and Jonathan's own destiny.
 </t>
   </si>
   <si>
-    <t>In "Half-Life 2," the introductory monologue delivered by the enigmatic G-Man sets the stage for the game's gripping and dystopian narrative. The player takes on the role of Gordon Freeman, a theoretical physicist who is awakened by the G-Man to find Earth under the oppressive rule of the alien Combine. Humanity is on the brink of extinction, and the world is heavily controlled, with citizens living in fear. As Gordon, the player must navigate through this bleak environment, joining forces with the resistance to fight against the Combine's tyranny. The game explores themes of freedom, resistance, and the impact of one individual's actions in the face of overwhelming odds. Through innovative gameplay and immersive storytelling, players experience the struggle to reclaim Earth and uncover the deeper mysteries surrounding the G-Man's intentions and the true nature of the Combine's control.</t>
+    <t>In "Fallout", the introductory monologue delivered by the narrator, sets the stage for the game's post-apocalyptic narrative. The player takes on the role of a Vault Dweller, a descendant of those who survived the nuclear war of 2077 by seeking refuge in Vault 13. For generations, the inhabitants have lived in the safety of the underground Vault, isolated from the devastated world above. However, the Vault's water purification chip fails, and the player is tasked with venturing into the dangerous, irradiated wasteland to find a replacement. The game explores themes of survival, the consequences of war, and the rebuilding of civilization, as the player navigates through a world filled with mutated creatures, hostile factions, and remnants of pre-war society. The player's actions and decisions will shape the future of the wasteland and determine the fate of humanity's remnants.</t>
+  </si>
+  <si>
+    <t>In "Godfall", the introductory monologue delivered by the main protagonist, Orin, sets the stage for the game's epic fantasy narrative. The player takes on the role of Orin, a powerful warrior from the Knight's Order, who was betrayed by his own brother, Macros. Macros sought to achieve godhood, manipulating his fellow warriors and turning them against each other. Left for dead by Macros, Orin survives and begins a quest for vengeance. The player must gather powerful weapons and armor, known as Valorplates, to combat Macros and his army. As Orin, the player navigates through various realms, battling formidable enemies and uncovering the truth behind Macros's treachery. The game explores themes of betrayal, redemption, and the relentless pursuit of justice in a world filled with mythic heroes and divine powers.</t>
+  </si>
+  <si>
+    <t>In "DOOM: Eternal", the introductory monologue delivered by the ARC (Armored Response Coalition) sets the stage for the game's intense and brutal narrative. The player takes on the role of the Doom Slayer, humanity's last hope against the demonic forces of Hell that have overrun Earth. Tasked with stopping the apocalypse, the Doom Slayer must battle through hordes of demons using a vast arsenal of weapons and brutal combat skills. The game explores themes of unrelenting determination, the fight against overwhelming odds, and the quest to save humanity from annihilation. As the Doom Slayer, the player navigates through various hellish landscapes, ripping and tearing through enemies to fulfill the mission: to end the demonic invasion and restore order to the universe.</t>
+  </si>
+  <si>
+    <t>In "Titanfall 2", the introductory monologue delivered by Jack Cooper sets the stage for the game's high-octane narrative. The player takes on the role of Jack Cooper, a rifleman in the Frontier Militia, who dreams of becoming a pilot—elite warriors capable of controlling powerful Titans. Pilots are fast, agile, and formidable, with a unique bond to their Titans that makes them nearly unstoppable. The Frontier, Cooper's home, has been ravaged by the oppressive IMC, which exploits the region's resources and brutalizes its inhabitants. Despite recent victories, the fight against the IMC is far from over. Cooper's journey begins with a mission that quickly spirals into chaos, leading him to inherit a Titan named BT-7274 after its pilot is killed. As Cooper and BT form a bond, the player navigates through intense combat scenarios, utilizing both Pilot agility and Titan firepower. The game explores themes of camaraderie, resilience, and the struggle for freedom, as Cooper strives to honor his fallen mentor and help liberate the Frontier from IMC control.</t>
+  </si>
+  <si>
+    <t>In "Mad Max: Fury Road", the introductory monologue delivered by Max Rockatansky sets the stage for the game's post-apocalyptic narrative. The player takes on the role of Max, a lone survivor in a desolate world where civilization has collapsed and most of humanity has perished. Those who were born into this harsh new reality know no other life, while the survivors from the old world are haunted by memories of what once was. Max, a broken man driven by his past, navigates through the wasteland, battling vicious warlords and scavenging for resources. The game explores themes of survival, loss, and the relentless fight to find hope and redemption in a brutal, unforgiving environment. As Max, the player must overcome overwhelming odds and forge alliances to endure in this desolate landscape.</t>
+  </si>
+  <si>
+    <t>In "Middle-earth: Shadow of Mordor", the introductory monologue delivered by a narrator sets the stage for the game's dark and epic narrative. The player takes on the role of Talion, a Ranger of Gondor, who is stationed at the Black Gate of Mordor. This once mighty fortress is now a desolate outpost where the Rangers have guarded against the resurgence of the Dark Lord Sauron for two and a half thousand years. As the power and malice of Sauron grow, he returns to Mordor, bringing shadow and flame that devastate the land. Talion, along with his family, falls victim to Sauron's forces, but he is resurrected and bound to a mysterious Wraith, Celebrimbor. Together, they embark on a quest for vengeance against Sauron and his minions. The game explores themes of revenge, redemption, and the blurred lines between good and evil. As Talion, the player must navigate the treacherous land of Mordor, build an army, and dismantle Sauron's forces from within using a unique nemesis system that personalizes enemy interactions and rivalries.</t>
+  </si>
+  <si>
+    <t>In "Kingdom Come: Deliverance", the introductory monologue delivered by Henry, the protagonist, sets the stage for the game's historical narrative. The game is set in the Kingdom of Bohemia during a time of great turmoil following the death of Emperor Charles IV. His son, Wenceslas IV, ascends to the throne but proves to be an ineffective ruler, neglecting his duties in favor of personal indulgences. This leads to political instability, prompting Wenceslas's half-brother, King Sigismund of Hungary, to seize the opportunity to take control. Sigismund kidnaps Wenceslas and invades Bohemia with a mercenary army, causing widespread chaos and destruction. The player takes on the role of Henry, a blacksmith's son whose peaceful life is shattered when his village is attacked by Sigismund's forces. Driven by a desire for revenge and justice, Henry becomes embroiled in the conflict, seeking to restore order to his homeland. The game explores themes of loyalty, vengeance, and the struggle for power in a meticulously recreated medieval world, where the player's choices and actions shape Henry's journey and the fate of Bohemia.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of confirmed deaths has passed 200. The governor has called a state of emergency. Hundreds of bodies line the streets. Panic spread worldwide after a leaked report from the World Health Organization showed that the latest vaccination tests have failed. Bureaucrats have power, and we can finally take necessary actions. Los Angeles is now under martial law. All residents must report to designated quarantines. This has continued for a third consecutive day, and winter rations are at an all-time low. A group called the Fireflies claimed responsibility for both attacks. Their public charter calls for the return of all branches of government. Demonstrations broke out following the execution of six more alleged Fireflies. Still rise with us. Remember, when you are lost in the darkness, look for the light. Believe in the Fireflies.
+</t>
+  </si>
+  <si>
+    <t>I see you gather before me, hungry, terrified, clutching your babes to your breasts. Emperor Emhyr has marched his legions into our lands, laid siege to every fortress from here to the Blue Mountains. Rabid and ravenous, he bites and bites away. Men of the North, you stand at the precipice; your kings have failed you. So now you turn to the gods. And yet you do not plead, you do not kneel to dust your heads with ash. Instead, you wail, Why have the gods forsaken us? We must look into the trials we failed long ago. In a time past, our world intertwined with another through an upheaval scholars call the Conjunction of the Spheres. The gods allowed unholy forces to slip into our domain. The offspring of that cataclysm was the nefarious force called magic. Yet we did not banish it. Instead, we studied the arcane for our own power and wealth. And the monsters at our door—the unholy relics of this conjunction, the trolls, the corpse eaters. Did we raise our swords against them? Or have we laid this burden on others, on so-called witches? Stray children taught the ways of foul sorcery, their bodies mutated through blasphemous ritual, sent to fight monsters, though they could not distinguish good from evil. The flicker of humanity long extinguished within them. Yes, their numbers have dwindled through the years, but a few still roam our lands, offering their bloody work for coin. To this day, they shame us with their very existence. The North bleeds, flogged by war. The battles are the gods' whip, chastisement for our sins. Let us not forget the terrors; the scourge is from beyond our world. The Wild Hunt rides the sky with every full moon. The dark raiders abduct our children into lands unknown. Some say they herald a second conjunction. Can we chart a course back into the light? Will we find the strength to banish the mages from our kingdoms, unite around the warmth of the eternal fire? Nigh is the time of the sword and axe. Nigh is the time of madness and disdain.</t>
+  </si>
+  <si>
+    <t>War. War never changes. When atomic fire consumed the earth, those who survived did so in great underground vaults. When they opened, their inhabitants set out across the ruins to build new societies. As decades passed, the American Southwest united under the New California Republic, dedicated to democracy and the rule of law. As the Republic grew, it sent scouts east into the Mojave Desert. They found a city untouched by warheads and a great wall spanning the Colorado River. The NCR sent its army to occupy Hoover Dam. Meanwhile, Caesar's Legion, a vast army of slaves, rose across the Colorado. Four years ago, the NCR barely held the dam against the Legion's onslaught. The Legion now gathers strength. The New Vegas Strip remains open under Mr. House and his robots. You are a courier, hired to deliver a package to New Vegas, but your job has taken a turn for the worse. Sorry you got twisted up in this. From where you're kneeling, it must seem like an 18-carat run of bad luck. The truth is, the game was rigged from the start.</t>
+  </si>
+  <si>
+    <t>Yes, indeed. It is called Lothric, where the transitory lands of the Lords of Cinder converge. In venturing north, the pilgrims discover the truth of the old words: (The fire fades and the lords go without thrones.) When the link of fire is threatened, the bell tolls, unearthing the old Lords of Cinder from their graves...Aldrich, Saint of the Deep... Farron's Undead Legion, the Abyss Watchers... And the reclusive lord of the Profaned Capital, Yhorm the Giant... Only, in truth... the Lords will abandon their thrones... And the Unkindled will rise. Nameless, accursed Undead, unfit even to be cinder. And so it is, that ash seeketh embers.</t>
+  </si>
+  <si>
+    <t>Eora: a world where mortals live, die, and are reborn through the turning of the Wheel, the cycle of reincarnation is watched over by the gods and made possible through pillars of a mystical substance known as adra. Five years ago, you traveled from your home to the Deerwood, a nation that had waged war against the incarnated God of Light, Eothas, resulting in his destruction. The country suffered from a plague of Hollowborn infants, born without souls, a tragedy many believed was punishment for killing a god.
+In an ancient, secluded ruin, you witnessed a secret ritual that inadvertently transformed you into a Watcher, one who can see and speak with souls. This ritual also gave you horrible visions—waking nightmares of a past life that threatened your sanity. To put them to rest, you pursued the man who had led the ritual, a seemingly immortal agent of the gods known as Thaos Ix Arkannon. With divine assistance, you confronted and defeated Thaos, ending your visions and resolving the Hollowborn crisis. In so doing, you also learned the great secret that Thaos had protected: that the ancient empire of Engwith had transformed themselves into gods.
+Your visions finally put to rest, you retired to the castle of Caed Nua, built atop a massive statue of pure adra, where you ruled in relative peace and prosperity. 
+Made a nice story. You fixing up that old keep, lifting the curse. Must ‘ve told it a hundred times. But … something got to gnawin’ at me… Thinkin’ the spirits there were not really at rest. Maybe the gods weren't finished with us yet. I used to dream that when my god came back, he would forgive us. That's the trouble with dreams… sooner or later, we all have to wake up.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5596,12 +5596,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0D0D0D"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -5653,7 +5647,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5972,7 +5966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11C34C5E-0A98-4EB7-8A58-E8E94873121E}">
   <dimension ref="A1:C161"/>
   <sheetViews>
-    <sheetView topLeftCell="A135" workbookViewId="0">
+    <sheetView topLeftCell="A72" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -21396,67 +21390,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48AA9C6D-EFEE-4389-B779-BD4A88AD0E00}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C35" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40.33203125" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" style="9" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1811</v>
-      </c>
-      <c r="B1" s="7" t="s">
+        <v>1758</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>1662</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>1759</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1754</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1661</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>1665</v>
+      <c r="B2" s="9" t="s">
+        <v>1809</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>1760</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="375" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1663</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>1664</v>
+      <c r="B3" s="9" t="s">
+        <v>1810</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>1664</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>1666</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>1668</v>
-      </c>
       <c r="C4" s="7" t="s">
-        <v>1803</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>1665</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>1667</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>1669</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>1762</v>
@@ -21464,10 +21458,10 @@
     </row>
     <row r="6" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>1805</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>1670</v>
+        <v>1757</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>1668</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>1763</v>
@@ -21475,65 +21469,65 @@
     </row>
     <row r="7" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>1671</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>1672</v>
+        <v>1669</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>1811</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1764</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>1675</v>
+        <v>1755</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>1672</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>1670</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>1673</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>1676</v>
-      </c>
       <c r="C9" s="7" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>1674</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>1677</v>
-      </c>
       <c r="C10" s="7" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>1682</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>1678</v>
+        <v>1679</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>1675</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>1804</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>1702</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>1679</v>
+        <v>1698</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>1676</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>1769</v>
@@ -21541,431 +21535,431 @@
     </row>
     <row r="13" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>1680</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>1681</v>
+        <v>1677</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>1678</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>1808</v>
+        <v>1770</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>1684</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>1683</v>
+        <v>1681</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>1680</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>1770</v>
+        <v>1771</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>1685</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>1686</v>
+        <v>1682</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>1683</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>1771</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>1687</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>1688</v>
+        <v>1684</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>1685</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>1772</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>1701</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>1689</v>
+        <v>1697</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>1812</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>1773</v>
+        <v>1774</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>1690</v>
+        <v>1696</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>1686</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>1774</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>1691</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>1692</v>
+        <v>1687</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>1688</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>1807</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>1693</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>1694</v>
+        <v>1689</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>1690</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>1775</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>1695</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>1696</v>
+        <v>1691</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>1692</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>1776</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>1697</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>1698</v>
+        <v>1693</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>1694</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>1777</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>1699</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>1703</v>
-      </c>
       <c r="C23" s="7" t="s">
-        <v>1778</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>1704</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>1705</v>
+        <v>1700</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>1701</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>1806</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>1706</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>1707</v>
+        <v>1702</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>1703</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>1779</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>1708</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>1709</v>
+        <v>1704</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>1705</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>1780</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>1710</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>1711</v>
+        <v>1706</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>1707</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>1812</v>
+        <v>1784</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>1712</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>1713</v>
+        <v>1708</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>1709</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>1781</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>1714</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>1715</v>
+        <v>1710</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>1711</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>1782</v>
+        <v>1786</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>1716</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>1717</v>
+        <v>1712</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>1813</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>1783</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>1784</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>1718</v>
+        <v>1756</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>1713</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>1785</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>1720</v>
+        <v>1714</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>1715</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>1786</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>1721</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>1722</v>
+        <v>1716</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>1717</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>1787</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>1752</v>
+        <v>1718</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>1747</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>1802</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>1724</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>1725</v>
+        <v>1719</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>1720</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>1813</v>
+        <v>1792</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>1726</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>1727</v>
+        <v>1721</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>1722</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>1788</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>1728</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>1729</v>
+        <v>1723</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>1724</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>1789</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>1730</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>1731</v>
+        <v>1725</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>1726</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>1790</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>1733</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>1732</v>
+        <v>1728</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>1727</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>1791</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>1734</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>1735</v>
+        <v>1729</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>1730</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>1792</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>1736</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>1737</v>
+        <v>1731</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>1732</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>1809</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>1739</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>1738</v>
+        <v>1734</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>1733</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>1793</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>1740</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>1741</v>
+        <v>1735</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>1736</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>1794</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>1743</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>1742</v>
+        <v>1738</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>1737</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>1795</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>1744</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>1745</v>
+        <v>1739</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>1740</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>1796</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>1747</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>1746</v>
+        <v>1742</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>1741</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>1810</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>1749</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>1748</v>
+        <v>1744</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>1743</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>1797</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>1750</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>1751</v>
+        <v>1745</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>1746</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>1798</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>1753</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>1754</v>
+        <v>1748</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>1749</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>1799</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>1756</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>1755</v>
+        <v>1751</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>1750</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>1800</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>1758</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>1757</v>
+        <v>1753</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>1752</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>1801</v>
+        <v>1808</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix minor issues with the dataset, and started fix on an issue with the tokenization
</commit_message>
<xml_diff>
--- a/testing_excel.xlsx
+++ b/testing_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pumukl\Documents\GitHub\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32C6079-875F-4D3E-B135-9AAADC6F8E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274CD5DF-AEE5-4413-8D23-70175A2FEB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="769" firstSheet="10" activeTab="15" xr2:uid="{3104A2F9-7A17-4E5B-B5FF-CB166158170B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="769" firstSheet="17" activeTab="25" xr2:uid="{3104A2F9-7A17-4E5B-B5FF-CB166158170B}"/>
   </bookViews>
   <sheets>
     <sheet name="Greeting_Goodbyes" sheetId="2" r:id="rId1"/>
@@ -5349,9 +5349,6 @@
     <t>The Stanley Parable</t>
   </si>
   <si>
-    <t>an</t>
-  </si>
-  <si>
     <t>Game</t>
   </si>
   <si>
@@ -5673,6 +5670,9 @@
   </si>
   <si>
     <t>I'm not.</t>
+  </si>
+  <si>
+    <t>Fallout 4</t>
   </si>
 </sst>
 </file>
@@ -11670,7 +11670,7 @@
         <v>869</v>
       </c>
       <c r="D29" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -11684,7 +11684,7 @@
         <v>869</v>
       </c>
       <c r="D30" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -11698,7 +11698,7 @@
         <v>869</v>
       </c>
       <c r="D31" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -11712,7 +11712,7 @@
         <v>869</v>
       </c>
       <c r="D32" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -11726,7 +11726,7 @@
         <v>869</v>
       </c>
       <c r="D33" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -11740,7 +11740,7 @@
         <v>869</v>
       </c>
       <c r="D34" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -11754,7 +11754,7 @@
         <v>869</v>
       </c>
       <c r="D35" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -11768,7 +11768,7 @@
         <v>869</v>
       </c>
       <c r="D36" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -11782,7 +11782,7 @@
         <v>869</v>
       </c>
       <c r="D37" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -11796,7 +11796,7 @@
         <v>869</v>
       </c>
       <c r="D38" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -11810,7 +11810,7 @@
         <v>869</v>
       </c>
       <c r="D39" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -11824,7 +11824,7 @@
         <v>869</v>
       </c>
       <c r="D40" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -11838,7 +11838,7 @@
         <v>869</v>
       </c>
       <c r="D41" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -11852,7 +11852,7 @@
         <v>869</v>
       </c>
       <c r="D42" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -11866,7 +11866,7 @@
         <v>869</v>
       </c>
       <c r="D43" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -11880,7 +11880,7 @@
         <v>869</v>
       </c>
       <c r="D44" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -11894,7 +11894,7 @@
         <v>869</v>
       </c>
       <c r="D45" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -11908,7 +11908,7 @@
         <v>869</v>
       </c>
       <c r="D46" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -11922,7 +11922,7 @@
         <v>869</v>
       </c>
       <c r="D47" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -11936,7 +11936,7 @@
         <v>869</v>
       </c>
       <c r="D48" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -11950,7 +11950,7 @@
         <v>869</v>
       </c>
       <c r="D49" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -11964,7 +11964,7 @@
         <v>869</v>
       </c>
       <c r="D50" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -11978,7 +11978,7 @@
         <v>869</v>
       </c>
       <c r="D51" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -11992,7 +11992,7 @@
         <v>869</v>
       </c>
       <c r="D52" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -12006,7 +12006,7 @@
         <v>869</v>
       </c>
       <c r="D53" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -12020,7 +12020,7 @@
         <v>869</v>
       </c>
       <c r="D54" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -12034,7 +12034,7 @@
         <v>869</v>
       </c>
       <c r="D55" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -12048,7 +12048,7 @@
         <v>870</v>
       </c>
       <c r="D56" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -12062,7 +12062,7 @@
         <v>870</v>
       </c>
       <c r="D57" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -12076,7 +12076,7 @@
         <v>871</v>
       </c>
       <c r="D58" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -12090,7 +12090,7 @@
         <v>871</v>
       </c>
       <c r="D59" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -12104,7 +12104,7 @@
         <v>871</v>
       </c>
       <c r="D60" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -12118,7 +12118,7 @@
         <v>871</v>
       </c>
       <c r="D61" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -12132,7 +12132,7 @@
         <v>871</v>
       </c>
       <c r="D62" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -12146,7 +12146,7 @@
         <v>871</v>
       </c>
       <c r="D63" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -12160,7 +12160,7 @@
         <v>871</v>
       </c>
       <c r="D64" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -12174,7 +12174,7 @@
         <v>871</v>
       </c>
       <c r="D65" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -12188,7 +12188,7 @@
         <v>872</v>
       </c>
       <c r="D66" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -12202,7 +12202,7 @@
         <v>873</v>
       </c>
       <c r="D67" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -12216,7 +12216,7 @@
         <v>873</v>
       </c>
       <c r="D68" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -12230,7 +12230,7 @@
         <v>873</v>
       </c>
       <c r="D69" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -12244,7 +12244,7 @@
         <v>873</v>
       </c>
       <c r="D70" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -12258,7 +12258,7 @@
         <v>873</v>
       </c>
       <c r="D71" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -12272,7 +12272,7 @@
         <v>873</v>
       </c>
       <c r="D72" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -12286,7 +12286,7 @@
         <v>873</v>
       </c>
       <c r="D73" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -12300,7 +12300,7 @@
         <v>873</v>
       </c>
       <c r="D74" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -12314,7 +12314,7 @@
         <v>874</v>
       </c>
       <c r="D75" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -12328,7 +12328,7 @@
         <v>874</v>
       </c>
       <c r="D76" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -12342,7 +12342,7 @@
         <v>875</v>
       </c>
       <c r="D77" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -12356,7 +12356,7 @@
         <v>875</v>
       </c>
       <c r="D78" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -12370,7 +12370,7 @@
         <v>876</v>
       </c>
       <c r="D79" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -12384,7 +12384,7 @@
         <v>876</v>
       </c>
       <c r="D80" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -12398,7 +12398,7 @@
         <v>876</v>
       </c>
       <c r="D81" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -12412,7 +12412,7 @@
         <v>876</v>
       </c>
       <c r="D82" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -12426,7 +12426,7 @@
         <v>877</v>
       </c>
       <c r="D83" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -12440,7 +12440,7 @@
         <v>877</v>
       </c>
       <c r="D84" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -12566,7 +12566,7 @@
         <v>879</v>
       </c>
       <c r="D93" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -12594,7 +12594,7 @@
         <v>880</v>
       </c>
       <c r="D95" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -12608,7 +12608,7 @@
         <v>880</v>
       </c>
       <c r="D96" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -12622,7 +12622,7 @@
         <v>880</v>
       </c>
       <c r="D97" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -12636,7 +12636,7 @@
         <v>880</v>
       </c>
       <c r="D98" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -12650,7 +12650,7 @@
         <v>880</v>
       </c>
       <c r="D99" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -12664,7 +12664,7 @@
         <v>880</v>
       </c>
       <c r="D100" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -12678,7 +12678,7 @@
         <v>880</v>
       </c>
       <c r="D101" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -12692,7 +12692,7 @@
         <v>881</v>
       </c>
       <c r="D102" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -12706,7 +12706,7 @@
         <v>881</v>
       </c>
       <c r="D103" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -12720,7 +12720,7 @@
         <v>882</v>
       </c>
       <c r="D104" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -12734,7 +12734,7 @@
         <v>882</v>
       </c>
       <c r="D105" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -12748,7 +12748,7 @@
         <v>883</v>
       </c>
       <c r="D106" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -12762,7 +12762,7 @@
         <v>883</v>
       </c>
       <c r="D107" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -12776,7 +12776,7 @@
         <v>883</v>
       </c>
       <c r="D108" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -12790,7 +12790,7 @@
         <v>883</v>
       </c>
       <c r="D109" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -12804,7 +12804,7 @@
         <v>884</v>
       </c>
       <c r="D110" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -12818,7 +12818,7 @@
         <v>884</v>
       </c>
       <c r="D111" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -12944,7 +12944,7 @@
         <v>886</v>
       </c>
       <c r="D120" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -12958,7 +12958,7 @@
         <v>887</v>
       </c>
       <c r="D121" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -12972,7 +12972,7 @@
         <v>887</v>
       </c>
       <c r="D122" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -12986,7 +12986,7 @@
         <v>887</v>
       </c>
       <c r="D123" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -13000,7 +13000,7 @@
         <v>887</v>
       </c>
       <c r="D124" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -13014,7 +13014,7 @@
         <v>887</v>
       </c>
       <c r="D125" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -13028,7 +13028,7 @@
         <v>887</v>
       </c>
       <c r="D126" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -13042,7 +13042,7 @@
         <v>887</v>
       </c>
       <c r="D127" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -13056,7 +13056,7 @@
         <v>887</v>
       </c>
       <c r="D128" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -13070,7 +13070,7 @@
         <v>888</v>
       </c>
       <c r="D129" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -13084,7 +13084,7 @@
         <v>888</v>
       </c>
       <c r="D130" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -13098,7 +13098,7 @@
         <v>889</v>
       </c>
       <c r="D131" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -13112,7 +13112,7 @@
         <v>889</v>
       </c>
       <c r="D132" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -13126,7 +13126,7 @@
         <v>890</v>
       </c>
       <c r="D133" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -13140,7 +13140,7 @@
         <v>890</v>
       </c>
       <c r="D134" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -13154,7 +13154,7 @@
         <v>890</v>
       </c>
       <c r="D135" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -13168,7 +13168,7 @@
         <v>890</v>
       </c>
       <c r="D136" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -13182,7 +13182,7 @@
         <v>891</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -13196,7 +13196,7 @@
         <v>891</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -13210,7 +13210,7 @@
         <v>892</v>
       </c>
       <c r="D139" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -13224,7 +13224,7 @@
         <v>892</v>
       </c>
       <c r="D140" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -13238,7 +13238,7 @@
         <v>892</v>
       </c>
       <c r="D141" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -13252,7 +13252,7 @@
         <v>892</v>
       </c>
       <c r="D142" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -13266,7 +13266,7 @@
         <v>892</v>
       </c>
       <c r="D143" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -13280,7 +13280,7 @@
         <v>892</v>
       </c>
       <c r="D144" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -13294,7 +13294,7 @@
         <v>892</v>
       </c>
       <c r="D145" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -13308,7 +13308,7 @@
         <v>892</v>
       </c>
       <c r="D146" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -13322,7 +13322,7 @@
         <v>893</v>
       </c>
       <c r="D147" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -13336,7 +13336,7 @@
         <v>894</v>
       </c>
       <c r="D148" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -13350,7 +13350,7 @@
         <v>894</v>
       </c>
       <c r="D149" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -13364,7 +13364,7 @@
         <v>894</v>
       </c>
       <c r="D150" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -13378,7 +13378,7 @@
         <v>894</v>
       </c>
       <c r="D151" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -13392,7 +13392,7 @@
         <v>894</v>
       </c>
       <c r="D152" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -13406,7 +13406,7 @@
         <v>894</v>
       </c>
       <c r="D153" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -13420,7 +13420,7 @@
         <v>894</v>
       </c>
       <c r="D154" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -13434,7 +13434,7 @@
         <v>894</v>
       </c>
       <c r="D155" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -13448,7 +13448,7 @@
         <v>895</v>
       </c>
       <c r="D156" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -13462,7 +13462,7 @@
         <v>895</v>
       </c>
       <c r="D157" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -13476,7 +13476,7 @@
         <v>896</v>
       </c>
       <c r="D158" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -13490,7 +13490,7 @@
         <v>896</v>
       </c>
       <c r="D159" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -13504,7 +13504,7 @@
         <v>897</v>
       </c>
       <c r="D160" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -13518,7 +13518,7 @@
         <v>897</v>
       </c>
       <c r="D161" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -13532,7 +13532,7 @@
         <v>897</v>
       </c>
       <c r="D162" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -13546,7 +13546,7 @@
         <v>897</v>
       </c>
       <c r="D163" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -13560,7 +13560,7 @@
         <v>898</v>
       </c>
       <c r="D164" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -13574,7 +13574,7 @@
         <v>898</v>
       </c>
       <c r="D165" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -13588,7 +13588,7 @@
         <v>899</v>
       </c>
       <c r="D166" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -13602,7 +13602,7 @@
         <v>899</v>
       </c>
       <c r="D167" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -13616,7 +13616,7 @@
         <v>899</v>
       </c>
       <c r="D168" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -13630,7 +13630,7 @@
         <v>899</v>
       </c>
       <c r="D169" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -13644,7 +13644,7 @@
         <v>899</v>
       </c>
       <c r="D170" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -13658,7 +13658,7 @@
         <v>899</v>
       </c>
       <c r="D171" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -13672,7 +13672,7 @@
         <v>899</v>
       </c>
       <c r="D172" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -13686,7 +13686,7 @@
         <v>899</v>
       </c>
       <c r="D173" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -13700,7 +13700,7 @@
         <v>900</v>
       </c>
       <c r="D174" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -13714,7 +13714,7 @@
         <v>901</v>
       </c>
       <c r="D175" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -13728,7 +13728,7 @@
         <v>901</v>
       </c>
       <c r="D176" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -13742,7 +13742,7 @@
         <v>901</v>
       </c>
       <c r="D177" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -13756,7 +13756,7 @@
         <v>901</v>
       </c>
       <c r="D178" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -13770,7 +13770,7 @@
         <v>901</v>
       </c>
       <c r="D179" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -13784,7 +13784,7 @@
         <v>901</v>
       </c>
       <c r="D180" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -13798,7 +13798,7 @@
         <v>901</v>
       </c>
       <c r="D181" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -13812,7 +13812,7 @@
         <v>901</v>
       </c>
       <c r="D182" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -13826,7 +13826,7 @@
         <v>902</v>
       </c>
       <c r="D183" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -13840,7 +13840,7 @@
         <v>902</v>
       </c>
       <c r="D184" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -13854,7 +13854,7 @@
         <v>903</v>
       </c>
       <c r="D185" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -13868,7 +13868,7 @@
         <v>903</v>
       </c>
       <c r="D186" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -13882,7 +13882,7 @@
         <v>904</v>
       </c>
       <c r="D187" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -13896,7 +13896,7 @@
         <v>904</v>
       </c>
       <c r="D188" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -13910,7 +13910,7 @@
         <v>904</v>
       </c>
       <c r="D189" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -13924,7 +13924,7 @@
         <v>904</v>
       </c>
       <c r="D190" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
     </row>
   </sheetData>
@@ -13936,7 +13936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69F32C0-2867-41D3-BE5A-029A07962BF9}">
   <dimension ref="A1:D136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
@@ -19589,7 +19589,7 @@
         <v>1303</v>
       </c>
       <c r="B12" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -19597,7 +19597,7 @@
         <v>1304</v>
       </c>
       <c r="B13" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -19605,7 +19605,7 @@
         <v>1305</v>
       </c>
       <c r="B14" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -19613,7 +19613,7 @@
         <v>1306</v>
       </c>
       <c r="B15" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -19621,7 +19621,7 @@
         <v>1307</v>
       </c>
       <c r="B16" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -19629,7 +19629,7 @@
         <v>1308</v>
       </c>
       <c r="B17" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -19637,7 +19637,7 @@
         <v>1308</v>
       </c>
       <c r="B18" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -19645,7 +19645,7 @@
         <v>1309</v>
       </c>
       <c r="B19" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -19653,7 +19653,7 @@
         <v>1310</v>
       </c>
       <c r="B20" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -19661,7 +19661,7 @@
         <v>1311</v>
       </c>
       <c r="B21" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
     </row>
   </sheetData>
@@ -21498,8 +21498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48AA9C6D-EFEE-4389-B779-BD4A88AD0E00}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21511,7 +21511,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>1650</v>
@@ -21525,10 +21525,10 @@
         <v>1649</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="375" customHeight="1" x14ac:dyDescent="0.25">
@@ -21536,10 +21536,10 @@
         <v>1651</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21550,7 +21550,7 @@
         <v>1654</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21561,18 +21561,18 @@
         <v>1655</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1745</v>
+        <v>1850</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>1656</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21580,10 +21580,10 @@
         <v>1657</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21594,7 +21594,7 @@
         <v>1660</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21605,7 +21605,7 @@
         <v>1661</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21616,7 +21616,7 @@
         <v>1662</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21627,7 +21627,7 @@
         <v>1663</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21638,7 +21638,7 @@
         <v>1664</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21649,7 +21649,7 @@
         <v>1666</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21660,7 +21660,7 @@
         <v>1668</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21671,7 +21671,7 @@
         <v>1671</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21682,7 +21682,7 @@
         <v>1673</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21690,10 +21690,10 @@
         <v>1685</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21704,7 +21704,7 @@
         <v>1674</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21715,7 +21715,7 @@
         <v>1676</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21726,7 +21726,7 @@
         <v>1678</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21737,7 +21737,7 @@
         <v>1680</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21748,7 +21748,7 @@
         <v>1682</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21759,7 +21759,7 @@
         <v>1687</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21770,7 +21770,7 @@
         <v>1689</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21781,7 +21781,7 @@
         <v>1691</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21792,7 +21792,7 @@
         <v>1693</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21803,7 +21803,7 @@
         <v>1695</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21814,7 +21814,7 @@
         <v>1697</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21825,7 +21825,7 @@
         <v>1699</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21833,10 +21833,10 @@
         <v>1700</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21847,7 +21847,7 @@
         <v>1701</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21858,7 +21858,7 @@
         <v>1703</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21869,7 +21869,7 @@
         <v>1705</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21880,7 +21880,7 @@
         <v>1735</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21891,7 +21891,7 @@
         <v>1708</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21902,7 +21902,7 @@
         <v>1710</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21913,7 +21913,7 @@
         <v>1712</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21924,7 +21924,7 @@
         <v>1714</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21935,7 +21935,7 @@
         <v>1715</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21946,7 +21946,7 @@
         <v>1718</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21957,7 +21957,7 @@
         <v>1720</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21968,7 +21968,7 @@
         <v>1721</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21979,7 +21979,7 @@
         <v>1724</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21990,7 +21990,7 @@
         <v>1725</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -22001,7 +22001,7 @@
         <v>1728</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -22012,7 +22012,7 @@
         <v>1729</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -22023,7 +22023,7 @@
         <v>1731</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -22034,7 +22034,7 @@
         <v>1734</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -22045,7 +22045,7 @@
         <v>1737</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -22056,7 +22056,7 @@
         <v>1738</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -22067,7 +22067,7 @@
         <v>1740</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
     </row>
   </sheetData>
@@ -23133,7 +23133,7 @@
         <v>265</v>
       </c>
       <c r="C2" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -23144,7 +23144,7 @@
         <v>266</v>
       </c>
       <c r="C3" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -23155,7 +23155,7 @@
         <v>267</v>
       </c>
       <c r="C4" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -23166,7 +23166,7 @@
         <v>268</v>
       </c>
       <c r="C5" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -23177,7 +23177,7 @@
         <v>269</v>
       </c>
       <c r="C6" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -23188,7 +23188,7 @@
         <v>270</v>
       </c>
       <c r="C7" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -23199,7 +23199,7 @@
         <v>272</v>
       </c>
       <c r="C8" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -23210,7 +23210,7 @@
         <v>272</v>
       </c>
       <c r="C9" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -23221,7 +23221,7 @@
         <v>274</v>
       </c>
       <c r="C10" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -23232,7 +23232,7 @@
         <v>275</v>
       </c>
       <c r="C11" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -23243,7 +23243,7 @@
         <v>275</v>
       </c>
       <c r="C12" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -23254,7 +23254,7 @@
         <v>276</v>
       </c>
       <c r="C13" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -23265,7 +23265,7 @@
         <v>277</v>
       </c>
       <c r="C14" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -23276,7 +23276,7 @@
         <v>278</v>
       </c>
       <c r="C15" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -23287,7 +23287,7 @@
         <v>279</v>
       </c>
       <c r="C16" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -23298,7 +23298,7 @@
         <v>280</v>
       </c>
       <c r="C17" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -23309,7 +23309,7 @@
         <v>281</v>
       </c>
       <c r="C18" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -23320,7 +23320,7 @@
         <v>282</v>
       </c>
       <c r="C19" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -23331,7 +23331,7 @@
         <v>283</v>
       </c>
       <c r="C20" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -23342,7 +23342,7 @@
         <v>302</v>
       </c>
       <c r="C21" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -23353,7 +23353,7 @@
         <v>284</v>
       </c>
       <c r="C22" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -23364,7 +23364,7 @@
         <v>285</v>
       </c>
       <c r="C23" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -23375,7 +23375,7 @@
         <v>285</v>
       </c>
       <c r="C24" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -23386,7 +23386,7 @@
         <v>286</v>
       </c>
       <c r="C25" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -23397,7 +23397,7 @@
         <v>287</v>
       </c>
       <c r="C26" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -23408,7 +23408,7 @@
         <v>288</v>
       </c>
       <c r="C27" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -23419,7 +23419,7 @@
         <v>289</v>
       </c>
       <c r="C28" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -23430,7 +23430,7 @@
         <v>290</v>
       </c>
       <c r="C29" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -23441,7 +23441,7 @@
         <v>291</v>
       </c>
       <c r="C30" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -23452,7 +23452,7 @@
         <v>292</v>
       </c>
       <c r="C31" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -23463,7 +23463,7 @@
         <v>293</v>
       </c>
       <c r="C32" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -23474,7 +23474,7 @@
         <v>294</v>
       </c>
       <c r="C33" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -23485,7 +23485,7 @@
         <v>295</v>
       </c>
       <c r="C34" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -23496,7 +23496,7 @@
         <v>296</v>
       </c>
       <c r="C35" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -23507,7 +23507,7 @@
         <v>297</v>
       </c>
       <c r="C36" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -23518,7 +23518,7 @@
         <v>288</v>
       </c>
       <c r="C37" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -23529,7 +23529,7 @@
         <v>299</v>
       </c>
       <c r="C38" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -23540,7 +23540,7 @@
         <v>300</v>
       </c>
       <c r="C39" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -23551,7 +23551,7 @@
         <v>301</v>
       </c>
       <c r="C40" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -24026,10 +24026,10 @@
         <v>339</v>
       </c>
       <c r="C2" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="D2" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -24040,10 +24040,10 @@
         <v>340</v>
       </c>
       <c r="C3" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="D3" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -24054,10 +24054,10 @@
         <v>341</v>
       </c>
       <c r="C4" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="D4" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -24068,10 +24068,10 @@
         <v>342</v>
       </c>
       <c r="C5" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="D5" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -24082,10 +24082,10 @@
         <v>343</v>
       </c>
       <c r="C6" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="D6" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -24096,10 +24096,10 @@
         <v>344</v>
       </c>
       <c r="C7" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="D7" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -24110,10 +24110,10 @@
         <v>345</v>
       </c>
       <c r="C8" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="D8" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -24124,10 +24124,10 @@
         <v>346</v>
       </c>
       <c r="C9" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="D9" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -24141,7 +24141,7 @@
         <v>1474</v>
       </c>
       <c r="D10" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -24155,7 +24155,7 @@
         <v>1474</v>
       </c>
       <c r="D11" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -24169,7 +24169,7 @@
         <v>1474</v>
       </c>
       <c r="D12" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -24183,7 +24183,7 @@
         <v>1474</v>
       </c>
       <c r="D13" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -24197,7 +24197,7 @@
         <v>1474</v>
       </c>
       <c r="D14" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -24211,7 +24211,7 @@
         <v>1474</v>
       </c>
       <c r="D15" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -24225,7 +24225,7 @@
         <v>1475</v>
       </c>
       <c r="D16" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -24239,7 +24239,7 @@
         <v>1475</v>
       </c>
       <c r="D17" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -24253,7 +24253,7 @@
         <v>1475</v>
       </c>
       <c r="D18" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -24267,7 +24267,7 @@
         <v>1475</v>
       </c>
       <c r="D19" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -24281,7 +24281,7 @@
         <v>1475</v>
       </c>
       <c r="D20" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -24295,7 +24295,7 @@
         <v>1475</v>
       </c>
       <c r="D21" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -24309,7 +24309,7 @@
         <v>1475</v>
       </c>
       <c r="D22" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -24323,7 +24323,7 @@
         <v>1475</v>
       </c>
       <c r="D23" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -24337,7 +24337,7 @@
         <v>1476</v>
       </c>
       <c r="D24" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -24351,7 +24351,7 @@
         <v>1476</v>
       </c>
       <c r="D25" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -24365,7 +24365,7 @@
         <v>1476</v>
       </c>
       <c r="D26" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -24379,7 +24379,7 @@
         <v>1476</v>
       </c>
       <c r="D27" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -24393,7 +24393,7 @@
         <v>1476</v>
       </c>
       <c r="D28" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -24407,7 +24407,7 @@
         <v>1476</v>
       </c>
       <c r="D29" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -24421,7 +24421,7 @@
         <v>1476</v>
       </c>
       <c r="D30" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -24435,7 +24435,7 @@
         <v>1476</v>
       </c>
       <c r="D31" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -24449,7 +24449,7 @@
         <v>1477</v>
       </c>
       <c r="D32" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -24463,7 +24463,7 @@
         <v>1478</v>
       </c>
       <c r="D33" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -24477,7 +24477,7 @@
         <v>1478</v>
       </c>
       <c r="D34" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -24491,7 +24491,7 @@
         <v>1479</v>
       </c>
       <c r="D35" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -24505,7 +24505,7 @@
         <v>1479</v>
       </c>
       <c r="D36" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
   </sheetData>
@@ -25498,10 +25498,10 @@
         <v>861</v>
       </c>
       <c r="B11" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="C11" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="D11" t="s">
         <v>1480</v>
@@ -25512,10 +25512,10 @@
         <v>861</v>
       </c>
       <c r="B12" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="C12" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="D12" t="s">
         <v>1480</v>
@@ -25526,10 +25526,10 @@
         <v>861</v>
       </c>
       <c r="B13" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="C13" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="D13" t="s">
         <v>1480</v>
@@ -25540,10 +25540,10 @@
         <v>861</v>
       </c>
       <c r="B14" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="C14" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="D14" t="s">
         <v>1480</v>
@@ -25554,10 +25554,10 @@
         <v>861</v>
       </c>
       <c r="B15" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="C15" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="D15" t="s">
         <v>1480</v>
@@ -25568,10 +25568,10 @@
         <v>861</v>
       </c>
       <c r="B16" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="C16" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="D16" t="s">
         <v>1480</v>
@@ -25582,10 +25582,10 @@
         <v>861</v>
       </c>
       <c r="B17" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="C17" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="D17" t="s">
         <v>1480</v>
@@ -25596,10 +25596,10 @@
         <v>861</v>
       </c>
       <c r="B18" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="C18" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="D18" t="s">
         <v>1480</v>
@@ -25610,10 +25610,10 @@
         <v>861</v>
       </c>
       <c r="B19" t="s">
+        <v>1802</v>
+      </c>
+      <c r="C19" t="s">
         <v>1803</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1804</v>
       </c>
       <c r="D19" t="s">
         <v>1480</v>
@@ -25624,10 +25624,10 @@
         <v>861</v>
       </c>
       <c r="B20" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="C20" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="D20" t="s">
         <v>1480</v>
@@ -25638,10 +25638,10 @@
         <v>861</v>
       </c>
       <c r="B21" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="C21" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="D21" t="s">
         <v>1480</v>
@@ -25652,10 +25652,10 @@
         <v>861</v>
       </c>
       <c r="B22" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="C22" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="D22" t="s">
         <v>1480</v>
@@ -25666,10 +25666,10 @@
         <v>861</v>
       </c>
       <c r="B23" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="C23" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="D23" t="s">
         <v>1480</v>
@@ -25680,10 +25680,10 @@
         <v>861</v>
       </c>
       <c r="B24" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="C24" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="D24" t="s">
         <v>1480</v>
@@ -25694,10 +25694,10 @@
         <v>861</v>
       </c>
       <c r="B25" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="C25" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="D25" t="s">
         <v>1480</v>
@@ -25708,10 +25708,10 @@
         <v>861</v>
       </c>
       <c r="B26" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="C26" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="D26" t="s">
         <v>1480</v>
@@ -25851,7 +25851,7 @@
         <v>447</v>
       </c>
       <c r="C36" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="D36" t="s">
         <v>1480</v>
@@ -25865,7 +25865,7 @@
         <v>451</v>
       </c>
       <c r="C37" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="D37" t="s">
         <v>1480</v>
@@ -25879,7 +25879,7 @@
         <v>451</v>
       </c>
       <c r="C38" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="D38" t="s">
         <v>1480</v>
@@ -25893,7 +25893,7 @@
         <v>454</v>
       </c>
       <c r="C39" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="D39" t="s">
         <v>1480</v>
@@ -25907,7 +25907,7 @@
         <v>457</v>
       </c>
       <c r="C40" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="D40" t="s">
         <v>1480</v>
@@ -25921,7 +25921,7 @@
         <v>460</v>
       </c>
       <c r="C41" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="D41" t="s">
         <v>1480</v>
@@ -25935,7 +25935,7 @@
         <v>463</v>
       </c>
       <c r="C42" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="D42" t="s">
         <v>1480</v>
@@ -25949,7 +25949,7 @@
         <v>466</v>
       </c>
       <c r="C43" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="D43" t="s">
         <v>1480</v>
@@ -25963,7 +25963,7 @@
         <v>469</v>
       </c>
       <c r="C44" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="D44" t="s">
         <v>1480</v>

</xml_diff>

<commit_message>
Fix problem with the introduction dataset.
</commit_message>
<xml_diff>
--- a/testing_excel.xlsx
+++ b/testing_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pumukl\Documents\GitHub\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9249DB9B-FDB9-4947-8F31-47AACD7FA8B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D232CDE-74D4-42B2-ACB5-2924BA196980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="769" firstSheet="7" activeTab="14" xr2:uid="{3104A2F9-7A17-4E5B-B5FF-CB166158170B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="769" firstSheet="14" activeTab="25" xr2:uid="{3104A2F9-7A17-4E5B-B5FF-CB166158170B}"/>
   </bookViews>
   <sheets>
     <sheet name="Greeting_Goodbyes" sheetId="2" r:id="rId1"/>
@@ -5302,242 +5302,242 @@
     <t>The Eye of Talos was a fine ship, once. Now it lies wrecked, off an island just north of here.</t>
   </si>
   <si>
-    <t>In &lt;TITLE&gt;The Last of Us&lt;TITLE&gt;, the introductory monologue is delivered by a news reporter who grimly details the escalating crisis. This sets the stage for the game's post-apocalyptic narrative, where society collapses due to a devastating fungal outbreak. Players follow Joel, a hardened survivor, and Ellie, a young girl who might hold the key to humanity's survival, as they navigate a world filled with infected mutants and hostile human factions. The Fireflies, a revolutionary militia group, seek to restore government control, adding to the chaos and conflict that define the game's intense and emotional journey.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;The Witcher 3: Wild Hunt&lt;TITLE&gt;, the introductory monologue is delivered by a foreboding narrator who addresses the chaos and despair gripping the land. This sets the stage for the game's dark fantasy narrative, where players follow Geralt of Rivia, a monster hunter known as a Witcher, on a quest to find his adopted daughter Ciri, who is being pursued by the otherworldly Wild Hunt. The game is set in a war-torn world filled with political intrigue, dangerous creatures, and morally complex choices. As Geralt, players must navigate through the turmoil, battling both human and monstrous foes, while making decisions that shape the fate of the world and its inhabitants.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Elden Ring&lt;TITLE&gt;, the introductory monologue delivered by a narrator sets the stage for the game's epic dark fantasy narrative. The player takes on the role of a Tarnished, one of the dead who yet live, called back to the Lands Between to restore the fractured world. The once-great Elden Ring has been shattered, and Queen Marika the Eternal has disappeared. On the Night of the Black Knives, the demigod Godwin the Golden was the first to fall, leading Marika's demigod offspring to seize the shards of the Elden Ring. Their newfound power triggered the Shattering, a catastrophic war that left the Lands Between in chaos and abandoned by the Greater Will. The Tarnished, including chieftains, sorcerers, and other notable figures, are beckoned by the call of long-lost grace to reclaim their destiny. As a Tarnished of no renown, the player must cross the fog to the Lands Between, face formidable foes, and seek to reunite the Elden Ring, ultimately striving to become the Elden Lord. The game explores themes of power, legacy, and redemption in a richly detailed and mysterious world.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Fallout 3&lt;TITLE&gt;, the introductory monologue is delivered by the narrator, setting a grim tone for the game. This monologue introduces players to a post-apocalyptic world devastated by nuclear war in 2077. Players assume the role of a character born and raised in Vault 101, one of the many underground shelters designed to protect humanity from the horrors of nuclear fallout. The vault's motto, &lt;TITLE&gt;no one ever enters, and no one ever leaves&lt;TITLE&gt;, shapes the protagonist's early life until circumstances force them to venture into the harsh and desolate wasteland of the Capital Wasteland. As they search for their missing father, players must navigate through a world filled with radiation, mutated creatures, and hostile factions, all while uncovering the secrets of their family's past and the broader mysteries of the post-apocalyptic society.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Fallout 4&lt;TITLE&gt;, the introductory monologue is delivered by the protagonist, setting the stage for the game's post-apocalyptic narrative. The game begins in 2077, just before a nuclear war devastates the world. Players take on the role of a character who survives the apocalypse by taking refuge in Vault 111. Emerging 200 years later, the protagonist finds a drastically changed world and embarks on a quest to find their kidnapped son. The journey takes them through the Commonwealth, a region filled with mutated creatures, hostile factions, and the remnants of pre-war society, as they uncover the truth about their past and influence the future of the wasteland.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Fallout: New Vegas&lt;TITLE&gt;, the introductory monologue is delivered by the narrator and sets the stage for the game's post-apocalyptic narrative. Players assume the role of a courier in the Mojave Desert, an area where the New California Republic and Caesar's Legion vie for control of the Hoover Dam. The city of New Vegas remains untouched by nuclear war, under the control of Mr. House and his robotic army. As the courier, players begin their journey after surviving an ambush intended to prevent the delivery of a mysterious package. The protagonist's quest for revenge and discovery leads them through a world filled with factions, conflicts, and the remnants of pre-war society, ultimately influencing the fate of New Vegas and its inhabitants.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Borderlands&lt;TITLE&gt;, the introductory monologue, delivered by the character Marcus Kincaid, sets the stage for the game's adventure-filled narrative. Players take on the role of Vault Hunters on the planet Pandora, a lawless and dangerous world rumored to hold the legendary Vault, filled with advanced alien technology and unimaginable riches. Guided by a mysterious Guardian Angel, the Vault Hunters embark on a quest to find this mythical treasure. The journey is filled with peril, bizarre creatures, and treacherous bandits, as they uncover the secrets of Pandora and strive to claim the legendary Vault's bounty.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Borderlands 2&lt;TITLE&gt;, the introductory monologue is delivered by the charismatic and humorous narrator, Marcus Kincaid. This monologue sets the stage for the game's high-stakes narrative. Players assume the role of new Vault Hunters on Pandora, a planet now infused with the rare and valuable mineral Eridium, which emerged after the first Vault's opening. The Hyperion Corporation, led by the ruthless Handsome Jack, seeks to exploit this resource and bring order to Pandora by uncovering an even greater Vault. Drawn by the promise of danger and loot, the Vault Hunters embark on a quest to stop Handsome Jack, uncover Pandora's hidden secrets, and ultimately save the planet from his tyrannical grip. The journey is filled with intense battles, quirky characters, and a struggle against the corporate oppression of Hyperion.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Borderlands 3&lt;TITLE&gt;, the introductory monologue is delivered by Marcus Kincaid, setting the stage for the game's thrilling adventure. Players take on the role of new Vault Hunters on the planet Pandora, a land known for its greed and violence but also its opportunities. Guided by tales of hidden alien treasures, these Vault Hunters embark on a journey answering the call of Lilith, a legendary Siren and hero of Pandora. She is assembling a team to hunt for a man leading to Vaults across the galaxy. However, dark forces have emerged, posing unprecedented threats to the Borderlands. The adventure begins with these bold and hungry Vault Hunters, embarking on a quest filled with danger, treasure, and the enduring charm of Marcus's storytelling.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Helldivers 2&lt;TITLE&gt;, the introductory monologue delivered by a recruitment officer sets the stage for the game's action-packed narrative. The player takes on the role of a new recruit in the Helldivers, an elite peacekeeping force dedicated to protecting Super Earth and spreading its values of democracy and freedom across the galaxy. Facing constant threats from hostile alien species such as the Bugs, Cyborgs, and Illuminates, the Helldivers engage in cooperative missions on various planets, battling to defend strategic locations and uphold their way of life. The game focuses on themes of duty, sacrifice, and the relentless fight for freedom, as players work together to complete challenging missions, combat diverse and dangerous enemies, and ensure the survival and expansion of Super Earth's ideals in an ever-dangerous universe.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;God of War III&lt;TITLE&gt;, the introductory monologue is delivered by Gaia, the Titaness of Earth, setting the stage for the epic conclusion of Kratos's journey. The narrator recounts the rise of Kratos, who, despite becoming the new God of War, remains haunted by the tragic memories of murdering his own family. Neither death nor the Sisters of Fate could contain him. As the game begins, Kratos, driven by an unyielding desire for vengeance, embarks on a relentless quest to bring down the gods of Olympus who have wronged him. This climactic chapter sees Kratos confronting powerful deities and mythical creatures, fueled by his rage and determination to seek justice for the torment he has endured.</t>
+    <t>the Guard speaking is a Stormcloak Guard</t>
+  </si>
+  <si>
+    <t>the Guard speaking is a Imperial Guard</t>
+  </si>
+  <si>
+    <t>the Guard speaking is an Imperial Guard</t>
+  </si>
+  <si>
+    <t>the Guard is in the Windhelm region</t>
+  </si>
+  <si>
+    <t>the Player is a member of Thieves Guild</t>
+  </si>
+  <si>
+    <t>Guard reacting to the Player's weapon</t>
+  </si>
+  <si>
+    <t>Guard reacting to the Player's artifacts and unique items</t>
+  </si>
+  <si>
+    <t>a Guard reacting to the Player's race</t>
+  </si>
+  <si>
+    <t>a Guard reacting to the Player's high skill level in Alchemy</t>
+  </si>
+  <si>
+    <t>a Guard reacting to the Player's high skill level in Conjuration</t>
+  </si>
+  <si>
+    <t>a Guard reacting to the Player's high skill level in Destruction</t>
+  </si>
+  <si>
+    <t>a Guard reacting to the Player's high skill level in Enchanting</t>
+  </si>
+  <si>
+    <t>a Guard reacting to the Player's high skill level in the use of heavy armor</t>
+  </si>
+  <si>
+    <t>a Guard reacting to the Player's high skill level in Illusions</t>
+  </si>
+  <si>
+    <t>a Guard reacting to the Player's high skill level in the use of light armor</t>
+  </si>
+  <si>
+    <t>a Guard reacting to the Player's high skill level in Lockpicking</t>
+  </si>
+  <si>
+    <t>a Guard reacting to the Player's high skill level in the use of one-handed weapons</t>
+  </si>
+  <si>
+    <t>a Guard reacting to the Player's high skill level in Pickpocketing</t>
+  </si>
+  <si>
+    <t>a Guard reacting to the Player's high skill level in Restoration</t>
+  </si>
+  <si>
+    <t>a Guard reacting to the Player's high skill level in Sneaking</t>
+  </si>
+  <si>
+    <t>a Guard reacting to the Player's high skill level in the use of Speech</t>
+  </si>
+  <si>
+    <t>a Guard reacting to the Player's high skill level in the use of Two-Handed weapons</t>
+  </si>
+  <si>
+    <t>the Player has not purchased Breezehome</t>
+  </si>
+  <si>
+    <t>the Player has purchased Breezehome</t>
+  </si>
+  <si>
+    <t>the Player has a desease</t>
+  </si>
+  <si>
+    <t>the Player has not purchased  Hjerim</t>
+  </si>
+  <si>
+    <t>the Player has purchased Hjerim</t>
+  </si>
+  <si>
+    <t>an NPC witnessing a theft</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;The Last of Us&lt;/TITLE&gt;, the introductory monologue is delivered by a news reporter who grimly details the escalating crisis. This sets the stage for the game's post-apocalyptic narrative, where society collapses due to a devastating fungal outbreak. Players follow Joel, a hardened survivor, and Ellie, a young girl who might hold the key to humanity's survival, as they navigate a world filled with infected mutants and hostile human factions. The Fireflies, a revolutionary militia group, seek to restore government control, adding to the chaos and conflict that define the game's intense and emotional journey.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;The Witcher 3: Wild Hunt&lt;/TITLE&gt;, the introductory monologue is delivered by a foreboding narrator who addresses the chaos and despair gripping the land. This sets the stage for the game's dark fantasy narrative, where players follow Geralt of Rivia, a monster hunter known as a Witcher, on a quest to find his adopted daughter Ciri, who is being pursued by the otherworldly Wild Hunt. The game is set in a war-torn world filled with political intrigue, dangerous creatures, and morally complex choices. As Geralt, players must navigate through the turmoil, battling both human and monstrous foes, while making decisions that shape the fate of the world and its inhabitants.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Elden Ring&lt;/TITLE&gt;, the introductory monologue delivered by a narrator sets the stage for the game's epic dark fantasy narrative. The player takes on the role of a Tarnished, one of the dead who yet live, called back to the Lands Between to restore the fractured world. The once-great Elden Ring has been shattered, and Queen Marika the Eternal has disappeared. On the Night of the Black Knives, the demigod Godwin the Golden was the first to fall, leading Marika's demigod offspring to seize the shards of the Elden Ring. Their newfound power triggered the Shattering, a catastrophic war that left the Lands Between in chaos and abandoned by the Greater Will. The Tarnished, including chieftains, sorcerers, and other notable figures, are beckoned by the call of long-lost grace to reclaim their destiny. As a Tarnished of no renown, the player must cross the fog to the Lands Between, face formidable foes, and seek to reunite the Elden Ring, ultimately striving to become the Elden Lord. The game explores themes of power, legacy, and redemption in a richly detailed and mysterious world.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Fallout 3&lt;/TITLE&gt;, the introductory monologue is delivered by the narrator, setting a grim tone for the game. This monologue introduces players to a post-apocalyptic world devastated by nuclear war in 2077. Players assume the role of a character born and raised in Vault 101, one of the many underground shelters designed to protect humanity from the horrors of nuclear fallout. The vault's motto, &lt;TITLE&gt;no one ever enters, and no one ever leaves&lt;TITLE&gt;, shapes the protagonist's early life until circumstances force them to venture into the harsh and desolate wasteland of the Capital Wasteland. As they search for their missing father, players must navigate through a world filled with radiation, mutated creatures, and hostile factions, all while uncovering the secrets of their family's past and the broader mysteries of the post-apocalyptic society.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Fallout 4&lt;/TITLE&gt;, the introductory monologue is delivered by the protagonist, setting the stage for the game's post-apocalyptic narrative. The game begins in 2077, just before a nuclear war devastates the world. Players take on the role of a character who survives the apocalypse by taking refuge in Vault 111. Emerging 200 years later, the protagonist finds a drastically changed world and embarks on a quest to find their kidnapped son. The journey takes them through the Commonwealth, a region filled with mutated creatures, hostile factions, and the remnants of pre-war society, as they uncover the truth about their past and influence the future of the wasteland.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Fallout: New Vegas&lt;/TITLE&gt;, the introductory monologue is delivered by the narrator and sets the stage for the game's post-apocalyptic narrative. Players assume the role of a courier in the Mojave Desert, an area where the New California Republic and Caesar's Legion vie for control of the Hoover Dam. The city of New Vegas remains untouched by nuclear war, under the control of Mr. House and his robotic army. As the courier, players begin their journey after surviving an ambush intended to prevent the delivery of a mysterious package. The protagonist's quest for revenge and discovery leads them through a world filled with factions, conflicts, and the remnants of pre-war society, ultimately influencing the fate of New Vegas and its inhabitants.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Borderlands&lt;/TITLE&gt;, the introductory monologue, delivered by the character Marcus Kincaid, sets the stage for the game's adventure-filled narrative. Players take on the role of Vault Hunters on the planet Pandora, a lawless and dangerous world rumored to hold the legendary Vault, filled with advanced alien technology and unimaginable riches. Guided by a mysterious Guardian Angel, the Vault Hunters embark on a quest to find this mythical treasure. The journey is filled with peril, bizarre creatures, and treacherous bandits, as they uncover the secrets of Pandora and strive to claim the legendary Vault's bounty.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Borderlands 2&lt;/TITLE&gt;, the introductory monologue is delivered by the charismatic and humorous narrator, Marcus Kincaid. This monologue sets the stage for the game's high-stakes narrative. Players assume the role of new Vault Hunters on Pandora, a planet now infused with the rare and valuable mineral Eridium, which emerged after the first Vault's opening. The Hyperion Corporation, led by the ruthless Handsome Jack, seeks to exploit this resource and bring order to Pandora by uncovering an even greater Vault. Drawn by the promise of danger and loot, the Vault Hunters embark on a quest to stop Handsome Jack, uncover Pandora's hidden secrets, and ultimately save the planet from his tyrannical grip. The journey is filled with intense battles, quirky characters, and a struggle against the corporate oppression of Hyperion.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Borderlands 3&lt;/TITLE&gt;, the introductory monologue is delivered by Marcus Kincaid, setting the stage for the game's thrilling adventure. Players take on the role of new Vault Hunters on the planet Pandora, a land known for its greed and violence but also its opportunities. Guided by tales of hidden alien treasures, these Vault Hunters embark on a journey answering the call of Lilith, a legendary Siren and hero of Pandora. She is assembling a team to hunt for a man leading to Vaults across the galaxy. However, dark forces have emerged, posing unprecedented threats to the Borderlands. The adventure begins with these bold and hungry Vault Hunters, embarking on a quest filled with danger, treasure, and the enduring charm of Marcus's storytelling.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Helldivers 2&lt;/TITLE&gt;, the introductory monologue delivered by a recruitment officer sets the stage for the game's action-packed narrative. The player takes on the role of a new recruit in the Helldivers, an elite peacekeeping force dedicated to protecting Super Earth and spreading its values of democracy and freedom across the galaxy. Facing constant threats from hostile alien species such as the Bugs, Cyborgs, and Illuminates, the Helldivers engage in cooperative missions on various planets, battling to defend strategic locations and uphold their way of life. The game focuses on themes of duty, sacrifice, and the relentless fight for freedom, as players work together to complete challenging missions, combat diverse and dangerous enemies, and ensure the survival and expansion of Super Earth's ideals in an ever-dangerous universe.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;God of War III&lt;/TITLE&gt;, the introductory monologue is delivered by Gaia, the Titaness of Earth, setting the stage for the epic conclusion of Kratos's journey. The narrator recounts the rise of Kratos, who, despite becoming the new God of War, remains haunted by the tragic memories of murdering his own family. Neither death nor the Sisters of Fate could contain him. As the game begins, Kratos, driven by an unyielding desire for vengeance, embarks on a relentless quest to bring down the gods of Olympus who have wronged him. This climactic chapter sees Kratos confronting powerful deities and mythical creatures, fueled by his rage and determination to seek justice for the torment he has endured.</t>
   </si>
   <si>
     <t xml:space="preserve">
-In &lt;TITLE&gt;Dying Light 2&lt;TITLE&gt;, the introductory monologue delivered by a narrator sets the stage for the game's post-apocalyptic narrative. The player takes on the role of Aiden Caldwell, a pilgrim who traverses dangerous wastelands to connect isolated human settlements. Civilization has collapsed due to a new variant of the Hurran virus, which spread rapidly after escaping from secret military research labs. Now, the remnants of humanity live in small enclaves, with one last city standing as a bastion of hope. This city is isolated, governed by unique rules, and represents humanity's final chance to learn from past mistakes. The game explores themes of survival, choice, and consequence, as every decision Aiden makes shapes the future of this fragile society. The player must navigate the city, forge alliances, and face threats both human and infected to determine the fate of humanity.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Assassin's Creed: Revelations&lt;TITLE&gt;, the introductory monologue is delivered by Ezio Auditore in a letter to his sister, Claudia, setting the stage for his journey. Ezio has arrived in Masyaf, seeking a hidden library mentioned by their father. This library, located beneath Masyaf Castle, is believed to contain invaluable wisdom and secrets left by the legendary Assassin, Altair. Players take on the role of Ezio, now a seasoned Master Assassin, as he navigates the perilous journey to uncover the hidden knowledge. The road to Masyaf is fraught with mercenaries and bandits, making the mission dangerous and uncertain. As Ezio, players must use their skills and cunning to overcome these threats, unravel the mysteries of the past, and gain insight into the true purpose of the Assassin Brotherhood. The game delves into Ezio's introspective quest for clarity and understanding, while also connecting his fate with that of Altair and Desmond Miles, bridging the gaps between different eras of the Assassin's Creed saga.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Assassin's Creed: Mirage&lt;TITLE&gt;, the introductory monologue is delivered by a narrator reflecting on the memory of a pivotal figure. This sets the stage for the game's narrative, focusing on a man who rose from being a common thief on the streets of Baghdad to a significant member of the Hidden Ones, the predecessors of the Assassin Brotherhood. Players take on the role of this man, navigating the bustling and dangerous streets of Baghdad during the height of the Abbasid Caliphate. Despite the city's golden age, a sinister rot lies beneath, with the Order of the Ancients spreading their influence and cruelty. As a member of the Hidden Ones, the protagonist engages in a shadowy struggle against these oppressive forces. The journey is not just one of external conflict but also of personal growth and understanding. The protagonist's story is a testament to honoring the Creed, challenging it, and recognizing the thin line between the shadows they walk and the light they serve. Players must navigate this complex world, making choices that reflect the eternal struggle between freedom and oppression, light and darkness.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Assassin's Creed III&lt;TITLE&gt;, the introductory monologue is delivered by William Miles, setting the stage for the game's narrative. He reflects on the end of the world, a concept once dismissed but now frighteningly real. The story begins with the abduction of Desmond Miles, his son, who possesses a denied heritage. Desmond was captured by Abstergo Industries, known to the Assassins as the Templars, who sought his help to find the Apple of Eden, a powerful artifact. Players take on the role of Desmond Miles, using the Animus to explore the lives of his ancestors and uncover hidden truths about the Assassins and Templars. As Desmond, players must gain the knowledge and skills of his ancestors, Altair and Ezio, to prevent an impending apocalypse foretold to occur on December 21, 2012. The journey involves mastering combat and stealth, solving complex puzzles, and making strategic decisions that impact the course of history. Armed with the Apple of Eden and supported by his fellow Assassins, Desmond stands at the brink of the final confrontation, ready to use his newfound abilities to save humanity from disaster.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Dark Souls III&lt;TITLE&gt;, the introductory monologue is delivered by an unseen narrator, setting the stage for the game's dark and foreboding narrative. It begins with a description of Lothric, a land where the transitory realms of the Lords of Cinder converge. As the fire fades and the lords forsake their thrones, a bell tolls, awakening the old Lords of Cinder from their graves: Aldrich, Saint of the Deep; Farron's Undead Legion, the Abyss Watchers; and Yhorm the Giant, the reclusive lord of the Profaned Capital. However, the Lords abandon their thrones, leaving the Unkindled to rise. Players assume the role of an Unkindled, a nameless and accursed undead, unfit even to be cinder. Their journey involves seeking embers, confronting the revived Lords of Cinder, and ultimately rekindling the First Flame to prevent the world from falling into darkness. The player's role is to navigate this treacherous world, mastering its challenging combat, uncovering its hidden lore, and making decisions that shape the fate of Lothric and its inhabitants.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Dark Souls II&lt;TITLE&gt;, the introductory monologue is delivered by an unseen narrator, setting the stage for the game's dark and mysterious narrative. The story begins by introducing a murky, forgotten land where souls can mend an ailing mind. Players are warned that they will lose everything once branded with the symbol of the curse, becoming something other than human—a Hollow. The narrative speaks of a walled-off land far to the north where a great king built the kingdom of Drangleic. As players, you assume the role of a cursed individual drawn to Drangleic without fully understanding why, like a moth to a flame. Your journey will be one of relentless anguish, facing challenges and uncovering the deep lore of this decrepit kingdom. The player's role involves navigating the perilous world of Drangleic, mastering its brutal combat, and seeking to lift the curse that plagues them, all while unraveling the secrets of this enigmatic land.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Dark Souls&lt;TITLE&gt;, the introductory monologue is delivered by an unseen narrator, setting the stage for the game's dark and mythic narrative. The story begins in the Age of Ancients, a time when the world was unformed and shrouded by fog, populated by gray crags, Archtrees, and Everlasting Dragons. Then, Fire emerged, bringing disparity—heat and cold, life and death, light and dark. From the dark, powerful beings found the Souls of Lords within the flame. With their newfound strength, they challenged the Dragons, leading to the Age of Fire. However, the flames are fading, and darkness threatens to take over. Now, only embers remain, and humanity is left in endless night. Among the living are those branded with the accursed Darksign. Players assume the role of an Undead, branded by the Darksign and corralled to the north, where they are locked away to await the end of the world. This is your fate. As the Undead, you must navigate a perilous world, uncover its deep lore, and seek to rekindle the fading flames, battling formidable foes and overcoming tremendous challenges along the way.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;The Elder Scrolls IV: Oblivion&lt;TITLE&gt;, the introductory monologue is delivered by Emperor Uriel Septim VII, who reflects on his long reign and impending doom. This sets the stage for the game's epic fantasy narrative, where players take on the role of an anonymous prisoner destined to thwart a dire prophecy. As gates to the demonic realm of Oblivion open and dark forces threaten to engulf the land of Tamriel, players must navigate a richly detailed world, undertake quests, and battle fearsome enemies. The story unfolds with the player seeking to find and protect the lost heir to the throne, ultimately striving to seal the gates of Oblivion and save the Empire from destruction.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;The Elder Scrolls Online&lt;TITLE&gt;, the introductory monologue is delivered by a narrator who sets the ominous tone of impending conflict and ancient evil. This sets the stage for the game's expansive MMORPG narrative, where players enter the world of Tamriel during a time of great turmoil and war. The year is 582 of the Second Era, and various factions vie for control of the Imperial City and the Ruby Throne. Players can choose from a variety of races and classes, embarking on epic quests, exploring vast regions, and battling both monsters and rival factions. As they uncover hidden dangers and dark schemes, players must navigate alliances and conflicts, shaping the fate of Tamriel in an ever-evolving world filled with adventure and danger.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Fallout 2&lt;TITLE&gt;, the introductory monologue is delivered by a narrator who reflects on the unchanging nature of war and the catastrophic events that led to the world's near-destruction. This sets the stage for the game's post-apocalyptic narrative, where players take on the role of the Chosen One, a descendant of the legendary Vault Dweller. Emerging from the tribal village of Arroyo, the player embarks on a perilous journey to save their home from ecological disaster. The story unfolds in a vast, irradiated wasteland filled with mutated creatures, ruthless factions, and remnants of pre-war technology. As the Chosen One, players must navigate this dangerous world, making crucial decisions that will determine the fate of their tribe and the future of humanity.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Metal Gear Solid V: The Phantom Pain&lt;TITLE&gt;, the introductory monologue is delivered by a narrator who describes the evolution of modern warfare into an automated and controlled system. This sets the stage for the game's complex narrative, where players follow the story of Big Boss, also known as Venom Snake, as he builds a new private army to take revenge on the shadowy organization Cipher. The game is set in an open world, where players undertake missions across various global conflict zones, employing stealth, strategy, and combat skills. The narrative delves into themes of revenge, loyalty, and the impact of war, all while exploring the technological advancements that have transformed the battlefield into a highly regulated and monitored environment. As Venom Snake, players must navigate this dangerous world, building and managing their own mercenary army, the Diamond Dogs. They engage in tactical espionage operations, gather resources, recruit soldiers, and develop new weapons and technology.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Alan Wake&lt;TITLE&gt;, the introductory monologue is delivered by the titular character, Alan Wake, a writer grappling with unsettling nightmares and a vivid imagination. This sets the stage for the game's psychological thriller narrative, where players follow Alan Wake as he embarks on a quest to find his missing wife, Alice, in the mysterious town of Bright Falls. The story begins with a haunting dream sequence that sets the tone for the surreal and dark events that follow. As Alan Wake, players explore a world where the lines between reality and fiction blur, with nightmarish occurrences manifesting from Wake's own writing. The game combines elements of action and horror, as players use light to combat the shadowy entities that emerge from the darkness. Throughout the game, players uncover manuscript pages that foreshadow events, adding to the suspense and intrigue. The narrative delves into themes of fear, the power of storytelling, and the struggle between light and darkness. Players must navigate the eerie environment, solve puzzles, and confront their deepest fears to uncover the truth behind Alice's disappearance and Alan's own psychological torment. The unanswered mysteries and unsettling atmosphere make &lt;TITLE&gt;Alan Wake&lt;TITLE&gt; a memorable and gripping experience.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Alan Wake II&lt;TITLE&gt;, the introductory monologue is delivered by a narrator who sets a haunting and mysterious tone. This sets the stage for the game's psychological horror narrative, where players follow Alan Wake, a troubled writer, as he navigates a surreal and nightmarish world. Alan Wake's journey is deeply entwined with the dark lore of Cauldron Lake, a mysterious body of water with the power to blur the lines between fiction and reality. The lake's supernatural influence has a history of ensnaring creative minds, warping their creations into terrifying manifestations. As Alan delves deeper into this twisted reality, he encounters shadowy figures and malevolent forces drawn from his own writings, all while trying to reclaim his lost memories and escape the encroaching darkness. The lore-rich environment is filled with references to ancient myths, eerie folklore, and the psychological horror elements that define Alan's struggle. Throughout the game, players must uncover the truth behind the dark presence that haunts Cauldron Lake, confront their deepest fears, and piece together the fragmented narrative to ultimately survive the harrowing ordeal.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Darkest Dungeon&lt;TITLE&gt;, the introductory monologue is delivered by the Ancestor, who sets a grim and foreboding tone. This sets the stage for the game's gothic horror narrative, where players inherit a decayed estate plagued by eldritch horrors and madness. The Ancestor recounts how his insatiable curiosity and pursuit of forbidden knowledge led him to unearth a portal to an ancient, malevolent force beneath the manor. This act unleashed unspeakable evils that now corrupt the land and its inhabitants. Players take on the role of the heir, tasked with reclaiming the family estate and confronting the horrors that lurk within the Darkest Dungeon. The journey is fraught with peril, as players must assemble and lead a band of flawed heroes through nightmarish dungeons, battling terrifying creatures and coping with the ever-present threat of insanity. The game's rich lore is steeped in themes of decay, corruption, and the psychological toll of facing one's deepest fears. To restore the family’s honor, players must delve into the depths of the manor, uncover its dark secrets, and ultimately confront the ancient evil that has taken root in their ancestral home.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In &lt;TITLE&gt;NieR: Automata&lt;TITLE&gt;, the introductory monologue delivered by the protagonist, 2B, sets the stage for the game's profound and philosophical narrative. The player takes on the role of 2B, an android soldier in the YoRHa unit, tasked with fighting a proxy war on Earth between human-made androids and alien-created machines. The remnants of humanity have fled to the Moon, leaving Earth as a battleground. As 2B, alongside her companion 9S, the player uncovers hidden truths about the war, their enemies, and themselves. The game explores themes of existentialism, the nature of life and death, and the search for meaning in a seemingly endless cycle of conflict. Through intense combat and emotional storytelling, the player's choices and actions reveal the complex layers of this post-apocalyptic world, challenging their perceptions of purpose and identity.
+In &lt;TITLE&gt;Dying Light 2&lt;/TITLE&gt;, the introductory monologue delivered by a narrator sets the stage for the game's post-apocalyptic narrative. The player takes on the role of Aiden Caldwell, a pilgrim who traverses dangerous wastelands to connect isolated human settlements. Civilization has collapsed due to a new variant of the Hurran virus, which spread rapidly after escaping from secret military research labs. Now, the remnants of humanity live in small enclaves, with one last city standing as a bastion of hope. This city is isolated, governed by unique rules, and represents humanity's final chance to learn from past mistakes. The game explores themes of survival, choice, and consequence, as every decision Aiden makes shapes the future of this fragile society. The player must navigate the city, forge alliances, and face threats both human and infected to determine the fate of humanity.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Assassin's Creed: Revelations&lt;/TITLE&gt;, the introductory monologue is delivered by Ezio Auditore in a letter to his sister, Claudia, setting the stage for his journey. Ezio has arrived in Masyaf, seeking a hidden library mentioned by their father. This library, located beneath Masyaf Castle, is believed to contain invaluable wisdom and secrets left by the legendary Assassin, Altair. Players take on the role of Ezio, now a seasoned Master Assassin, as he navigates the perilous journey to uncover the hidden knowledge. The road to Masyaf is fraught with mercenaries and bandits, making the mission dangerous and uncertain. As Ezio, players must use their skills and cunning to overcome these threats, unravel the mysteries of the past, and gain insight into the true purpose of the Assassin Brotherhood. The game delves into Ezio's introspective quest for clarity and understanding, while also connecting his fate with that of Altair and Desmond Miles, bridging the gaps between different eras of the Assassin's Creed saga.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Assassin's Creed: Mirage&lt;/TITLE&gt;, the introductory monologue is delivered by a narrator reflecting on the memory of a pivotal figure. This sets the stage for the game's narrative, focusing on a man who rose from being a common thief on the streets of Baghdad to a significant member of the Hidden Ones, the predecessors of the Assassin Brotherhood. Players take on the role of this man, navigating the bustling and dangerous streets of Baghdad during the height of the Abbasid Caliphate. Despite the city's golden age, a sinister rot lies beneath, with the Order of the Ancients spreading their influence and cruelty. As a member of the Hidden Ones, the protagonist engages in a shadowy struggle against these oppressive forces. The journey is not just one of external conflict but also of personal growth and understanding. The protagonist's story is a testament to honoring the Creed, challenging it, and recognizing the thin line between the shadows they walk and the light they serve. Players must navigate this complex world, making choices that reflect the eternal struggle between freedom and oppression, light and darkness.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Assassin's Creed III&lt;/TITLE&gt;, the introductory monologue is delivered by William Miles, setting the stage for the game's narrative. He reflects on the end of the world, a concept once dismissed but now frighteningly real. The story begins with the abduction of Desmond Miles, his son, who possesses a denied heritage. Desmond was captured by Abstergo Industries, known to the Assassins as the Templars, who sought his help to find the Apple of Eden, a powerful artifact. Players take on the role of Desmond Miles, using the Animus to explore the lives of his ancestors and uncover hidden truths about the Assassins and Templars. As Desmond, players must gain the knowledge and skills of his ancestors, Altair and Ezio, to prevent an impending apocalypse foretold to occur on December 21, 2012. The journey involves mastering combat and stealth, solving complex puzzles, and making strategic decisions that impact the course of history. Armed with the Apple of Eden and supported by his fellow Assassins, Desmond stands at the brink of the final confrontation, ready to use his newfound abilities to save humanity from disaster.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Dark Souls III&lt;/TITLE&gt;, the introductory monologue is delivered by an unseen narrator, setting the stage for the game's dark and foreboding narrative. It begins with a description of Lothric, a land where the transitory realms of the Lords of Cinder converge. As the fire fades and the lords forsake their thrones, a bell tolls, awakening the old Lords of Cinder from their graves: Aldrich, Saint of the Deep; Farron's Undead Legion, the Abyss Watchers; and Yhorm the Giant, the reclusive lord of the Profaned Capital. However, the Lords abandon their thrones, leaving the Unkindled to rise. Players assume the role of an Unkindled, a nameless and accursed undead, unfit even to be cinder. Their journey involves seeking embers, confronting the revived Lords of Cinder, and ultimately rekindling the First Flame to prevent the world from falling into darkness. The player's role is to navigate this treacherous world, mastering its challenging combat, uncovering its hidden lore, and making decisions that shape the fate of Lothric and its inhabitants.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Dark Souls II&lt;/TITLE&gt;, the introductory monologue is delivered by an unseen narrator, setting the stage for the game's dark and mysterious narrative. The story begins by introducing a murky, forgotten land where souls can mend an ailing mind. Players are warned that they will lose everything once branded with the symbol of the curse, becoming something other than human—a Hollow. The narrative speaks of a walled-off land far to the north where a great king built the kingdom of Drangleic. As players, you assume the role of a cursed individual drawn to Drangleic without fully understanding why, like a moth to a flame. Your journey will be one of relentless anguish, facing challenges and uncovering the deep lore of this decrepit kingdom. The player's role involves navigating the perilous world of Drangleic, mastering its brutal combat, and seeking to lift the curse that plagues them, all while unraveling the secrets of this enigmatic land.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Dark Souls&lt;/TITLE&gt;, the introductory monologue is delivered by an unseen narrator, setting the stage for the game's dark and mythic narrative. The story begins in the Age of Ancients, a time when the world was unformed and shrouded by fog, populated by gray crags, Archtrees, and Everlasting Dragons. Then, Fire emerged, bringing disparity—heat and cold, life and death, light and dark. From the dark, powerful beings found the Souls of Lords within the flame. With their newfound strength, they challenged the Dragons, leading to the Age of Fire. However, the flames are fading, and darkness threatens to take over. Now, only embers remain, and humanity is left in endless night. Among the living are those branded with the accursed Darksign. Players assume the role of an Undead, branded by the Darksign and corralled to the north, where they are locked away to await the end of the world. This is your fate. As the Undead, you must navigate a perilous world, uncover its deep lore, and seek to rekindle the fading flames, battling formidable foes and overcoming tremendous challenges along the way.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;The Elder Scrolls IV: Oblivion&lt;/TITLE&gt;, the introductory monologue is delivered by Emperor Uriel Septim VII, who reflects on his long reign and impending doom. This sets the stage for the game's epic fantasy narrative, where players take on the role of an anonymous prisoner destined to thwart a dire prophecy. As gates to the demonic realm of Oblivion open and dark forces threaten to engulf the land of Tamriel, players must navigate a richly detailed world, undertake quests, and battle fearsome enemies. The story unfolds with the player seeking to find and protect the lost heir to the throne, ultimately striving to seal the gates of Oblivion and save the Empire from destruction.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;The Elder Scrolls Online&lt;/TITLE&gt;, the introductory monologue is delivered by a narrator who sets the ominous tone of impending conflict and ancient evil. This sets the stage for the game's expansive MMORPG narrative, where players enter the world of Tamriel during a time of great turmoil and war. The year is 582 of the Second Era, and various factions vie for control of the Imperial City and the Ruby Throne. Players can choose from a variety of races and classes, embarking on epic quests, exploring vast regions, and battling both monsters and rival factions. As they uncover hidden dangers and dark schemes, players must navigate alliances and conflicts, shaping the fate of Tamriel in an ever-evolving world filled with adventure and danger.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Fallout 2&lt;/TITLE&gt;, the introductory monologue is delivered by a narrator who reflects on the unchanging nature of war and the catastrophic events that led to the world's near-destruction. This sets the stage for the game's post-apocalyptic narrative, where players take on the role of the Chosen One, a descendant of the legendary Vault Dweller. Emerging from the tribal village of Arroyo, the player embarks on a perilous journey to save their home from ecological disaster. The story unfolds in a vast, irradiated wasteland filled with mutated creatures, ruthless factions, and remnants of pre-war technology. As the Chosen One, players must navigate this dangerous world, making crucial decisions that will determine the fate of their tribe and the future of humanity.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Metal Gear Solid V: The Phantom Pain&lt;/TITLE&gt;, the introductory monologue is delivered by a narrator who describes the evolution of modern warfare into an automated and controlled system. This sets the stage for the game's complex narrative, where players follow the story of Big Boss, also known as Venom Snake, as he builds a new private army to take revenge on the shadowy organization Cipher. The game is set in an open world, where players undertake missions across various global conflict zones, employing stealth, strategy, and combat skills. The narrative delves into themes of revenge, loyalty, and the impact of war, all while exploring the technological advancements that have transformed the battlefield into a highly regulated and monitored environment. As Venom Snake, players must navigate this dangerous world, building and managing their own mercenary army, the Diamond Dogs. They engage in tactical espionage operations, gather resources, recruit soldiers, and develop new weapons and technology.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Alan Wake&lt;/TITLE&gt;, the introductory monologue is delivered by the titular character, Alan Wake, a writer grappling with unsettling nightmares and a vivid imagination. This sets the stage for the game's psychological thriller narrative, where players follow Alan Wake as he embarks on a quest to find his missing wife, Alice, in the mysterious town of Bright Falls. The story begins with a haunting dream sequence that sets the tone for the surreal and dark events that follow. As Alan Wake, players explore a world where the lines between reality and fiction blur, with nightmarish occurrences manifesting from Wake's own writing. The game combines elements of action and horror, as players use light to combat the shadowy entities that emerge from the darkness. Throughout the game, players uncover manuscript pages that foreshadow events, adding to the suspense and intrigue. The narrative delves into themes of fear, the power of storytelling, and the struggle between light and darkness. Players must navigate the eerie environment, solve puzzles, and confront their deepest fears to uncover the truth behind Alice's disappearance and Alan's own psychological torment. The unanswered mysteries and unsettling atmosphere make &lt;TITLE&gt;Alan Wake&lt;TITLE&gt; a memorable and gripping experience.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Alan Wake II&lt;/TITLE&gt;, the introductory monologue is delivered by a narrator who sets a haunting and mysterious tone. This sets the stage for the game's psychological horror narrative, where players follow Alan Wake, a troubled writer, as he navigates a surreal and nightmarish world. Alan Wake's journey is deeply entwined with the dark lore of Cauldron Lake, a mysterious body of water with the power to blur the lines between fiction and reality. The lake's supernatural influence has a history of ensnaring creative minds, warping their creations into terrifying manifestations. As Alan delves deeper into this twisted reality, he encounters shadowy figures and malevolent forces drawn from his own writings, all while trying to reclaim his lost memories and escape the encroaching darkness. The lore-rich environment is filled with references to ancient myths, eerie folklore, and the psychological horror elements that define Alan's struggle. Throughout the game, players must uncover the truth behind the dark presence that haunts Cauldron Lake, confront their deepest fears, and piece together the fragmented narrative to ultimately survive the harrowing ordeal.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Darkest Dungeon&lt;/TITLE&gt;, the introductory monologue is delivered by the Ancestor, who sets a grim and foreboding tone. This sets the stage for the game's gothic horror narrative, where players inherit a decayed estate plagued by eldritch horrors and madness. The Ancestor recounts how his insatiable curiosity and pursuit of forbidden knowledge led him to unearth a portal to an ancient, malevolent force beneath the manor. This act unleashed unspeakable evils that now corrupt the land and its inhabitants. Players take on the role of the heir, tasked with reclaiming the family estate and confronting the horrors that lurk within the Darkest Dungeon. The journey is fraught with peril, as players must assemble and lead a band of flawed heroes through nightmarish dungeons, battling terrifying creatures and coping with the ever-present threat of insanity. The game's rich lore is steeped in themes of decay, corruption, and the psychological toll of facing one's deepest fears. To restore the family’s honor, players must delve into the depths of the manor, uncover its dark secrets, and ultimately confront the ancient evil that has taken root in their ancestral home.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In &lt;TITLE&gt;NieR: Automata&lt;/TITLE&gt;, the introductory monologue delivered by the protagonist, 2B, sets the stage for the game's profound and philosophical narrative. The player takes on the role of 2B, an android soldier in the YoRHa unit, tasked with fighting a proxy war on Earth between human-made androids and alien-created machines. The remnants of humanity have fled to the Moon, leaving Earth as a battleground. As 2B, alongside her companion 9S, the player uncovers hidden truths about the war, their enemies, and themselves. The game explores themes of existentialism, the nature of life and death, and the search for meaning in a seemingly endless cycle of conflict. Through intense combat and emotional storytelling, the player's choices and actions reveal the complex layers of this post-apocalyptic world, challenging their perceptions of purpose and identity.
 </t>
   </si>
   <si>
-    <t>In &lt;TITLE&gt;Rise of the Ronin&lt;TITLE&gt;, the introductory monologue is delivered by a narrator who sets the historical and tumultuous tone of the game. This sets the stage for the game's narrative, set during the closing days of Japan's Edo period under the Tokugawa Shogunate. For three centuries, Japan remained isolated from the rest of the world, experiencing an era of apparent peace and prosperity. However, beneath this facade, tensions simmered as the feudal lords, or Daimyo, were held under strict control, fostering seeds of rebellion. In the remote mountains of Kurosu, a secret rebellion began to take shape with the clandestine forging of weapons. The Shogunate's forces discovered the plot and responded with brutal reprisals. Yet, another formidable force was being forged: the Veiled Edge. These elite warriors, masters of stealth and swordsmanship, trained in pairs known as blade twins, were unparalleled in their abilities. Players take on the role of a member of the Veiled Edge, navigating a world filled with political intrigue, ancient traditions, and the upheaval of a nation on the brink of revolution. The game's rich lore delves into the complexities of loyalty, honor, and the struggle for freedom, set against the backdrop of a changing Japan.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Sekiro: Shadows Die Twice&lt;TITLE&gt;, the introductory monologue sets the stage for the game's intense and immersive narrative. Taking place in the closing years of the Sengoku era, Japan is engulfed in relentless conflict. Amidst the chaos, Master swordsman Isshin Ashina seizes control of the land through a violent coup. A young orphan from the battlefield is taken under his wing, training to become a formidable shinobi. Twenty years later, the Ashina clan faces imminent collapse, and the shinobi, known as Wolf, finds himself bereft of both his mentor and the young lord he was duty-bound to protect. Players guide Wolf through a perilous journey of vengeance and redemption, navigating a beautifully crafted world filled with deadly foes and intricate challenges, as he seeks to restore his honor and rescue his lord.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Pillars of Eternity II: Deadfire&lt;TITLE&gt;, the introductory monologue sets the stage for the game's rich narrative. In the world of Eora, mortals live, die, and are reborn through the Wheel, overseen by the gods and facilitated by adra pillars. Five years ago, the protagonist, whom the player controls, was transformed into a Watcher with the ability to see and speak with souls. The player ended a crisis of soulless infants and defeated the immortal agent Thaos Ix Arkannon. After uncovering that the ancient Engwithans had turned themselves into gods, the protagonist retired to rule the castle of Caed Nua. However, unresolved tensions hint at further divine machinations, propelling the player into new adventures.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;The Stanley Parable&lt;TITLE&gt;, the introductory monologue sets the stage for the game's narrative. The player takes on the role of Stanley, an office worker who discovers that his colleagues have mysteriously vanished. As Stanley, the player navigates the deserted office, making choices that impact the story's direction. The game explores themes of free will, control, and the nature of decision-making, with the player's actions leading to various endings, all while a narrator comments on and sometimes reacts to Stanley's choices.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Killzone&lt;TITLE&gt;, the introductory monologue is delivered by Scolar Visari, the  ruthless leader of the Helghast and sets sets the stage for the game's intense and dramatic narrative. The player takes on the role of a soldier in the Interplanetary Strategic Alliance (ISA) fighting against Visari's forces. The Helghast, once oppressed and exiled to the harsh planet of Helghan, have grown stronger under Visari's leadership and now seek vengeance against those who wronged them. The player must navigate through war-torn environments, battling the formidable Helghast forces to protect their own people and prevent the Helghast from achieving their goal of conquest and retribution. The game explores themes of revenge, survival, and the brutal reality of war.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Call of Duty: Modern Warfare III&lt;TITLE&gt;, the introductory monologue sets the stage for the game's high-stakes narrative and is delivered by Vladimir Makarov, the primary antagonist. Makarov's actions have turned the world into a battlefield, exploiting deceit and the desire for vengeance to incite widespread conflict. The player takes on the roles of multiple soldiers across various international task forces as they combat Makarov's global threat. As the story unfolds, the player navigates through intense combat scenarios and covert operations to thwart Makarov's plans and restore peace. The game delves into themes of deception, the cost of war, and the impact of individual actions on global events.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Batman: Arkham Knight&lt;TITLE&gt;, the introductory monologue is delivered by Commissioner Gordon, setting the stage for the game's dark and intense narrative. Gotham City has descended into chaos following the death of the Joker, with criminal elements seizing control. The player takes on the role of Batman, Gotham’s last hope, as he faces a new threat led by the mysterious Arkham Knight and the returning Scarecrow. The game follows Batman as he battles to restore order, confronting his greatest foes and grappling with his own demons. Themes of fear, redemption, and the hero’s journey are central to this final chapter in the Arkham series.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Half-Life 2&lt;TITLE&gt;, the introductory monologue delivered by the enigmatic G-Man sets the stage for the game's gripping and dystopian narrative. The player takes on the role of Gordon Freeman, a theoretical physicist who is awakened by the G-Man to find Earth under the oppressive rule of the alien Combine. Humanity is on the brink of extinction, and the world is heavily controlled, with citizens living in fear. As Gordon, the player must navigate through this bleak environment, joining forces with the resistance to fight against the Combine's tyranny. The game explores themes of freedom, resistance, and the impact of one individual's actions in the face of overwhelming odds. Through innovative gameplay and immersive storytelling, players experience the struggle to reclaim Earth and uncover the deeper mysteries surrounding the G-Man's intentions and the true nature of the Combine's control.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;BioShock&lt;TITLE&gt;, the introductory monologue is delivered by Andrew Ryan, the visionary founder of the underwater city of Rapture. This sets the stage for the game's thought-provoking narrative. The player takes on the role of Jack, a man who finds himself in the mysterious and decaying utopia of Rapture after a plane crash. As Jack explores the city, he uncovers the dark secrets behind its creation and the societal collapse that ensued. The game delves into themes of objectivism, free will, and the consequences of unbridled ambition, as the player navigates through the dystopian landscape, facing mutated inhabitants and unraveling the truth about Rapture's downfall.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Dragon Age: Origins&lt;TITLE&gt;, the introductory monologue is delivered by Duncan, a senior member of the Grey Wardens. This sets the stage for the game's epic fantasy narrative. The player takes on the role of a new recruit to the Grey Wardens, an ancient order dedicated to combating the darkspawn—a monstrous race that threatens to bring about another Blight. As the darkspawn menace resurfaces, the player must unite the fractured kingdoms of Thedas, form alliances, and build an army to face the looming threat. The game explores themes of sacrifice, unity, and heroism, as the player navigates a richly detailed world filled with complex characters and moral choices, ultimately striving to save the world from annihilation.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Child of Light&lt;TITLE&gt;, the introductory monologue is delivered by a narrator, setting the stage for the game's enchanting narrative. The player takes on the role of Aurora, a young girl who mysteriously falls into a deep sleep and awakens in the magical land of Lemuria. As Aurora, the player embarks on a quest to return home by battling dark creatures and restoring the stolen light to Lemuria. Along the way, she gathers companions and uncovers the secrets of her destiny. The game explores themes of bravery, love, and self-discovery, all wrapped in a beautifully illustrated, fairy-tale world filled with poetry and wonder.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Metroid Prime&lt;TITLE&gt;, the introductory monologue is delivered by the main Character, setting the stage for the game's thrilling sci-fi narrative. The player takes on the role of Samus Aran, an interstellar bounty hunter who previously defeated the Space Pirates and their leader, Mother Brain, on Planet Zebes. Despite this victory, remnants of the Space Pirate forces survived and fled to regroup. Now, Samus has discovered a potential pirate colony on Planet Tallon IV. The player must explore this alien world, uncover its secrets, and thwart the Space Pirates' plans for resurgence. The game delves into themes of exploration, survival, and the relentless pursuit of justice as Samus battles to eliminate the pirate threat once and for all.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Mass Effect&lt;TITLE&gt;, the introductory monologue is delivered by a narrator, setting the stage for the game's expansive sci-fi narrative. The player takes on the role of Commander Shepard, a skilled soldier in the Systems Alliance. In 2148, humanity discovered advanced technology on Mars left behind by an ancient spacefaring civilization, which enabled faster-than-light travel and ushered in a new era of space exploration. This technology, known as Mass Effect, allowed humanity to join a galactic community of diverse alien species. As Commander Shepard, the player must navigate political intrigue, form alliances, and combat a looming threat that endangers the entire galaxy. The game explores themes of unity, destiny, and the struggle to protect all life from annihilation.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Fallout 76&lt;TITLE&gt;, the introductory monologue is delivered by the Overseer of Vault 76, setting the stage for the game's post-apocalyptic narrative. The player emerges as one of the first survivors to leave Vault 76, a secure underground shelter built to preserve America's best and brightest. The game begins on July 4th, 2076, marking 300 years since the founding of the United States. After a nuclear war devastates the world, the player must venture into the wasteland of West Virginia to rebuild society. The game explores themes of survival, community, and the enduring spirit of humanity as players work together to restore civilization in the face of a harsh and dangerous new world.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In &lt;TITLE&gt;Metro 2033&lt;TITLE&gt;, the introductory monologue delivered by Artyom sets the stage for the game's intense narrative. The player assumes the role of Artyom, a young man born just before a nuclear war forced humanity to seek refuge in the underground Metro stations of Moscow. Twenty years later, the Metro has become a bastion of human survival amidst a frozen, irradiated wasteland. As Artyom, the player must navigate the dangers of both the tunnels and the surface, contending with mutants, hostile factions, and a new, mysterious threat. The game explores themes of survival, hope, and the enduring human spirit as Artyom embarks on a perilous journey to save his home and uncover the secrets of the post-apocalyptic world.
+    <t>In &lt;TITLE&gt;Rise of the Ronin&lt;/TITLE&gt;, the introductory monologue is delivered by a narrator who sets the historical and tumultuous tone of the game. This sets the stage for the game's narrative, set during the closing days of Japan's Edo period under the Tokugawa Shogunate. For three centuries, Japan remained isolated from the rest of the world, experiencing an era of apparent peace and prosperity. However, beneath this facade, tensions simmered as the feudal lords, or Daimyo, were held under strict control, fostering seeds of rebellion. In the remote mountains of Kurosu, a secret rebellion began to take shape with the clandestine forging of weapons. The Shogunate's forces discovered the plot and responded with brutal reprisals. Yet, another formidable force was being forged: the Veiled Edge. These elite warriors, masters of stealth and swordsmanship, trained in pairs known as blade twins, were unparalleled in their abilities. Players take on the role of a member of the Veiled Edge, navigating a world filled with political intrigue, ancient traditions, and the upheaval of a nation on the brink of revolution. The game's rich lore delves into the complexities of loyalty, honor, and the struggle for freedom, set against the backdrop of a changing Japan.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Sekiro: Shadows Die Twice&lt;/TITLE&gt;, the introductory monologue sets the stage for the game's intense and immersive narrative. Taking place in the closing years of the Sengoku era, Japan is engulfed in relentless conflict. Amidst the chaos, Master swordsman Isshin Ashina seizes control of the land through a violent coup. A young orphan from the battlefield is taken under his wing, training to become a formidable shinobi. Twenty years later, the Ashina clan faces imminent collapse, and the shinobi, known as Wolf, finds himself bereft of both his mentor and the young lord he was duty-bound to protect. Players guide Wolf through a perilous journey of vengeance and redemption, navigating a beautifully crafted world filled with deadly foes and intricate challenges, as he seeks to restore his honor and rescue his lord.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Pillars of Eternity II: Deadfire&lt;/TITLE&gt;, the introductory monologue sets the stage for the game's rich narrative. In the world of Eora, mortals live, die, and are reborn through the Wheel, overseen by the gods and facilitated by adra pillars. Five years ago, the protagonist, whom the player controls, was transformed into a Watcher with the ability to see and speak with souls. The player ended a crisis of soulless infants and defeated the immortal agent Thaos Ix Arkannon. After uncovering that the ancient Engwithans had turned themselves into gods, the protagonist retired to rule the castle of Caed Nua. However, unresolved tensions hint at further divine machinations, propelling the player into new adventures.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;The Stanley Parable&lt;/TITLE&gt;, the introductory monologue sets the stage for the game's narrative. The player takes on the role of Stanley, an office worker who discovers that his colleagues have mysteriously vanished. As Stanley, the player navigates the deserted office, making choices that impact the story's direction. The game explores themes of free will, control, and the nature of decision-making, with the player's actions leading to various endings, all while a narrator comments on and sometimes reacts to Stanley's choices.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Killzone&lt;/TITLE&gt;, the introductory monologue is delivered by Scolar Visari, the  ruthless leader of the Helghast and sets sets the stage for the game's intense and dramatic narrative. The player takes on the role of a soldier in the Interplanetary Strategic Alliance (ISA) fighting against Visari's forces. The Helghast, once oppressed and exiled to the harsh planet of Helghan, have grown stronger under Visari's leadership and now seek vengeance against those who wronged them. The player must navigate through war-torn environments, battling the formidable Helghast forces to protect their own people and prevent the Helghast from achieving their goal of conquest and retribution. The game explores themes of revenge, survival, and the brutal reality of war.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Call of Duty: Modern Warfare III&lt;/TITLE&gt;, the introductory monologue sets the stage for the game's high-stakes narrative and is delivered by Vladimir Makarov, the primary antagonist. Makarov's actions have turned the world into a battlefield, exploiting deceit and the desire for vengeance to incite widespread conflict. The player takes on the roles of multiple soldiers across various international task forces as they combat Makarov's global threat. As the story unfolds, the player navigates through intense combat scenarios and covert operations to thwart Makarov's plans and restore peace. The game delves into themes of deception, the cost of war, and the impact of individual actions on global events.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Batman: Arkham Knight&lt;/TITLE&gt;, the introductory monologue is delivered by Commissioner Gordon, setting the stage for the game's dark and intense narrative. Gotham City has descended into chaos following the death of the Joker, with criminal elements seizing control. The player takes on the role of Batman, Gotham’s last hope, as he faces a new threat led by the mysterious Arkham Knight and the returning Scarecrow. The game follows Batman as he battles to restore order, confronting his greatest foes and grappling with his own demons. Themes of fear, redemption, and the hero’s journey are central to this final chapter in the Arkham series.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Half-Life 2&lt;/TITLE&gt;, the introductory monologue delivered by the enigmatic G-Man sets the stage for the game's gripping and dystopian narrative. The player takes on the role of Gordon Freeman, a theoretical physicist who is awakened by the G-Man to find Earth under the oppressive rule of the alien Combine. Humanity is on the brink of extinction, and the world is heavily controlled, with citizens living in fear. As Gordon, the player must navigate through this bleak environment, joining forces with the resistance to fight against the Combine's tyranny. The game explores themes of freedom, resistance, and the impact of one individual's actions in the face of overwhelming odds. Through innovative gameplay and immersive storytelling, players experience the struggle to reclaim Earth and uncover the deeper mysteries surrounding the G-Man's intentions and the true nature of the Combine's control.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;BioShock&lt;/TITLE&gt;, the introductory monologue is delivered by Andrew Ryan, the visionary founder of the underwater city of Rapture. This sets the stage for the game's thought-provoking narrative. The player takes on the role of Jack, a man who finds himself in the mysterious and decaying utopia of Rapture after a plane crash. As Jack explores the city, he uncovers the dark secrets behind its creation and the societal collapse that ensued. The game delves into themes of objectivism, free will, and the consequences of unbridled ambition, as the player navigates through the dystopian landscape, facing mutated inhabitants and unraveling the truth about Rapture's downfall.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Dragon Age: Origins&lt;/TITLE&gt;, the introductory monologue is delivered by Duncan, a senior member of the Grey Wardens. This sets the stage for the game's epic fantasy narrative. The player takes on the role of a new recruit to the Grey Wardens, an ancient order dedicated to combating the darkspawn—a monstrous race that threatens to bring about another Blight. As the darkspawn menace resurfaces, the player must unite the fractured kingdoms of Thedas, form alliances, and build an army to face the looming threat. The game explores themes of sacrifice, unity, and heroism, as the player navigates a richly detailed world filled with complex characters and moral choices, ultimately striving to save the world from annihilation.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Child of Light&lt;/TITLE&gt;, the introductory monologue is delivered by a narrator, setting the stage for the game's enchanting narrative. The player takes on the role of Aurora, a young girl who mysteriously falls into a deep sleep and awakens in the magical land of Lemuria. As Aurora, the player embarks on a quest to return home by battling dark creatures and restoring the stolen light to Lemuria. Along the way, she gathers companions and uncovers the secrets of her destiny. The game explores themes of bravery, love, and self-discovery, all wrapped in a beautifully illustrated, fairy-tale world filled with poetry and wonder.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Metroid Prime&lt;/TITLE&gt;, the introductory monologue is delivered by the main Character, setting the stage for the game's thrilling sci-fi narrative. The player takes on the role of Samus Aran, an interstellar bounty hunter who previously defeated the Space Pirates and their leader, Mother Brain, on Planet Zebes. Despite this victory, remnants of the Space Pirate forces survived and fled to regroup. Now, Samus has discovered a potential pirate colony on Planet Tallon IV. The player must explore this alien world, uncover its secrets, and thwart the Space Pirates' plans for resurgence. The game delves into themes of exploration, survival, and the relentless pursuit of justice as Samus battles to eliminate the pirate threat once and for all.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Mass Effect&lt;/TITLE&gt;, the introductory monologue is delivered by a narrator, setting the stage for the game's expansive sci-fi narrative. The player takes on the role of Commander Shepard, a skilled soldier in the Systems Alliance. In 2148, humanity discovered advanced technology on Mars left behind by an ancient spacefaring civilization, which enabled faster-than-light travel and ushered in a new era of space exploration. This technology, known as Mass Effect, allowed humanity to join a galactic community of diverse alien species. As Commander Shepard, the player must navigate political intrigue, form alliances, and combat a looming threat that endangers the entire galaxy. The game explores themes of unity, destiny, and the struggle to protect all life from annihilation.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Fallout 76&lt;/TITLE&gt;, the introductory monologue is delivered by the Overseer of Vault 76, setting the stage for the game's post-apocalyptic narrative. The player emerges as one of the first survivors to leave Vault 76, a secure underground shelter built to preserve America's best and brightest. The game begins on July 4th, 2076, marking 300 years since the founding of the United States. After a nuclear war devastates the world, the player must venture into the wasteland of West Virginia to rebuild society. The game explores themes of survival, community, and the enduring spirit of humanity as players work together to restore civilization in the face of a harsh and dangerous new world.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In &lt;TITLE&gt;Metro 2033&lt;/TITLE&gt;, the introductory monologue delivered by Artyom sets the stage for the game's intense narrative. The player assumes the role of Artyom, a young man born just before a nuclear war forced humanity to seek refuge in the underground Metro stations of Moscow. Twenty years later, the Metro has become a bastion of human survival amidst a frozen, irradiated wasteland. As Artyom, the player must navigate the dangers of both the tunnels and the surface, contending with mutants, hostile factions, and a new, mysterious threat. The game explores themes of survival, hope, and the enduring human spirit as Artyom embarks on a perilous journey to save his home and uncover the secrets of the post-apocalyptic world.
 </t>
   </si>
   <si>
-    <t>In &lt;TITLE&gt;Metro: Exodus&lt;TITLE&gt;, the introductory monologue delivered by Artyom sets the stage for the game's post-apocalyptic journey. The player takes on the role of Artyom, a survivor living in the Metro tunnels beneath Moscow after a devastating nuclear war. Driven by a belief that life still exists beyond the irradiated ruins, Artyom embarks on a perilous quest to find a new home on the surface. Alongside a group of fellow survivors, he travels across the vast, dangerous landscapes of Russia aboard the Aurora, a heavily modified steam locomotive. The game explores themes of survival, hope, and the search for a better future, as Artyom and his companions face hostile environments, mutated creatures, and human adversaries in their quest to rebuild their lives.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In &lt;TITLE&gt;Vampyr&lt;TITLE&gt;, the introductory monologue sets the tone for the game's dark and atmospheric narrative. The player takes on the role of Dr. Jonathan Reid, a renowned surgeon in early 20th-century London who is transformed into a vampire amidst a deadly flu epidemic. Struggling with his new supernatural condition, Jonathan must find a balance between his duty to save the citizens as a doctor and his uncontrollable thirst for blood. As he navigates the eerie, plague-ridden streets of London, Jonathan uncovers dark secrets and faces moral dilemmas that challenge his humanity. The game explores themes of life, death, and redemption, with the player's choices deeply influencing the fate of the city's inhabitants and Jonathan's own destiny.
+    <t>In &lt;TITLE&gt;Metro: Exodus&lt;/TITLE&gt;, the introductory monologue delivered by Artyom sets the stage for the game's post-apocalyptic journey. The player takes on the role of Artyom, a survivor living in the Metro tunnels beneath Moscow after a devastating nuclear war. Driven by a belief that life still exists beyond the irradiated ruins, Artyom embarks on a perilous quest to find a new home on the surface. Alongside a group of fellow survivors, he travels across the vast, dangerous landscapes of Russia aboard the Aurora, a heavily modified steam locomotive. The game explores themes of survival, hope, and the search for a better future, as Artyom and his companions face hostile environments, mutated creatures, and human adversaries in their quest to rebuild their lives.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In &lt;TITLE&gt;Vampyr&lt;/TITLE&gt;, the introductory monologue sets the tone for the game's dark and atmospheric narrative. The player takes on the role of Dr. Jonathan Reid, a renowned surgeon in early 20th-century London who is transformed into a vampire amidst a deadly flu epidemic. Struggling with his new supernatural condition, Jonathan must find a balance between his duty to save the citizens as a doctor and his uncontrollable thirst for blood. As he navigates the eerie, plague-ridden streets of London, Jonathan uncovers dark secrets and faces moral dilemmas that challenge his humanity. The game explores themes of life, death, and redemption, with the player's choices deeply influencing the fate of the city's inhabitants and Jonathan's own destiny.
 </t>
   </si>
   <si>
-    <t>In &lt;TITLE&gt;Fallout&lt;TITLE&gt;, the introductory monologue delivered by the narrator, sets the stage for the game's post-apocalyptic narrative. The player takes on the role of a Vault Dweller, a descendant of those who survived the nuclear war of 2077 by seeking refuge in Vault 13. For generations, the inhabitants have lived in the safety of the underground Vault, isolated from the devastated world above. However, the Vault's water purification chip fails, and the player is tasked with venturing into the dangerous, irradiated wasteland to find a replacement. The game explores themes of survival, the consequences of war, and the rebuilding of civilization, as the player navigates through a world filled with mutated creatures, hostile factions, and remnants of pre-war society. The player's actions and decisions will shape the future of the wasteland and determine the fate of humanity's remnants.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Godfall&lt;TITLE&gt;, the introductory monologue delivered by the main protagonist, Orin, sets the stage for the game's epic fantasy narrative. The player takes on the role of Orin, a powerful warrior from the Knight's Order, who was betrayed by his own brother, Macros. Macros sought to achieve godhood, manipulating his fellow warriors and turning them against each other. Left for dead by Macros, Orin survives and begins a quest for vengeance. The player must gather powerful weapons and armor, known as Valorplates, to combat Macros and his army. As Orin, the player navigates through various realms, battling formidable enemies and uncovering the truth behind Macros's treachery. The game explores themes of betrayal, redemption, and the relentless pursuit of justice in a world filled with mythic heroes and divine powers.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;DOOM: Eternal&lt;TITLE&gt;, the introductory monologue delivered by the ARC (Armored Response Coalition) sets the stage for the game's intense and brutal narrative. The player takes on the role of the Doom Slayer, humanity's last hope against the demonic forces of Hell that have overrun Earth. Tasked with stopping the apocalypse, the Doom Slayer must battle through hordes of demons using a vast arsenal of weapons and brutal combat skills. The game explores themes of unrelenting determination, the fight against overwhelming odds, and the quest to save humanity from annihilation. As the Doom Slayer, the player navigates through various hellish landscapes, ripping and tearing through enemies to fulfill the mission: to end the demonic invasion and restore order to the universe.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Titanfall 2&lt;TITLE&gt;, the introductory monologue delivered by Jack Cooper sets the stage for the game's high-octane narrative. The player takes on the role of Jack Cooper, a rifleman in the Frontier Militia, who dreams of becoming a pilot—elite warriors capable of controlling powerful Titans. Pilots are fast, agile, and formidable, with a unique bond to their Titans that makes them nearly unstoppable. The Frontier, Cooper's home, has been ravaged by the oppressive IMC, which exploits the region's resources and brutalizes its inhabitants. Despite recent victories, the fight against the IMC is far from over. Cooper's journey begins with a mission that quickly spirals into chaos, leading him to inherit a Titan named BT-7274 after its pilot is killed. As Cooper and BT form a bond, the player navigates through intense combat scenarios, utilizing both Pilot agility and Titan firepower. The game explores themes of camaraderie, resilience, and the struggle for freedom, as Cooper strives to honor his fallen mentor and help liberate the Frontier from IMC control.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Mad Max: Fury Road&lt;TITLE&gt;, the introductory monologue delivered by Max Rockatansky sets the stage for the game's post-apocalyptic narrative. The player takes on the role of Max, a lone survivor in a desolate world where civilization has collapsed and most of humanity has perished. Those who were born into this harsh new reality know no other life, while the survivors from the old world are haunted by memories of what once was. Max, a broken man driven by his past, navigates through the wasteland, battling vicious warlords and scavenging for resources. The game explores themes of survival, loss, and the relentless fight to find hope and redemption in a brutal, unforgiving environment. As Max, the player must overcome overwhelming odds and forge alliances to endure in this desolate landscape.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Middle-earth: Shadow of Mordor&lt;TITLE&gt;, the introductory monologue delivered by a narrator sets the stage for the game's dark and epic narrative. The player takes on the role of Talion, a Ranger of Gondor, who is stationed at the Black Gate of Mordor. This once mighty fortress is now a desolate outpost where the Rangers have guarded against the resurgence of the Dark Lord Sauron for two and a half thousand years. As the power and malice of Sauron grow, he returns to Mordor, bringing shadow and flame that devastate the land. Talion, along with his family, falls victim to Sauron's forces, but he is resurrected and bound to a mysterious Wraith, Celebrimbor. Together, they embark on a quest for vengeance against Sauron and his minions. The game explores themes of revenge, redemption, and the blurred lines between good and evil. As Talion, the player must navigate the treacherous land of Mordor, build an army, and dismantle Sauron's forces from within using a unique nemesis system that personalizes enemy interactions and rivalries.</t>
-  </si>
-  <si>
-    <t>In &lt;TITLE&gt;Kingdom Come: Deliverance&lt;TITLE&gt;, the introductory monologue delivered by Henry, the protagonist, sets the stage for the game's historical narrative. The game is set in the Kingdom of Bohemia during a time of great turmoil following the death of Emperor Charles IV. His son, Wenceslas IV, ascends to the throne but proves to be an ineffective ruler, neglecting his duties in favor of personal indulgences. This leads to political instability, prompting Wenceslas's half-brother, King Sigismund of Hungary, to seize the opportunity to take control. Sigismund kidnaps Wenceslas and invades Bohemia with a mercenary army, causing widespread chaos and destruction. The player takes on the role of Henry, a blacksmith's son whose peaceful life is shattered when his village is attacked by Sigismund's forces. Driven by a desire for revenge and justice, Henry becomes embroiled in the conflict, seeking to restore order to his homeland. The game explores themes of loyalty, vengeance, and the struggle for power in a meticulously recreated medieval world, where the player's choices and actions shape Henry's journey and the fate of Bohemia.</t>
-  </si>
-  <si>
-    <t>the Guard speaking is a Stormcloak Guard</t>
-  </si>
-  <si>
-    <t>the Guard speaking is a Imperial Guard</t>
-  </si>
-  <si>
-    <t>the Guard speaking is an Imperial Guard</t>
-  </si>
-  <si>
-    <t>the Guard is in the Windhelm region</t>
-  </si>
-  <si>
-    <t>the Player is a member of Thieves Guild</t>
-  </si>
-  <si>
-    <t>Guard reacting to the Player's weapon</t>
-  </si>
-  <si>
-    <t>Guard reacting to the Player's artifacts and unique items</t>
-  </si>
-  <si>
-    <t>a Guard reacting to the Player's race</t>
-  </si>
-  <si>
-    <t>a Guard reacting to the Player's high skill level in Alchemy</t>
-  </si>
-  <si>
-    <t>a Guard reacting to the Player's high skill level in Conjuration</t>
-  </si>
-  <si>
-    <t>a Guard reacting to the Player's high skill level in Destruction</t>
-  </si>
-  <si>
-    <t>a Guard reacting to the Player's high skill level in Enchanting</t>
-  </si>
-  <si>
-    <t>a Guard reacting to the Player's high skill level in the use of heavy armor</t>
-  </si>
-  <si>
-    <t>a Guard reacting to the Player's high skill level in Illusions</t>
-  </si>
-  <si>
-    <t>a Guard reacting to the Player's high skill level in the use of light armor</t>
-  </si>
-  <si>
-    <t>a Guard reacting to the Player's high skill level in Lockpicking</t>
-  </si>
-  <si>
-    <t>a Guard reacting to the Player's high skill level in the use of one-handed weapons</t>
-  </si>
-  <si>
-    <t>a Guard reacting to the Player's high skill level in Pickpocketing</t>
-  </si>
-  <si>
-    <t>a Guard reacting to the Player's high skill level in Restoration</t>
-  </si>
-  <si>
-    <t>a Guard reacting to the Player's high skill level in Sneaking</t>
-  </si>
-  <si>
-    <t>a Guard reacting to the Player's high skill level in the use of Speech</t>
-  </si>
-  <si>
-    <t>a Guard reacting to the Player's high skill level in the use of Two-Handed weapons</t>
-  </si>
-  <si>
-    <t>the Player has not purchased Breezehome</t>
-  </si>
-  <si>
-    <t>the Player has purchased Breezehome</t>
-  </si>
-  <si>
-    <t>the Player has a desease</t>
-  </si>
-  <si>
-    <t>the Player has not purchased  Hjerim</t>
-  </si>
-  <si>
-    <t>the Player has purchased Hjerim</t>
-  </si>
-  <si>
-    <t>an NPC witnessing a theft</t>
+    <t>In &lt;TITLE&gt;Fallout&lt;/TITLE&gt;, the introductory monologue delivered by the narrator, sets the stage for the game's post-apocalyptic narrative. The player takes on the role of a Vault Dweller, a descendant of those who survived the nuclear war of 2077 by seeking refuge in Vault 13. For generations, the inhabitants have lived in the safety of the underground Vault, isolated from the devastated world above. However, the Vault's water purification chip fails, and the player is tasked with venturing into the dangerous, irradiated wasteland to find a replacement. The game explores themes of survival, the consequences of war, and the rebuilding of civilization, as the player navigates through a world filled with mutated creatures, hostile factions, and remnants of pre-war society. The player's actions and decisions will shape the future of the wasteland and determine the fate of humanity's remnants.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Godfall&lt;/TITLE&gt;, the introductory monologue delivered by the main protagonist, Orin, sets the stage for the game's epic fantasy narrative. The player takes on the role of Orin, a powerful warrior from the Knight's Order, who was betrayed by his own brother, Macros. Macros sought to achieve godhood, manipulating his fellow warriors and turning them against each other. Left for dead by Macros, Orin survives and begins a quest for vengeance. The player must gather powerful weapons and armor, known as Valorplates, to combat Macros and his army. As Orin, the player navigates through various realms, battling formidable enemies and uncovering the truth behind Macros's treachery. The game explores themes of betrayal, redemption, and the relentless pursuit of justice in a world filled with mythic heroes and divine powers.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;DOOM: Eternal&lt;/TITLE&gt;, the introductory monologue delivered by the ARC (Armored Response Coalition) sets the stage for the game's intense and brutal narrative. The player takes on the role of the Doom Slayer, humanity's last hope against the demonic forces of Hell that have overrun Earth. Tasked with stopping the apocalypse, the Doom Slayer must battle through hordes of demons using a vast arsenal of weapons and brutal combat skills. The game explores themes of unrelenting determination, the fight against overwhelming odds, and the quest to save humanity from annihilation. As the Doom Slayer, the player navigates through various hellish landscapes, ripping and tearing through enemies to fulfill the mission: to end the demonic invasion and restore order to the universe.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Titanfall 2&lt;/TITLE&gt;, the introductory monologue delivered by Jack Cooper sets the stage for the game's high-octane narrative. The player takes on the role of Jack Cooper, a rifleman in the Frontier Militia, who dreams of becoming a pilot—elite warriors capable of controlling powerful Titans. Pilots are fast, agile, and formidable, with a unique bond to their Titans that makes them nearly unstoppable. The Frontier, Cooper's home, has been ravaged by the oppressive IMC, which exploits the region's resources and brutalizes its inhabitants. Despite recent victories, the fight against the IMC is far from over. Cooper's journey begins with a mission that quickly spirals into chaos, leading him to inherit a Titan named BT-7274 after its pilot is killed. As Cooper and BT form a bond, the player navigates through intense combat scenarios, utilizing both Pilot agility and Titan firepower. The game explores themes of camaraderie, resilience, and the struggle for freedom, as Cooper strives to honor his fallen mentor and help liberate the Frontier from IMC control.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Mad Max: Fury Road&lt;/TITLE&gt;, the introductory monologue delivered by Max Rockatansky sets the stage for the game's post-apocalyptic narrative. The player takes on the role of Max, a lone survivor in a desolate world where civilization has collapsed and most of humanity has perished. Those who were born into this harsh new reality know no other life, while the survivors from the old world are haunted by memories of what once was. Max, a broken man driven by his past, navigates through the wasteland, battling vicious warlords and scavenging for resources. The game explores themes of survival, loss, and the relentless fight to find hope and redemption in a brutal, unforgiving environment. As Max, the player must overcome overwhelming odds and forge alliances to endure in this desolate landscape.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Middle-earth: Shadow of Mordor&lt;/TITLE&gt;, the introductory monologue delivered by a narrator sets the stage for the game's dark and epic narrative. The player takes on the role of Talion, a Ranger of Gondor, who is stationed at the Black Gate of Mordor. This once mighty fortress is now a desolate outpost where the Rangers have guarded against the resurgence of the Dark Lord Sauron for two and a half thousand years. As the power and malice of Sauron grow, he returns to Mordor, bringing shadow and flame that devastate the land. Talion, along with his family, falls victim to Sauron's forces, but he is resurrected and bound to a mysterious Wraith, Celebrimbor. Together, they embark on a quest for vengeance against Sauron and his minions. The game explores themes of revenge, redemption, and the blurred lines between good and evil. As Talion, the player must navigate the treacherous land of Mordor, build an army, and dismantle Sauron's forces from within using a unique nemesis system that personalizes enemy interactions and rivalries.</t>
+  </si>
+  <si>
+    <t>In &lt;TITLE&gt;Kingdom Come: Deliverance&lt;/TITLE&gt;, the introductory monologue delivered by Henry, the protagonist, sets the stage for the game's historical narrative. The game is set in the Kingdom of Bohemia during a time of great turmoil following the death of Emperor Charles IV. His son, Wenceslas IV, ascends to the throne but proves to be an ineffective ruler, neglecting his duties in favor of personal indulgences. This leads to political instability, prompting Wenceslas's half-brother, King Sigismund of Hungary, to seize the opportunity to take control. Sigismund kidnaps Wenceslas and invades Bohemia with a mercenary army, causing widespread chaos and destruction. The player takes on the role of Henry, a blacksmith's son whose peaceful life is shattered when his village is attacked by Sigismund's forces. Driven by a desire for revenge and justice, Henry becomes embroiled in the conflict, seeking to restore order to his homeland. The game explores themes of loyalty, vengeance, and the struggle for power in a meticulously recreated medieval world, where the player's choices and actions shape Henry's journey and the fate of Bohemia.</t>
   </si>
 </sst>
 </file>
@@ -11121,7 +11121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F4422B-9562-488B-BAFD-465E06419C42}">
   <dimension ref="A1:D190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -18352,7 +18352,7 @@
         <v>154</v>
       </c>
       <c r="D2" t="s">
-        <v>1785</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -18366,7 +18366,7 @@
         <v>154</v>
       </c>
       <c r="D3" t="s">
-        <v>1785</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -18380,7 +18380,7 @@
         <v>265</v>
       </c>
       <c r="D4" t="s">
-        <v>1785</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -18394,7 +18394,7 @@
         <v>266</v>
       </c>
       <c r="D5" t="s">
-        <v>1785</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -18408,7 +18408,7 @@
         <v>266</v>
       </c>
       <c r="D6" t="s">
-        <v>1785</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -18422,7 +18422,7 @@
         <v>267</v>
       </c>
       <c r="D7" t="s">
-        <v>1785</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -18436,7 +18436,7 @@
         <v>268</v>
       </c>
       <c r="D8" t="s">
-        <v>1785</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -18450,7 +18450,7 @@
         <v>269</v>
       </c>
       <c r="D9" t="s">
-        <v>1785</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -18464,7 +18464,7 @@
         <v>269</v>
       </c>
       <c r="D10" t="s">
-        <v>1785</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -18478,7 +18478,7 @@
         <v>154</v>
       </c>
       <c r="D11" t="s">
-        <v>1785</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -18492,7 +18492,7 @@
         <v>154</v>
       </c>
       <c r="D12" t="s">
-        <v>1785</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -18506,7 +18506,7 @@
         <v>265</v>
       </c>
       <c r="D13" t="s">
-        <v>1785</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -18520,7 +18520,7 @@
         <v>154</v>
       </c>
       <c r="D14" t="s">
-        <v>1785</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -18534,7 +18534,7 @@
         <v>154</v>
       </c>
       <c r="D15" t="s">
-        <v>1785</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -18548,7 +18548,7 @@
         <v>270</v>
       </c>
       <c r="D16" t="s">
-        <v>1785</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -18562,7 +18562,7 @@
         <v>270</v>
       </c>
       <c r="D17" t="s">
-        <v>1785</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -18576,7 +18576,7 @@
         <v>154</v>
       </c>
       <c r="D18" t="s">
-        <v>1785</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -18590,7 +18590,7 @@
         <v>154</v>
       </c>
       <c r="D19" t="s">
-        <v>1785</v>
+        <v>1735</v>
       </c>
     </row>
   </sheetData>
@@ -18640,7 +18640,7 @@
         <v>154</v>
       </c>
       <c r="D2" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -18654,7 +18654,7 @@
         <v>154</v>
       </c>
       <c r="D3" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -18668,7 +18668,7 @@
         <v>154</v>
       </c>
       <c r="D4" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -18682,7 +18682,7 @@
         <v>154</v>
       </c>
       <c r="D5" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -18696,7 +18696,7 @@
         <v>154</v>
       </c>
       <c r="D6" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -18710,7 +18710,7 @@
         <v>154</v>
       </c>
       <c r="D7" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -18724,7 +18724,7 @@
         <v>154</v>
       </c>
       <c r="D8" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -18738,7 +18738,7 @@
         <v>154</v>
       </c>
       <c r="D9" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -18752,7 +18752,7 @@
         <v>154</v>
       </c>
       <c r="D10" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -18766,7 +18766,7 @@
         <v>154</v>
       </c>
       <c r="D11" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -18780,7 +18780,7 @@
         <v>154</v>
       </c>
       <c r="D12" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -18794,7 +18794,7 @@
         <v>154</v>
       </c>
       <c r="D13" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -18808,7 +18808,7 @@
         <v>154</v>
       </c>
       <c r="D14" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -18822,7 +18822,7 @@
         <v>154</v>
       </c>
       <c r="D15" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -18836,7 +18836,7 @@
         <v>154</v>
       </c>
       <c r="D16" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -18850,7 +18850,7 @@
         <v>154</v>
       </c>
       <c r="D17" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -18864,7 +18864,7 @@
         <v>154</v>
       </c>
       <c r="D18" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -18878,7 +18878,7 @@
         <v>154</v>
       </c>
       <c r="D19" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -18892,7 +18892,7 @@
         <v>154</v>
       </c>
       <c r="D20" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -18906,7 +18906,7 @@
         <v>154</v>
       </c>
       <c r="D21" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -18920,7 +18920,7 @@
         <v>154</v>
       </c>
       <c r="D22" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -18931,10 +18931,10 @@
         <v>178</v>
       </c>
       <c r="C23" t="s">
-        <v>1778</v>
+        <v>1728</v>
       </c>
       <c r="D23" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -18945,10 +18945,10 @@
         <v>178</v>
       </c>
       <c r="C24" t="s">
-        <v>1779</v>
+        <v>1729</v>
       </c>
       <c r="D24" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -18959,10 +18959,10 @@
         <v>181</v>
       </c>
       <c r="C25" t="s">
-        <v>1778</v>
+        <v>1728</v>
       </c>
       <c r="D25" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -18973,10 +18973,10 @@
         <v>181</v>
       </c>
       <c r="C26" t="s">
-        <v>1779</v>
+        <v>1729</v>
       </c>
       <c r="D26" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -18990,7 +18990,7 @@
         <v>271</v>
       </c>
       <c r="D27" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -19004,7 +19004,7 @@
         <v>271</v>
       </c>
       <c r="D28" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -19015,10 +19015,10 @@
         <v>183</v>
       </c>
       <c r="C29" t="s">
-        <v>1778</v>
+        <v>1728</v>
       </c>
       <c r="D29" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -19029,10 +19029,10 @@
         <v>183</v>
       </c>
       <c r="C30" t="s">
-        <v>1780</v>
+        <v>1730</v>
       </c>
       <c r="D30" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -19043,10 +19043,10 @@
         <v>184</v>
       </c>
       <c r="C31" t="s">
-        <v>1778</v>
+        <v>1728</v>
       </c>
       <c r="D31" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -19057,10 +19057,10 @@
         <v>184</v>
       </c>
       <c r="C32" t="s">
-        <v>1780</v>
+        <v>1730</v>
       </c>
       <c r="D32" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -19074,7 +19074,7 @@
         <v>154</v>
       </c>
       <c r="D33" t="s">
-        <v>1783</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -19088,7 +19088,7 @@
         <v>154</v>
       </c>
       <c r="D34" t="s">
-        <v>1784</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -19102,7 +19102,7 @@
         <v>154</v>
       </c>
       <c r="D35" t="s">
-        <v>1784</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -19116,7 +19116,7 @@
         <v>272</v>
       </c>
       <c r="D36" t="s">
-        <v>1784</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -19127,10 +19127,10 @@
         <v>190</v>
       </c>
       <c r="C37" t="s">
-        <v>1781</v>
+        <v>1731</v>
       </c>
       <c r="D37" t="s">
-        <v>1784</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -19141,10 +19141,10 @@
         <v>190</v>
       </c>
       <c r="C38" t="s">
-        <v>1781</v>
+        <v>1731</v>
       </c>
       <c r="D38" t="s">
-        <v>1784</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -19158,7 +19158,7 @@
         <v>154</v>
       </c>
       <c r="D39" t="s">
-        <v>1784</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -19172,7 +19172,7 @@
         <v>154</v>
       </c>
       <c r="D40" t="s">
-        <v>1784</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -19186,7 +19186,7 @@
         <v>154</v>
       </c>
       <c r="D41" t="s">
-        <v>1784</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -19200,7 +19200,7 @@
         <v>154</v>
       </c>
       <c r="D42" t="s">
-        <v>1784</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -19214,7 +19214,7 @@
         <v>154</v>
       </c>
       <c r="D43" t="s">
-        <v>1784</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -19228,7 +19228,7 @@
         <v>154</v>
       </c>
       <c r="D44" t="s">
-        <v>1784</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -19242,7 +19242,7 @@
         <v>154</v>
       </c>
       <c r="D45" t="s">
-        <v>1784</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -19256,7 +19256,7 @@
         <v>154</v>
       </c>
       <c r="D46" t="s">
-        <v>1784</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -19270,7 +19270,7 @@
         <v>154</v>
       </c>
       <c r="D47" t="s">
-        <v>1784</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -19284,7 +19284,7 @@
         <v>154</v>
       </c>
       <c r="D48" t="s">
-        <v>1784</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -19298,7 +19298,7 @@
         <v>154</v>
       </c>
       <c r="D49" t="s">
-        <v>1784</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -19309,10 +19309,10 @@
         <v>199</v>
       </c>
       <c r="C50" t="s">
-        <v>1782</v>
+        <v>1732</v>
       </c>
       <c r="D50" t="s">
-        <v>1784</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -19326,7 +19326,7 @@
         <v>154</v>
       </c>
       <c r="D51" t="s">
-        <v>1784</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -19340,7 +19340,7 @@
         <v>154</v>
       </c>
       <c r="D52" t="s">
-        <v>1784</v>
+        <v>1734</v>
       </c>
     </row>
   </sheetData>
@@ -19375,7 +19375,7 @@
         <v>1584</v>
       </c>
       <c r="B2" t="s">
-        <v>1786</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -19383,7 +19383,7 @@
         <v>1585</v>
       </c>
       <c r="B3" t="s">
-        <v>1786</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -19391,7 +19391,7 @@
         <v>1586</v>
       </c>
       <c r="B4" t="s">
-        <v>1786</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -19399,7 +19399,7 @@
         <v>1587</v>
       </c>
       <c r="B5" t="s">
-        <v>1786</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -19407,7 +19407,7 @@
         <v>1588</v>
       </c>
       <c r="B6" t="s">
-        <v>1787</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -19415,7 +19415,7 @@
         <v>1589</v>
       </c>
       <c r="B7" t="s">
-        <v>1788</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -19423,7 +19423,7 @@
         <v>1590</v>
       </c>
       <c r="B8" t="s">
-        <v>1789</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -19431,7 +19431,7 @@
         <v>1591</v>
       </c>
       <c r="B9" t="s">
-        <v>1790</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -19439,7 +19439,7 @@
         <v>1592</v>
       </c>
       <c r="B10" t="s">
-        <v>1791</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -19447,7 +19447,7 @@
         <v>1593</v>
       </c>
       <c r="B11" t="s">
-        <v>1792</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -19455,7 +19455,7 @@
         <v>1594</v>
       </c>
       <c r="B12" t="s">
-        <v>1793</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -19463,7 +19463,7 @@
         <v>1595</v>
       </c>
       <c r="B13" t="s">
-        <v>1794</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -19471,7 +19471,7 @@
         <v>1596</v>
       </c>
       <c r="B14" t="s">
-        <v>1795</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -19479,7 +19479,7 @@
         <v>1597</v>
       </c>
       <c r="B15" t="s">
-        <v>1795</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -19487,7 +19487,7 @@
         <v>1598</v>
       </c>
       <c r="B16" t="s">
-        <v>1796</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -19495,7 +19495,7 @@
         <v>1599</v>
       </c>
       <c r="B17" t="s">
-        <v>1795</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -19503,7 +19503,7 @@
         <v>1599</v>
       </c>
       <c r="B18" t="s">
-        <v>1797</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -19511,7 +19511,7 @@
         <v>1600</v>
       </c>
       <c r="B19" t="s">
-        <v>1798</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -19519,7 +19519,7 @@
         <v>1601</v>
       </c>
       <c r="B20" t="s">
-        <v>1798</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -19527,7 +19527,7 @@
         <v>1602</v>
       </c>
       <c r="B21" t="s">
-        <v>1799</v>
+        <v>1749</v>
       </c>
     </row>
   </sheetData>
@@ -20616,7 +20616,7 @@
         <v>217</v>
       </c>
       <c r="C53" t="s">
-        <v>1800</v>
+        <v>1750</v>
       </c>
       <c r="D53" t="s">
         <v>220</v>
@@ -20630,7 +20630,7 @@
         <v>217</v>
       </c>
       <c r="C54" t="s">
-        <v>1801</v>
+        <v>1751</v>
       </c>
       <c r="D54" t="s">
         <v>220</v>
@@ -20812,7 +20812,7 @@
         <v>218</v>
       </c>
       <c r="C67" t="s">
-        <v>1802</v>
+        <v>1752</v>
       </c>
       <c r="D67" t="s">
         <v>220</v>
@@ -20826,7 +20826,7 @@
         <v>218</v>
       </c>
       <c r="C68" t="s">
-        <v>1803</v>
+        <v>1753</v>
       </c>
       <c r="D68" t="s">
         <v>220</v>
@@ -20840,7 +20840,7 @@
         <v>218</v>
       </c>
       <c r="C69" t="s">
-        <v>1804</v>
+        <v>1754</v>
       </c>
       <c r="D69" t="s">
         <v>220</v>
@@ -21364,15 +21364,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48AA9C6D-EFEE-4389-B779-BD4A88AD0E00}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.28515625" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="7"/>
+    <col min="3" max="3" width="102" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -21394,7 +21394,7 @@
         <v>483</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>1728</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="375" customHeight="1" x14ac:dyDescent="0.25">
@@ -21405,7 +21405,7 @@
         <v>484</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>1729</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21416,7 +21416,7 @@
         <v>391</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>1730</v>
+        <v>1758</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21427,7 +21427,7 @@
         <v>392</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>1731</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21438,7 +21438,7 @@
         <v>393</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>1732</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21449,7 +21449,7 @@
         <v>485</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>1733</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21460,7 +21460,7 @@
         <v>397</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>1734</v>
+        <v>1762</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21471,7 +21471,7 @@
         <v>398</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>1735</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21482,10 +21482,10 @@
         <v>399</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>1736</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="240" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>404</v>
       </c>
@@ -21493,10 +21493,10 @@
         <v>400</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>1737</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>1765</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="210" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>423</v>
       </c>
@@ -21504,7 +21504,7 @@
         <v>401</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>1738</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21515,7 +21515,7 @@
         <v>403</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>1739</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21526,7 +21526,7 @@
         <v>405</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>1740</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21537,7 +21537,7 @@
         <v>408</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>1741</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21548,10 +21548,10 @@
         <v>410</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>1742</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="315" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>422</v>
       </c>
@@ -21559,10 +21559,10 @@
         <v>486</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>1743</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="360" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>421</v>
       </c>
@@ -21570,7 +21570,7 @@
         <v>411</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>1744</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21581,10 +21581,10 @@
         <v>413</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>1745</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>1773</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>414</v>
       </c>
@@ -21592,10 +21592,10 @@
         <v>415</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>1746</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>416</v>
       </c>
@@ -21603,7 +21603,7 @@
         <v>417</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>1747</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21614,7 +21614,7 @@
         <v>419</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>1748</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21625,7 +21625,7 @@
         <v>424</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>1749</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21636,10 +21636,10 @@
         <v>426</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>1750</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>1778</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="360" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>427</v>
       </c>
@@ -21647,7 +21647,7 @@
         <v>428</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>1751</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21658,10 +21658,10 @@
         <v>430</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>1752</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="225" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>431</v>
       </c>
@@ -21669,7 +21669,7 @@
         <v>432</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>1753</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21680,10 +21680,10 @@
         <v>434</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>1754</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>1782</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="300" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>435</v>
       </c>
@@ -21691,7 +21691,7 @@
         <v>436</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>1755</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21702,7 +21702,7 @@
         <v>487</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>1756</v>
+        <v>1784</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21713,7 +21713,7 @@
         <v>438</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>1757</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21724,10 +21724,10 @@
         <v>440</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>1758</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="240" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>441</v>
       </c>
@@ -21735,7 +21735,7 @@
         <v>442</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>1759</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21746,10 +21746,10 @@
         <v>472</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>1760</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>1788</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>444</v>
       </c>
@@ -21757,10 +21757,10 @@
         <v>445</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>1761</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="375" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>446</v>
       </c>
@@ -21768,7 +21768,7 @@
         <v>447</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>1762</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21779,10 +21779,10 @@
         <v>449</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>1763</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="375" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>450</v>
       </c>
@@ -21790,10 +21790,10 @@
         <v>451</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>1764</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="315" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>453</v>
       </c>
@@ -21801,10 +21801,10 @@
         <v>452</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="225" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>454</v>
       </c>
@@ -21812,7 +21812,7 @@
         <v>455</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>1766</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21823,10 +21823,10 @@
         <v>457</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>1767</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="315" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>459</v>
       </c>
@@ -21834,7 +21834,7 @@
         <v>458</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>1768</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21845,7 +21845,7 @@
         <v>461</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>1769</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21856,7 +21856,7 @@
         <v>462</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>1770</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21867,10 +21867,10 @@
         <v>465</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="210" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>467</v>
       </c>
@@ -21878,10 +21878,10 @@
         <v>466</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>1772</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>469</v>
       </c>
@@ -21889,7 +21889,7 @@
         <v>468</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>1773</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21900,10 +21900,10 @@
         <v>471</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>473</v>
       </c>
@@ -21911,10 +21911,10 @@
         <v>474</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>1775</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="240" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>476</v>
       </c>
@@ -21922,7 +21922,7 @@
         <v>475</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>1776</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
@@ -21933,7 +21933,7 @@
         <v>477</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>1777</v>
+        <v>1805</v>
       </c>
     </row>
   </sheetData>
@@ -22210,7 +22210,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1805</v>
+        <v>1755</v>
       </c>
       <c r="B2" t="s">
         <v>702</v>
@@ -22218,7 +22218,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1805</v>
+        <v>1755</v>
       </c>
       <c r="B3" t="s">
         <v>703</v>

</xml_diff>

<commit_message>
Initialise Llama 2 fine-tuning and fix errors
</commit_message>
<xml_diff>
--- a/testing_excel.xlsx
+++ b/testing_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pumukl\Documents\GitHub\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D232CDE-74D4-42B2-ACB5-2924BA196980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F1E686-FD19-44CE-BEC2-5CD88CA96747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="769" firstSheet="14" activeTab="25" xr2:uid="{3104A2F9-7A17-4E5B-B5FF-CB166158170B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="769" firstSheet="14" activeTab="21" xr2:uid="{3104A2F9-7A17-4E5B-B5FF-CB166158170B}"/>
   </bookViews>
   <sheets>
     <sheet name="Greeting_Goodbyes" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5873" uniqueCount="1806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5873" uniqueCount="1807">
   <si>
     <t>Greetings</t>
   </si>
@@ -5538,6 +5538,9 @@
   </si>
   <si>
     <t>In &lt;TITLE&gt;Kingdom Come: Deliverance&lt;/TITLE&gt;, the introductory monologue delivered by Henry, the protagonist, sets the stage for the game's historical narrative. The game is set in the Kingdom of Bohemia during a time of great turmoil following the death of Emperor Charles IV. His son, Wenceslas IV, ascends to the throne but proves to be an ineffective ruler, neglecting his duties in favor of personal indulgences. This leads to political instability, prompting Wenceslas's half-brother, King Sigismund of Hungary, to seize the opportunity to take control. Sigismund kidnaps Wenceslas and invades Bohemia with a mercenary army, causing widespread chaos and destruction. The player takes on the role of Henry, a blacksmith's son whose peaceful life is shattered when his village is attacked by Sigismund's forces. Driven by a desire for revenge and justice, Henry becomes embroiled in the conflict, seeking to restore order to his homeland. The game explores themes of loyalty, vengeance, and the struggle for power in a meticulously recreated medieval world, where the player's choices and actions shape Henry's journey and the fate of Bohemia.</t>
+  </si>
+  <si>
+    <t>Guard reacting to the Player's armor</t>
   </si>
 </sst>
 </file>
@@ -18603,8 +18606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A6A5B03-E547-411D-931D-5C70576C616D}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34:D52"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18836,7 +18839,7 @@
         <v>154</v>
       </c>
       <c r="D16" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -18850,7 +18853,7 @@
         <v>154</v>
       </c>
       <c r="D17" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -18864,7 +18867,7 @@
         <v>154</v>
       </c>
       <c r="D18" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -18878,7 +18881,7 @@
         <v>154</v>
       </c>
       <c r="D19" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -18892,7 +18895,7 @@
         <v>154</v>
       </c>
       <c r="D20" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -18906,7 +18909,7 @@
         <v>154</v>
       </c>
       <c r="D21" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -18920,7 +18923,7 @@
         <v>154</v>
       </c>
       <c r="D22" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -18934,7 +18937,7 @@
         <v>1728</v>
       </c>
       <c r="D23" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -18948,7 +18951,7 @@
         <v>1729</v>
       </c>
       <c r="D24" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -18962,7 +18965,7 @@
         <v>1728</v>
       </c>
       <c r="D25" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -18976,7 +18979,7 @@
         <v>1729</v>
       </c>
       <c r="D26" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -18990,7 +18993,7 @@
         <v>271</v>
       </c>
       <c r="D27" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -19004,7 +19007,7 @@
         <v>271</v>
       </c>
       <c r="D28" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -19018,7 +19021,7 @@
         <v>1728</v>
       </c>
       <c r="D29" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -19032,7 +19035,7 @@
         <v>1730</v>
       </c>
       <c r="D30" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -19046,7 +19049,7 @@
         <v>1728</v>
       </c>
       <c r="D31" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -19060,7 +19063,7 @@
         <v>1730</v>
       </c>
       <c r="D32" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -19074,7 +19077,7 @@
         <v>154</v>
       </c>
       <c r="D33" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -21364,7 +21367,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48AA9C6D-EFEE-4389-B779-BD4A88AD0E00}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix problem with guard_equipment_data.json
</commit_message>
<xml_diff>
--- a/testing_excel.xlsx
+++ b/testing_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pumukl\Documents\GitHub\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F1E686-FD19-44CE-BEC2-5CD88CA96747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BE82A8-48E7-40A1-BED5-9CE672FF94B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="769" firstSheet="14" activeTab="21" xr2:uid="{3104A2F9-7A17-4E5B-B5FF-CB166158170B}"/>
   </bookViews>
@@ -18606,8 +18606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A6A5B03-E547-411D-931D-5C70576C616D}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18741,7 +18741,7 @@
         <v>154</v>
       </c>
       <c r="D9" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -18755,7 +18755,7 @@
         <v>154</v>
       </c>
       <c r="D10" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -18769,7 +18769,7 @@
         <v>154</v>
       </c>
       <c r="D11" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -18783,7 +18783,7 @@
         <v>154</v>
       </c>
       <c r="D12" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -18797,7 +18797,7 @@
         <v>154</v>
       </c>
       <c r="D13" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -18811,7 +18811,7 @@
         <v>154</v>
       </c>
       <c r="D14" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -18825,7 +18825,7 @@
         <v>154</v>
       </c>
       <c r="D15" t="s">
-        <v>1733</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -19091,7 +19091,7 @@
         <v>154</v>
       </c>
       <c r="D34" t="s">
-        <v>1734</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>